<commit_message>
received tabular data for verification of state models
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -1154,12 +1154,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2753036437247"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.8056680161943"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.4453441295547"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1411,17 +1411,17 @@
   </sheetPr>
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2753036437247"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1555,7 +1555,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="21" t="n">
-        <v>0</v>
+        <v>5.47E-008</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>38</v>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="E8" s="24" t="n">
         <f aca="false">B8</f>
-        <v>0</v>
+        <v>5.47E-008</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,7 +1681,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="21" t="n">
-        <v>0</v>
+        <v>3.23E-009</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>38</v>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="E15" s="24" t="n">
         <f aca="false">B15</f>
-        <v>0</v>
+        <v>3.23E-009</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,7 +2360,7 @@
         <v>4456800</v>
       </c>
     </row>
-    <row r="53" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="32" t="s">
         <v>86</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>127434</v>
       </c>
     </row>
-    <row r="54" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="30" t="s">
         <v>88</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>-3637</v>
       </c>
     </row>
-    <row r="55" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="32" t="s">
         <v>90</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>5812</v>
       </c>
     </row>
-    <row r="56" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="33" t="s">
         <v>92</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>94</v>
       </c>
       <c r="B57" s="25" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C57" s="25" t="s">
         <v>95</v>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="E57" s="25" t="n">
         <f aca="false">B57</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F57" s="38"/>
     </row>
@@ -2457,7 +2457,7 @@
         <v>97</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>95</v>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="E58" s="0" t="n">
         <f aca="false">B58</f>
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="F58" s="38"/>
     </row>
@@ -2476,7 +2476,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>95</v>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="E59" s="0" t="n">
         <f aca="false">B59</f>
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="F59" s="38"/>
     </row>
@@ -2495,7 +2495,7 @@
         <v>101</v>
       </c>
       <c r="B60" s="25" t="n">
-        <v>0</v>
+        <v>-0.07</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>95</v>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="E60" s="25" t="n">
         <f aca="false">B60</f>
-        <v>0</v>
+        <v>-0.07</v>
       </c>
       <c r="F60" s="38"/>
     </row>
@@ -2514,7 +2514,7 @@
         <v>103</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>95</v>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="E61" s="0" t="n">
         <f aca="false">B61</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F61" s="38"/>
     </row>
@@ -2533,7 +2533,7 @@
         <v>105</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>95</v>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="E62" s="0" t="n">
         <f aca="false">B62</f>
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="F62" s="38"/>
     </row>
@@ -2580,8 +2580,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3133,8 +3133,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3251,12 +3251,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.9514170040486"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3539,9 +3539,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="11" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="52.165991902834"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="11" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3919,12 +3919,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="28" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="11" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4262,9 +4262,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="11" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="52.165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="52.5951417004049"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="28" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="11" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4704,15 +4704,15 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.5951417004049"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -4739,7 +4739,7 @@
         <v>82</v>
       </c>
       <c r="B2" s="11" t="n">
-        <v>0.2</v>
+        <v>25</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>24</v>
@@ -4747,7 +4747,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="54" t="n">
         <f aca="false">B2*1000</f>
-        <v>200</v>
+        <v>25000</v>
       </c>
       <c r="F2" s="11"/>
     </row>
@@ -4756,7 +4756,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="11" t="n">
-        <v>3.7</v>
+        <v>47</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>24</v>
@@ -4764,7 +4764,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="54" t="n">
         <f aca="false">B3*1000</f>
-        <v>3700</v>
+        <v>47000</v>
       </c>
       <c r="F3" s="11"/>
     </row>
@@ -4773,7 +4773,7 @@
         <v>86</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>-1.47</v>
+        <v>-32</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>24</v>
@@ -4781,7 +4781,7 @@
       <c r="D4" s="11"/>
       <c r="E4" s="54" t="n">
         <f aca="false">B4*1000</f>
-        <v>-1470</v>
+        <v>-32000</v>
       </c>
       <c r="F4" s="11"/>
     </row>
@@ -4790,7 +4790,7 @@
         <v>88</v>
       </c>
       <c r="B5" s="11" t="n">
-        <v>0.4</v>
+        <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -4798,7 +4798,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="54" t="n">
         <f aca="false">B5*1000</f>
-        <v>400</v>
+        <v>16000</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -4807,7 +4807,7 @@
         <v>90</v>
       </c>
       <c r="B6" s="11" t="n">
-        <v>-0.5</v>
+        <v>-29</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>31</v>
@@ -4815,7 +4815,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="54" t="n">
         <f aca="false">B6*1000</f>
-        <v>-500</v>
+        <v>-29000</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -4824,7 +4824,7 @@
         <v>92</v>
       </c>
       <c r="B7" s="11" t="n">
-        <v>1.3</v>
+        <v>13</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>31</v>
@@ -4832,7 +4832,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="54" t="n">
         <f aca="false">B7*1000</f>
-        <v>1300</v>
+        <v>13000</v>
       </c>
       <c r="F7" s="11"/>
     </row>

</xml_diff>

<commit_message>
Nonlinear propagation, in progress
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,11 +20,11 @@
     <sheet name="Constants" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="days2hrs" vbProcedure="false">Constants!$B$5</definedName>
-    <definedName function="false" hidden="false" name="g2mps2" vbProcedure="false">Constants!$B$4</definedName>
-    <definedName function="false" hidden="false" name="hr2min" vbProcedure="false">Constants!$B$1</definedName>
-    <definedName function="false" hidden="false" name="hr2sec" vbProcedure="false">Constants!$B$3</definedName>
-    <definedName function="false" hidden="false" name="min2sec" vbProcedure="false">Constants!$B$2</definedName>
+    <definedName function="false" hidden="false" name="days2hrs" vbProcedure="false">Constants!$B$6</definedName>
+    <definedName function="false" hidden="false" name="g2mps2" vbProcedure="false">Constants!$B$5</definedName>
+    <definedName function="false" hidden="false" name="hr2min" vbProcedure="false">Constants!$B$2</definedName>
+    <definedName function="false" hidden="false" name="hr2sec" vbProcedure="false">Constants!$B$4</definedName>
+    <definedName function="false" hidden="false" name="min2sec" vbProcedure="false">Constants!$B$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="196">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -320,30 +320,12 @@
     <t xml:space="preserve">z component of initial velocity of target (inertial)</t>
   </si>
   <si>
-    <t xml:space="preserve">egx</t>
+    <t xml:space="preserve">ax</t>
   </si>
   <si>
     <t xml:space="preserve">m/s^2</t>
   </si>
   <si>
-    <t xml:space="preserve">x component of gravity error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y component of gravity error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z component of gravity error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ax</t>
-  </si>
-  <si>
     <t xml:space="preserve">x component of atmospheric acceleration</t>
   </si>
   <si>
@@ -443,9 +425,6 @@
     <t xml:space="preserve">velT</t>
   </si>
   <si>
-    <t xml:space="preserve">errG</t>
-  </si>
-  <si>
     <t xml:space="preserve">accD</t>
   </si>
   <si>
@@ -639,13 +618,19 @@
   </si>
   <si>
     <t xml:space="preserve">days2hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muEarth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000E+00"/>
@@ -653,6 +638,7 @@
     <numFmt numFmtId="168" formatCode="0.0000000"/>
     <numFmt numFmtId="169" formatCode="0.00E+00"/>
     <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -844,7 +830,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1067,6 +1053,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1149,17 +1143,17 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.5910931174089"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1311,7 +1305,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>13</v>
@@ -1321,7 +1315,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">B9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1340,29 +1334,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>60</v>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1370,27 +1365,51 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B3" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
         <v>3600</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>9.81</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B5" s="0" t="n">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="57" t="n">
+        <v>398600.4418</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>299792.458</v>
       </c>
     </row>
   </sheetData>
@@ -1409,10 +1428,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1420,8 +1439,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.3400809716599"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.3765182186235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1699,7 +1718,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="26" t="n">
-        <v>0</v>
+        <v>7993.22895176268</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>24</v>
@@ -1709,7 +1728,7 @@
       </c>
       <c r="E16" s="27" t="n">
         <f aca="false">B16*1000</f>
-        <v>0</v>
+        <v>7993228.95176268</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1736,7 @@
         <v>48</v>
       </c>
       <c r="B17" s="21" t="n">
-        <v>0</v>
+        <v>2319.63567604595</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>24</v>
@@ -1727,7 +1746,7 @@
       </c>
       <c r="E17" s="20" t="n">
         <f aca="false">B17*1000</f>
-        <v>0</v>
+        <v>2319635.67604595</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,7 +1754,7 @@
         <v>49</v>
       </c>
       <c r="B18" s="22" t="n">
-        <v>0</v>
+        <v>1275.25350954771</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>24</v>
@@ -1745,7 +1764,7 @@
       </c>
       <c r="E18" s="23" t="n">
         <f aca="false">B18*1000</f>
-        <v>0</v>
+        <v>1275253.50954771</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,7 +1772,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="21" t="n">
-        <v>0</v>
+        <v>-2.15792847166078</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>31</v>
@@ -1763,7 +1782,7 @@
       </c>
       <c r="E19" s="20" t="n">
         <f aca="false">B19*1000</f>
-        <v>0</v>
+        <v>-2157.92847166078</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1790,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="21" t="n">
-        <v>0</v>
+        <v>5.94339709534114</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>31</v>
@@ -1781,7 +1800,7 @@
       </c>
       <c r="E20" s="20" t="n">
         <f aca="false">B20*1000</f>
-        <v>0</v>
+        <v>5943.39709534114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,7 +1808,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="21" t="n">
-        <v>0</v>
+        <v>-2.7149898983448</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>31</v>
@@ -1799,7 +1818,7 @@
       </c>
       <c r="E21" s="20" t="n">
         <f aca="false">B21*1000</f>
-        <v>0</v>
+        <v>-2714.9898983448</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,7 +1826,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="21" t="n">
-        <v>0</v>
+        <v>-2E-009</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>38</v>
@@ -1817,7 +1836,7 @@
       </c>
       <c r="E22" s="24" t="n">
         <f aca="false">B22</f>
-        <v>0</v>
+        <v>-2E-009</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2342,7 +2361,7 @@
         <v>7142800</v>
       </c>
     </row>
-    <row r="52" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="32" t="s">
         <v>84</v>
       </c>
@@ -2438,7 +2457,7 @@
         <v>94</v>
       </c>
       <c r="B57" s="25" t="n">
-        <v>0.01</v>
+        <v>-0.07</v>
       </c>
       <c r="C57" s="25" t="s">
         <v>95</v>
@@ -2448,7 +2467,7 @@
       </c>
       <c r="E57" s="25" t="n">
         <f aca="false">B57</f>
-        <v>0.01</v>
+        <v>-0.07</v>
       </c>
       <c r="F57" s="38"/>
     </row>
@@ -2457,7 +2476,7 @@
         <v>97</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>-0.01</v>
+        <v>0.1</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>95</v>
@@ -2467,7 +2486,7 @@
       </c>
       <c r="E58" s="0" t="n">
         <f aca="false">B58</f>
-        <v>-0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F58" s="38"/>
     </row>
@@ -2476,7 +2495,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>0.001</v>
+        <v>-0.04</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>95</v>
@@ -2486,74 +2505,20 @@
       </c>
       <c r="E59" s="0" t="n">
         <f aca="false">B59</f>
-        <v>0.001</v>
+        <v>-0.04</v>
       </c>
       <c r="F59" s="38"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="25" t="n">
-        <v>-0.07</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="E60" s="25" t="n">
-        <f aca="false">B60</f>
-        <v>-0.07</v>
-      </c>
-      <c r="F60" s="38"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="E61" s="0" t="n">
-        <f aca="false">B61</f>
-        <v>0.1</v>
-      </c>
-      <c r="F61" s="38"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>-0.04</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E62" s="0" t="n">
-        <f aca="false">B62</f>
-        <v>-0.04</v>
-      </c>
-      <c r="F62" s="38"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-    </row>
+      <c r="A60" s="25"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2570,41 +2535,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B2" s="39" t="n">
         <v>1</v>
@@ -2621,7 +2586,7 @@
     </row>
     <row r="3" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B3" s="39" t="n">
         <v>4</v>
@@ -2638,7 +2603,7 @@
     </row>
     <row r="4" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="39" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B4" s="39" t="n">
         <v>7</v>
@@ -2655,7 +2620,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">B2+7</f>
@@ -2676,7 +2641,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B3+7</f>
@@ -2697,7 +2662,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B4+7</f>
@@ -2718,7 +2683,7 @@
     </row>
     <row r="8" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="39" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B8" s="39" t="n">
         <f aca="false">B5+7</f>
@@ -2739,7 +2704,7 @@
     </row>
     <row r="9" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="39" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B9" s="39" t="n">
         <f aca="false">B6+7</f>
@@ -2760,7 +2725,7 @@
     </row>
     <row r="10" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="39" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B10" s="39" t="n">
         <f aca="false">B7+7</f>
@@ -2781,7 +2746,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B8+7</f>
@@ -2802,7 +2767,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">B9+7</f>
@@ -2823,7 +2788,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B10+7</f>
@@ -2844,7 +2809,7 @@
     </row>
     <row r="14" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="39" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B14" s="39" t="n">
         <f aca="false">B11+7</f>
@@ -2865,7 +2830,7 @@
     </row>
     <row r="15" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="39" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B15" s="39" t="n">
         <f aca="false">B12+7</f>
@@ -2886,7 +2851,7 @@
     </row>
     <row r="16" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B16" s="39" t="n">
         <f aca="false">B13+7</f>
@@ -2907,7 +2872,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">B14+7</f>
@@ -2928,7 +2893,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">B15+7</f>
@@ -2949,7 +2914,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">B16+7</f>
@@ -2970,7 +2935,7 @@
     </row>
     <row r="20" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B20" s="39" t="n">
         <f aca="false">B17+7</f>
@@ -2991,7 +2956,7 @@
     </row>
     <row r="21" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B21" s="39" t="n">
         <f aca="false">B18+7</f>
@@ -3012,7 +2977,7 @@
     </row>
     <row r="22" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="39" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B22" s="39" t="n">
         <f aca="false">B19+7</f>
@@ -3033,7 +2998,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B20+7</f>
@@ -3054,7 +3019,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B21+7</f>
@@ -3075,7 +3040,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>56</v>
@@ -3090,23 +3055,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>61</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3123,41 +3072,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -3174,7 +3123,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -3191,7 +3140,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -3206,27 +3155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3246,17 +3175,17 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3279,17 +3208,17 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B2" s="44" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E2" s="12" t="n">
         <f aca="false">B2/3</f>
@@ -3298,16 +3227,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B3" s="45" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E3" s="12" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
@@ -3317,16 +3246,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B4" s="47" t="n">
         <v>0.05</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E4" s="17" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
@@ -3335,16 +3264,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B5" s="45" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E5" s="12" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
@@ -3353,16 +3282,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B6" s="45" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E6" s="12" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
@@ -3371,16 +3300,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B7" s="45" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E7" s="12" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
@@ -3389,16 +3318,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B8" s="45" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E8" s="12" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
@@ -3407,16 +3336,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B9" s="45" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E9" s="12" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
@@ -3425,16 +3354,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B10" s="48" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E10" s="8" t="n">
         <f aca="false">B10/3</f>
@@ -3443,16 +3372,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B11" s="49" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E11" s="17" t="n">
         <f aca="false">B11/3</f>
@@ -3461,16 +3390,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B12" s="50" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E12" s="46" t="n">
         <f aca="false">B12/3</f>
@@ -3479,16 +3408,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B13" s="50" t="n">
         <v>100</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E13" s="46" t="n">
         <f aca="false">B13/3</f>
@@ -3497,16 +3426,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B14" s="50" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E14" s="46" t="n">
         <f aca="false">B14/3</f>
@@ -3539,9 +3468,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="11" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="52.5951417004049"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="11" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3564,16 +3493,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>4000</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="E2" s="8" t="n">
         <f aca="false">B2/3</f>
@@ -3582,16 +3511,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B3" s="11" t="n">
         <v>4000</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="E3" s="12" t="n">
         <f aca="false">B3/3</f>
@@ -3600,16 +3529,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B4" s="11" t="n">
         <v>4000</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="E4" s="12" t="n">
         <f aca="false">B4/3</f>
@@ -3618,16 +3547,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B5" s="11" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E5" s="12" t="n">
         <f aca="false">B5/3</f>
@@ -3636,16 +3565,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B6" s="11" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E6" s="12" t="n">
         <f aca="false">B6/3</f>
@@ -3654,16 +3583,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B7" s="11" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E7" s="12" t="n">
         <f aca="false">B7/3</f>
@@ -3672,16 +3601,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B8" s="11" t="n">
         <v>0.0005</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E8" s="12" t="n">
         <f aca="false">B8/3</f>
@@ -3690,16 +3619,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B9" s="11" t="n">
         <v>0.0005</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E9" s="12" t="n">
         <f aca="false">B9/3</f>
@@ -3708,16 +3637,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B10" s="11" t="n">
         <v>0.0005</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E10" s="12" t="n">
         <f aca="false">B10/3</f>
@@ -3726,17 +3655,17 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B11" s="11" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E11" s="12" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
@@ -3745,17 +3674,17 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B12" s="11" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E12" s="12" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
@@ -3764,17 +3693,17 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B13" s="11" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E13" s="12" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
@@ -3783,17 +3712,17 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B14" s="11" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E14" s="12" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
@@ -3802,17 +3731,17 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B15" s="11" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E15" s="12" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
@@ -3821,17 +3750,17 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B16" s="11" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E16" s="12" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
@@ -3840,17 +3769,17 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B17" s="11" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E17" s="12" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
@@ -3859,17 +3788,17 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B18" s="11" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E18" s="12" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
@@ -3878,17 +3807,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B19" s="16" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E19" s="17" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
@@ -3919,12 +3848,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="28" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="47.7732793522267"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="11" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4262,9 +4191,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="11" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="53.8825910931174"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="28" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="11" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4702,17 +4631,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.5951417004049"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.8825910931174"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -4841,7 +4770,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="11" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>95</v>
@@ -4849,7 +4778,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="54" t="n">
         <f aca="false">B8</f>
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F8" s="11"/>
     </row>
@@ -4858,7 +4787,7 @@
         <v>97</v>
       </c>
       <c r="B9" s="11" t="n">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>95</v>
@@ -4866,7 +4795,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="54" t="n">
         <f aca="false">B9</f>
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -4875,7 +4804,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="11" t="n">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>95</v>
@@ -4883,59 +4812,32 @@
       <c r="D10" s="11"/>
       <c r="E10" s="54" t="n">
         <f aca="false">B10</f>
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="F10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="11" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="A11" s="9"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="54" t="n">
-        <f aca="false">B11</f>
-        <v>0.01</v>
-      </c>
+      <c r="E11" s="54"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="11" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="A12" s="9"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="54" t="n">
-        <f aca="false">B12</f>
-        <v>-0.01</v>
-      </c>
+      <c r="E12" s="54"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="11" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>95</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="54" t="n">
-        <f aca="false">B13</f>
-        <v>-0.01</v>
-      </c>
+      <c r="E13" s="54"/>
       <c r="F13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4955,37 +4857,16 @@
       <c r="F15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="16"/>
-    </row>
+      <c r="A16" s="14"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
got linear error state modeling working. Need to check appropriateness of the expected error residual
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="202">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -638,6 +638,12 @@
   <si>
     <t xml:space="preserve">c</t>
   </si>
+  <si>
+    <t xml:space="preserve">tauBias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tauAtmo</t>
+  </si>
 </sst>
 </file>
 
@@ -818,7 +824,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="80">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -896,10 +902,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -996,14 +998,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1171,17 +1165,17 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5263157894737"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="80.2307692307692"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="81.6234817813765"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1261,7 +1255,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>13</v>
@@ -1271,7 +1265,7 @@
       </c>
       <c r="E5" s="13" t="n">
         <f aca="false">B5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,7 +1273,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>13</v>
@@ -1289,7 +1283,7 @@
       </c>
       <c r="E6" s="13" t="n">
         <f aca="false">B6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1344,7 @@
       <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="20" t="n">
+      <c r="B10" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1359,7 +1353,7 @@
       <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="21" t="n">
+      <c r="E10" s="20" t="n">
         <f aca="false">B10</f>
         <v>6</v>
       </c>
@@ -1378,7 +1372,7 @@
       <c r="D11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="22" t="n">
+      <c r="E11" s="21" t="n">
         <f aca="false">B11</f>
         <v>12</v>
       </c>
@@ -1404,24 +1398,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1470,7 +1464,7 @@
       <c r="A7" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="82" t="n">
+      <c r="B7" s="79" t="n">
         <v>398600.4418</v>
       </c>
     </row>
@@ -1480,6 +1474,22 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>299792.458</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1509,25 +1519,25 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="77.1255060728745"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="78.412955465587"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0"/>
@@ -2551,19 +2561,19 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="27" t="n">
         <v>7912.33967</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="29" t="n">
+      <c r="E2" s="28" t="n">
         <f aca="false">B2*1000</f>
         <v>7912339.67</v>
       </c>
@@ -3591,7 +3601,7 @@
       <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="30" t="n">
+      <c r="B3" s="29" t="n">
         <v>2836.1046</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -3600,7 +3610,7 @@
       <c r="D3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="29" t="n">
+      <c r="E3" s="28" t="n">
         <f aca="false">B3*1000</f>
         <v>2836104.6</v>
       </c>
@@ -4628,7 +4638,7 @@
       <c r="A4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="31" t="n">
+      <c r="B4" s="30" t="n">
         <v>500.0817</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -4637,7 +4647,7 @@
       <c r="D4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="32" t="n">
+      <c r="E4" s="31" t="n">
         <f aca="false">B4*1000</f>
         <v>500081.7</v>
       </c>
@@ -5665,16 +5675,16 @@
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="30" t="n">
+      <c r="B5" s="29" t="n">
         <v>-2.3535</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="29" t="n">
+      <c r="E5" s="28" t="n">
         <f aca="false">B5*1000</f>
         <v>-2353.5</v>
       </c>
@@ -6702,7 +6712,7 @@
       <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="30" t="n">
+      <c r="B6" s="29" t="n">
         <v>6.368</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -6711,7 +6721,7 @@
       <c r="D6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="29" t="n">
+      <c r="E6" s="28" t="n">
         <f aca="false">B6*1000</f>
         <v>6368</v>
       </c>
@@ -7739,7 +7749,7 @@
       <c r="A7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="31" t="n">
+      <c r="B7" s="30" t="n">
         <v>-1.1228565</v>
       </c>
       <c r="C7" s="17" t="s">
@@ -7748,7 +7758,7 @@
       <c r="D7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="32" t="n">
+      <c r="E7" s="31" t="n">
         <f aca="false">B7*1000</f>
         <v>-1122.8565</v>
       </c>
@@ -8776,7 +8786,7 @@
       <c r="A8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="30" t="n">
+      <c r="B8" s="29" t="n">
         <v>7600</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -8785,7 +8795,7 @@
       <c r="D8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="29" t="n">
+      <c r="E8" s="28" t="n">
         <f aca="false">B8*1000</f>
         <v>7600000</v>
       </c>
@@ -9813,7 +9823,7 @@
       <c r="A9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="30" t="n">
+      <c r="B9" s="29" t="n">
         <v>3589</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -9822,7 +9832,7 @@
       <c r="D9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="29" t="n">
+      <c r="E9" s="28" t="n">
         <f aca="false">B9*1000</f>
         <v>3589000</v>
       </c>
@@ -10850,7 +10860,7 @@
       <c r="A10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="31" t="n">
+      <c r="B10" s="30" t="n">
         <v>-500</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -10859,7 +10869,7 @@
       <c r="D10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="32" t="n">
+      <c r="E10" s="31" t="n">
         <f aca="false">B10*1000</f>
         <v>-500000</v>
       </c>
@@ -11887,16 +11897,16 @@
       <c r="A11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="30" t="n">
+      <c r="B11" s="29" t="n">
         <v>-2.839</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="29" t="n">
+      <c r="E11" s="28" t="n">
         <f aca="false">B11*1000</f>
         <v>-2839</v>
       </c>
@@ -11905,7 +11915,7 @@
       <c r="A12" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="30" t="n">
+      <c r="B12" s="29" t="n">
         <v>6.17</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -11914,7 +11924,7 @@
       <c r="D12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="29" t="n">
+      <c r="E12" s="28" t="n">
         <f aca="false">B12*1000</f>
         <v>6170</v>
       </c>
@@ -12942,7 +12952,7 @@
       <c r="A13" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="31" t="n">
+      <c r="B13" s="30" t="n">
         <v>-1.12</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -12951,7 +12961,7 @@
       <c r="D13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="32" t="n">
+      <c r="E13" s="31" t="n">
         <f aca="false">B13*1000</f>
         <v>-1120</v>
       </c>
@@ -13979,7 +13989,7 @@
       <c r="A14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="30" t="n">
+      <c r="B14" s="29" t="n">
         <v>7993.22895176268</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -13988,7 +13998,7 @@
       <c r="D14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="29" t="n">
+      <c r="E14" s="28" t="n">
         <f aca="false">B14*1000</f>
         <v>7993228.95176268</v>
       </c>
@@ -15016,7 +15026,7 @@
       <c r="A15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="30" t="n">
+      <c r="B15" s="29" t="n">
         <v>2319.63567604595</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -15025,7 +15035,7 @@
       <c r="D15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="29" t="n">
+      <c r="E15" s="28" t="n">
         <f aca="false">B15*1000</f>
         <v>2319635.67604595</v>
       </c>
@@ -16053,7 +16063,7 @@
       <c r="A16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="31" t="n">
+      <c r="B16" s="30" t="n">
         <v>1275.25350954771</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -16062,7 +16072,7 @@
       <c r="D16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="32" t="n">
+      <c r="E16" s="31" t="n">
         <f aca="false">B16*1000</f>
         <v>1275253.50954771</v>
       </c>
@@ -17090,16 +17100,16 @@
       <c r="A17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="29" t="n">
         <v>-2.15792847166078</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="29" t="n">
+      <c r="E17" s="28" t="n">
         <f aca="false">B17*1000</f>
         <v>-2157.92847166078</v>
       </c>
@@ -18127,7 +18137,7 @@
       <c r="A18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="29" t="n">
         <v>5.94339709534114</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -18136,7 +18146,7 @@
       <c r="D18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="29" t="n">
+      <c r="E18" s="28" t="n">
         <f aca="false">B18*1000</f>
         <v>5943.39709534114</v>
       </c>
@@ -19164,7 +19174,7 @@
       <c r="A19" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="31" t="n">
+      <c r="B19" s="30" t="n">
         <v>-2.7149898983448</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -19173,7 +19183,7 @@
       <c r="D19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="32" t="n">
+      <c r="E19" s="31" t="n">
         <f aca="false">B19*1000</f>
         <v>-2714.9898983448</v>
       </c>
@@ -20201,7 +20211,7 @@
       <c r="A20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -20210,7 +20220,7 @@
       <c r="D20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="33" t="n">
+      <c r="E20" s="32" t="n">
         <f aca="false">B20*1000</f>
         <v>0</v>
       </c>
@@ -21238,7 +21248,7 @@
       <c r="A21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="30" t="n">
+      <c r="B21" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -21247,7 +21257,7 @@
       <c r="D21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="29" t="n">
+      <c r="E21" s="28" t="n">
         <f aca="false">B21*1000</f>
         <v>0</v>
       </c>
@@ -22275,7 +22285,7 @@
       <c r="A22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="31" t="n">
+      <c r="B22" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="17" t="s">
@@ -22284,7 +22294,7 @@
       <c r="D22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="32" t="n">
+      <c r="E22" s="31" t="n">
         <f aca="false">B22*1000</f>
         <v>0</v>
       </c>
@@ -23312,16 +23322,16 @@
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="30" t="n">
+      <c r="B23" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="29" t="n">
+      <c r="E23" s="28" t="n">
         <f aca="false">B23*1000</f>
         <v>0</v>
       </c>
@@ -24349,7 +24359,7 @@
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="30" t="n">
+      <c r="B24" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -24358,7 +24368,7 @@
       <c r="D24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="29" t="n">
+      <c r="E24" s="28" t="n">
         <f aca="false">B24*1000</f>
         <v>0</v>
       </c>
@@ -25386,7 +25396,7 @@
       <c r="A25" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="31" t="n">
+      <c r="B25" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="17" t="s">
@@ -25395,7 +25405,7 @@
       <c r="D25" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="32" t="n">
+      <c r="E25" s="31" t="n">
         <f aca="false">B25*1000</f>
         <v>0</v>
       </c>
@@ -26423,7 +26433,7 @@
       <c r="A26" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="30" t="n">
+      <c r="B26" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -26432,7 +26442,7 @@
       <c r="D26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="29" t="n">
+      <c r="E26" s="28" t="n">
         <f aca="false">B26*1000</f>
         <v>0</v>
       </c>
@@ -27460,7 +27470,7 @@
       <c r="A27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="30" t="n">
+      <c r="B27" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -27469,7 +27479,7 @@
       <c r="D27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="29" t="n">
+      <c r="E27" s="28" t="n">
         <f aca="false">B27*1000</f>
         <v>0</v>
       </c>
@@ -28497,7 +28507,7 @@
       <c r="A28" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="31" t="n">
+      <c r="B28" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="17" t="s">
@@ -28506,7 +28516,7 @@
       <c r="D28" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="32" t="n">
+      <c r="E28" s="31" t="n">
         <f aca="false">B28*1000</f>
         <v>0</v>
       </c>
@@ -29534,16 +29544,16 @@
       <c r="A29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="30" t="n">
+      <c r="B29" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="29" t="n">
+      <c r="E29" s="28" t="n">
         <f aca="false">B29*1000</f>
         <v>0</v>
       </c>
@@ -30571,7 +30581,7 @@
       <c r="A30" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="30" t="n">
+      <c r="B30" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -30580,7 +30590,7 @@
       <c r="D30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="29" t="n">
+      <c r="E30" s="28" t="n">
         <f aca="false">B30*1000</f>
         <v>0</v>
       </c>
@@ -31608,7 +31618,7 @@
       <c r="A31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="31" t="n">
+      <c r="B31" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="17" t="s">
@@ -31617,7 +31627,7 @@
       <c r="D31" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="32" t="n">
+      <c r="E31" s="31" t="n">
         <f aca="false">B31*1000</f>
         <v>0</v>
       </c>
@@ -32645,7 +32655,7 @@
       <c r="A32" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="30" t="n">
+      <c r="B32" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -32654,7 +32664,7 @@
       <c r="D32" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="29" t="n">
+      <c r="E32" s="28" t="n">
         <f aca="false">B32*1000</f>
         <v>0</v>
       </c>
@@ -33682,7 +33692,7 @@
       <c r="A33" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="30" t="n">
+      <c r="B33" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -33691,7 +33701,7 @@
       <c r="D33" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="29" t="n">
+      <c r="E33" s="28" t="n">
         <f aca="false">B33*1000</f>
         <v>0</v>
       </c>
@@ -34719,7 +34729,7 @@
       <c r="A34" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="31" t="n">
+      <c r="B34" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="17" t="s">
@@ -34728,7 +34738,7 @@
       <c r="D34" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="32" t="n">
+      <c r="E34" s="31" t="n">
         <f aca="false">B34*1000</f>
         <v>0</v>
       </c>
@@ -35756,16 +35766,16 @@
       <c r="A35" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="30" t="n">
+      <c r="B35" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="29" t="n">
+      <c r="E35" s="28" t="n">
         <f aca="false">B35*1000</f>
         <v>0</v>
       </c>
@@ -36793,7 +36803,7 @@
       <c r="A36" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="30" t="n">
+      <c r="B36" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -36802,7 +36812,7 @@
       <c r="D36" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="29" t="n">
+      <c r="E36" s="28" t="n">
         <f aca="false">B36*1000</f>
         <v>0</v>
       </c>
@@ -37830,7 +37840,7 @@
       <c r="A37" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="31" t="n">
+      <c r="B37" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="17" t="s">
@@ -37839,7 +37849,7 @@
       <c r="D37" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="32" t="n">
+      <c r="E37" s="31" t="n">
         <f aca="false">B37*1000</f>
         <v>0</v>
       </c>
@@ -38867,7 +38877,7 @@
       <c r="A38" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="30" t="n">
+      <c r="B38" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C38" s="12" t="s">
@@ -38876,7 +38886,7 @@
       <c r="D38" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="29" t="n">
+      <c r="E38" s="28" t="n">
         <f aca="false">B38*1000</f>
         <v>0</v>
       </c>
@@ -39904,7 +39914,7 @@
       <c r="A39" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="30" t="n">
+      <c r="B39" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C39" s="12" t="s">
@@ -39913,7 +39923,7 @@
       <c r="D39" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="29" t="n">
+      <c r="E39" s="28" t="n">
         <f aca="false">B39*1000</f>
         <v>0</v>
       </c>
@@ -40941,7 +40951,7 @@
       <c r="A40" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="31" t="n">
+      <c r="B40" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C40" s="17" t="s">
@@ -40950,7 +40960,7 @@
       <c r="D40" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="32" t="n">
+      <c r="E40" s="31" t="n">
         <f aca="false">B40*1000</f>
         <v>0</v>
       </c>
@@ -41978,16 +41988,16 @@
       <c r="A41" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="30" t="n">
+      <c r="B41" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="29" t="n">
+      <c r="E41" s="28" t="n">
         <f aca="false">B41*1000</f>
         <v>0</v>
       </c>
@@ -43015,7 +43025,7 @@
       <c r="A42" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="30" t="n">
+      <c r="B42" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="12" t="s">
@@ -43024,7 +43034,7 @@
       <c r="D42" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="29" t="n">
+      <c r="E42" s="28" t="n">
         <f aca="false">B42*1000</f>
         <v>0</v>
       </c>
@@ -44052,7 +44062,7 @@
       <c r="A43" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="31" t="n">
+      <c r="B43" s="30" t="n">
         <v>0</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -44061,7 +44071,7 @@
       <c r="D43" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="32" t="n">
+      <c r="E43" s="31" t="n">
         <f aca="false">B43*1000</f>
         <v>0</v>
       </c>
@@ -45089,7 +45099,7 @@
       <c r="A44" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="34" t="n">
+      <c r="B44" s="33" t="n">
         <v>5.47E-008</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -45098,7 +45108,7 @@
       <c r="D44" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="33" t="n">
+      <c r="E44" s="32" t="n">
         <f aca="false">B44</f>
         <v>5.47E-008</v>
       </c>
@@ -46126,7 +46136,7 @@
       <c r="A45" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="34" t="n">
+      <c r="B45" s="33" t="n">
         <v>3.23E-009</v>
       </c>
       <c r="C45" s="12" t="s">
@@ -46135,7 +46145,7 @@
       <c r="D45" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E45" s="29" t="n">
+      <c r="E45" s="28" t="n">
         <f aca="false">B45</f>
         <v>3.23E-009</v>
       </c>
@@ -47163,7 +47173,7 @@
       <c r="A46" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="34" t="n">
+      <c r="B46" s="33" t="n">
         <v>-2E-009</v>
       </c>
       <c r="C46" s="12" t="s">
@@ -47172,7 +47182,7 @@
       <c r="D46" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="29" t="n">
+      <c r="E46" s="28" t="n">
         <f aca="false">B46</f>
         <v>-2E-009</v>
       </c>
@@ -48200,7 +48210,7 @@
       <c r="A47" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B47" s="34" t="n">
+      <c r="B47" s="33" t="n">
         <v>0</v>
       </c>
       <c r="C47" s="12" t="s">
@@ -48209,7 +48219,7 @@
       <c r="D47" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E47" s="29" t="n">
+      <c r="E47" s="28" t="n">
         <f aca="false">B47</f>
         <v>0</v>
       </c>
@@ -49237,7 +49247,7 @@
       <c r="A48" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="34" t="n">
+      <c r="B48" s="33" t="n">
         <v>0</v>
       </c>
       <c r="C48" s="12" t="s">
@@ -49246,7 +49256,7 @@
       <c r="D48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="29" t="n">
+      <c r="E48" s="28" t="n">
         <f aca="false">B48</f>
         <v>0</v>
       </c>
@@ -50274,7 +50284,7 @@
       <c r="A49" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="34" t="n">
+      <c r="B49" s="33" t="n">
         <v>0</v>
       </c>
       <c r="C49" s="12" t="s">
@@ -50283,7 +50293,7 @@
       <c r="D49" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="29" t="n">
+      <c r="E49" s="28" t="n">
         <f aca="false">B49</f>
         <v>0</v>
       </c>
@@ -51311,7 +51321,7 @@
       <c r="A50" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="35" t="n">
+      <c r="B50" s="34" t="n">
         <v>0</v>
       </c>
       <c r="C50" s="17" t="s">
@@ -51320,7 +51330,7 @@
       <c r="D50" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="32" t="n">
+      <c r="E50" s="31" t="n">
         <f aca="false">B50</f>
         <v>0</v>
       </c>
@@ -52344,56 +52354,56 @@
       <c r="AMI50" s="0"/>
       <c r="AMJ50" s="0"/>
     </row>
-    <row r="51" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="36" t="s">
+    <row r="51" s="37" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="36" t="n">
+      <c r="B51" s="35" t="n">
         <v>7142.8</v>
       </c>
-      <c r="C51" s="36" t="s">
+      <c r="C51" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="37" t="n">
+      <c r="E51" s="36" t="n">
         <f aca="false">B51*1000</f>
         <v>7142800</v>
       </c>
     </row>
-    <row r="52" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="38" t="s">
+    <row r="52" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="38" t="n">
+      <c r="B52" s="37" t="n">
         <v>4456.8</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="37" t="n">
+      <c r="E52" s="36" t="n">
         <f aca="false">B52*1000</f>
         <v>4456800</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="40" t="s">
+      <c r="A53" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="40" t="n">
+      <c r="B53" s="39" t="n">
         <v>127.434</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="40" t="s">
+      <c r="D53" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="E53" s="41" t="n">
+      <c r="E53" s="40" t="n">
         <f aca="false">B53*1000</f>
         <v>127434</v>
       </c>
@@ -52401,19 +52411,19 @@
       <c r="G53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="36" t="n">
+      <c r="B54" s="35" t="n">
         <v>-3.637</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="37" t="n">
+      <c r="E54" s="36" t="n">
         <f aca="false">B54*1000</f>
         <v>-3637</v>
       </c>
@@ -52421,19 +52431,19 @@
       <c r="G54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="38" t="n">
+      <c r="B55" s="37" t="n">
         <v>5.812</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D55" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E55" s="37" t="n">
+      <c r="E55" s="36" t="n">
         <f aca="false">B55*1000</f>
         <v>5812</v>
       </c>
@@ -52441,24 +52451,24 @@
       <c r="G55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="40" t="s">
+      <c r="A56" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="40" t="n">
+      <c r="B56" s="39" t="n">
         <v>-0.5906</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E56" s="41" t="n">
+      <c r="E56" s="40" t="n">
         <f aca="false">B56*1000</f>
         <v>-590.6</v>
       </c>
-      <c r="F56" s="36"/>
-      <c r="G56" s="43"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="42"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
@@ -52473,7 +52483,7 @@
       <c r="D57" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E57" s="44" t="n">
+      <c r="E57" s="43" t="n">
         <f aca="false">B57</f>
         <v>-0.07</v>
       </c>
@@ -52493,7 +52503,7 @@
       <c r="D58" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E58" s="21" t="n">
+      <c r="E58" s="20" t="n">
         <f aca="false">B58</f>
         <v>0.1</v>
       </c>
@@ -52513,7 +52523,7 @@
       <c r="D59" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="22" t="n">
+      <c r="E59" s="21" t="n">
         <f aca="false">B59</f>
         <v>-0.04</v>
       </c>
@@ -52544,25 +52554,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="45" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="45" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="45" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>115</v>
       </c>
       <c r="F1" s="0"/>
@@ -53585,65 +53595,65 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="s">
+    <row r="2" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="46" t="n">
+      <c r="B2" s="26" t="n">
         <f aca="false">IF(Na&gt;=1,1,0)</f>
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="n">
+      <c r="C2" s="26" t="n">
         <f aca="false">B2+2</f>
         <v>3</v>
       </c>
-      <c r="D2" s="46" t="n">
+      <c r="D2" s="26" t="n">
         <f aca="false">B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="46" t="n">
+      <c r="E2" s="26" t="n">
         <f aca="false">C2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="s">
+    <row r="3" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="46" t="n">
+      <c r="B3" s="26" t="n">
         <f aca="false">C2+1</f>
         <v>4</v>
       </c>
-      <c r="C3" s="46" t="n">
+      <c r="C3" s="26" t="n">
         <f aca="false">B3+2</f>
         <v>6</v>
       </c>
-      <c r="D3" s="46" t="n">
+      <c r="D3" s="26" t="n">
         <f aca="false">B3</f>
         <v>4</v>
       </c>
-      <c r="E3" s="46" t="n">
+      <c r="E3" s="26" t="n">
         <f aca="false">C3</f>
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="46" t="n">
+      <c r="B4" s="26" t="n">
         <f aca="false">IF(Na&gt;=2,C3+1,0)</f>
         <v>7</v>
       </c>
-      <c r="C4" s="46" t="n">
+      <c r="C4" s="26" t="n">
         <f aca="false">B4+2</f>
         <v>9</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="26" t="n">
         <f aca="false">B4</f>
         <v>7</v>
       </c>
-      <c r="E4" s="46" t="n">
+      <c r="E4" s="26" t="n">
         <f aca="false">C4</f>
         <v>9</v>
       </c>
@@ -54668,22 +54678,22 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="46" t="n">
+      <c r="B5" s="26" t="n">
         <f aca="false">C4+1</f>
         <v>10</v>
       </c>
-      <c r="C5" s="46" t="n">
+      <c r="C5" s="26" t="n">
         <f aca="false">B5+2</f>
         <v>12</v>
       </c>
-      <c r="D5" s="46" t="n">
+      <c r="D5" s="26" t="n">
         <f aca="false">B5</f>
         <v>10</v>
       </c>
-      <c r="E5" s="46" t="n">
+      <c r="E5" s="26" t="n">
         <f aca="false">C5</f>
         <v>12</v>
       </c>
@@ -55707,65 +55717,65 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
+    <row r="6" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="46" t="n">
+      <c r="B6" s="26" t="n">
         <f aca="false">IF(Na&gt;=3,C5+1,0)</f>
         <v>13</v>
       </c>
-      <c r="C6" s="46" t="n">
+      <c r="C6" s="26" t="n">
         <f aca="false">B6+2</f>
         <v>15</v>
       </c>
-      <c r="D6" s="46" t="n">
+      <c r="D6" s="26" t="n">
         <f aca="false">B6</f>
         <v>13</v>
       </c>
-      <c r="E6" s="46" t="n">
+      <c r="E6" s="26" t="n">
         <f aca="false">C6</f>
         <v>15</v>
       </c>
     </row>
-    <row r="7" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="s">
+    <row r="7" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="46" t="n">
+      <c r="B7" s="26" t="n">
         <f aca="false">C6+1</f>
         <v>16</v>
       </c>
-      <c r="C7" s="46" t="n">
+      <c r="C7" s="26" t="n">
         <f aca="false">B7+2</f>
         <v>18</v>
       </c>
-      <c r="D7" s="46" t="n">
+      <c r="D7" s="26" t="n">
         <f aca="false">B7</f>
         <v>16</v>
       </c>
-      <c r="E7" s="46" t="n">
+      <c r="E7" s="26" t="n">
         <f aca="false">C7</f>
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="46" t="n">
+      <c r="B8" s="26" t="n">
         <f aca="false">IF(Na&gt;=4,C7+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="46" t="n">
+      <c r="C8" s="26" t="n">
         <f aca="false">B8+2</f>
         <v>2</v>
       </c>
-      <c r="D8" s="46" t="n">
+      <c r="D8" s="26" t="n">
         <f aca="false">B8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="46" t="n">
+      <c r="E8" s="26" t="n">
         <f aca="false">C8</f>
         <v>2</v>
       </c>
@@ -56790,22 +56800,22 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="46" t="n">
+      <c r="B9" s="26" t="n">
         <f aca="false">C8+1</f>
         <v>3</v>
       </c>
-      <c r="C9" s="46" t="n">
+      <c r="C9" s="26" t="n">
         <f aca="false">B9+2</f>
         <v>5</v>
       </c>
-      <c r="D9" s="46" t="n">
+      <c r="D9" s="26" t="n">
         <f aca="false">B9</f>
         <v>3</v>
       </c>
-      <c r="E9" s="46" t="n">
+      <c r="E9" s="26" t="n">
         <f aca="false">C9</f>
         <v>5</v>
       </c>
@@ -57829,65 +57839,65 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46" t="s">
+    <row r="10" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="46" t="n">
+      <c r="B10" s="26" t="n">
         <f aca="false">IF(Na&gt;=5,C9+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="46" t="n">
+      <c r="C10" s="26" t="n">
         <f aca="false">B10+2</f>
         <v>2</v>
       </c>
-      <c r="D10" s="46" t="n">
+      <c r="D10" s="26" t="n">
         <f aca="false">B10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="46" t="n">
+      <c r="E10" s="26" t="n">
         <f aca="false">C10</f>
         <v>2</v>
       </c>
     </row>
-    <row r="11" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="46" t="s">
+    <row r="11" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="46" t="n">
+      <c r="B11" s="26" t="n">
         <f aca="false">C10+1</f>
         <v>3</v>
       </c>
-      <c r="C11" s="46" t="n">
+      <c r="C11" s="26" t="n">
         <f aca="false">B11+2</f>
         <v>5</v>
       </c>
-      <c r="D11" s="46" t="n">
+      <c r="D11" s="26" t="n">
         <f aca="false">B11</f>
         <v>3</v>
       </c>
-      <c r="E11" s="46" t="n">
+      <c r="E11" s="26" t="n">
         <f aca="false">C11</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="46" t="n">
+      <c r="B12" s="26" t="n">
         <f aca="false">IF(Na&gt;=6,C11+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="46" t="n">
+      <c r="C12" s="26" t="n">
         <f aca="false">B12+2</f>
         <v>2</v>
       </c>
-      <c r="D12" s="46" t="n">
+      <c r="D12" s="26" t="n">
         <f aca="false">B12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="46" t="n">
+      <c r="E12" s="26" t="n">
         <f aca="false">C12</f>
         <v>2</v>
       </c>
@@ -58912,22 +58922,22 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="46" t="n">
+      <c r="B13" s="26" t="n">
         <f aca="false">C12+1</f>
         <v>3</v>
       </c>
-      <c r="C13" s="46" t="n">
+      <c r="C13" s="26" t="n">
         <f aca="false">B13+2</f>
         <v>5</v>
       </c>
-      <c r="D13" s="46" t="n">
+      <c r="D13" s="26" t="n">
         <f aca="false">B13</f>
         <v>3</v>
       </c>
-      <c r="E13" s="46" t="n">
+      <c r="E13" s="26" t="n">
         <f aca="false">C13</f>
         <v>5</v>
       </c>
@@ -59951,128 +59961,128 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46" t="s">
+    <row r="14" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="46" t="n">
+      <c r="B14" s="26" t="n">
         <f aca="false">IF(Na&gt;=7,C13+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="46" t="n">
+      <c r="C14" s="26" t="n">
         <f aca="false">B14+2</f>
         <v>2</v>
       </c>
-      <c r="D14" s="46" t="n">
+      <c r="D14" s="26" t="n">
         <f aca="false">B14</f>
         <v>0</v>
       </c>
-      <c r="E14" s="46" t="n">
+      <c r="E14" s="26" t="n">
         <f aca="false">C14</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="46" t="s">
+    <row r="15" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="46" t="n">
+      <c r="B15" s="26" t="n">
         <f aca="false">C14+1</f>
         <v>3</v>
       </c>
-      <c r="C15" s="46" t="n">
+      <c r="C15" s="26" t="n">
         <f aca="false">B15+2</f>
         <v>5</v>
       </c>
-      <c r="D15" s="46" t="n">
+      <c r="D15" s="26" t="n">
         <f aca="false">B15</f>
         <v>3</v>
       </c>
-      <c r="E15" s="46" t="n">
+      <c r="E15" s="26" t="n">
         <f aca="false">C15</f>
         <v>5</v>
       </c>
     </row>
-    <row r="16" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="46" t="s">
+    <row r="16" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="46" t="n">
+      <c r="B16" s="26" t="n">
         <f aca="false">1+6*Na</f>
         <v>19</v>
       </c>
-      <c r="C16" s="46" t="n">
+      <c r="C16" s="26" t="n">
         <f aca="false">7*Na</f>
         <v>21</v>
       </c>
-      <c r="D16" s="46" t="n">
+      <c r="D16" s="26" t="n">
         <f aca="false">B16</f>
         <v>19</v>
       </c>
-      <c r="E16" s="46" t="n">
+      <c r="E16" s="26" t="n">
         <f aca="false">C16</f>
         <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="39" t="n">
+      <c r="B17" s="38" t="n">
         <f aca="false">C16+1</f>
         <v>22</v>
       </c>
-      <c r="C17" s="39" t="n">
+      <c r="C17" s="38" t="n">
         <f aca="false">B17+2</f>
         <v>24</v>
       </c>
-      <c r="D17" s="46" t="n">
+      <c r="D17" s="26" t="n">
         <f aca="false">B17</f>
         <v>22</v>
       </c>
-      <c r="E17" s="46" t="n">
+      <c r="E17" s="26" t="n">
         <f aca="false">C17</f>
         <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="39" t="n">
+      <c r="B18" s="38" t="n">
         <f aca="false">C17+1</f>
         <v>25</v>
       </c>
-      <c r="C18" s="39" t="n">
+      <c r="C18" s="38" t="n">
         <f aca="false">B18+2</f>
         <v>27</v>
       </c>
-      <c r="D18" s="46" t="n">
+      <c r="D18" s="26" t="n">
         <f aca="false">B18</f>
         <v>25</v>
       </c>
-      <c r="E18" s="46" t="n">
+      <c r="E18" s="26" t="n">
         <f aca="false">C18</f>
         <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="39" t="n">
+      <c r="B19" s="38" t="n">
         <f aca="false">C18+1</f>
         <v>28</v>
       </c>
-      <c r="C19" s="39" t="n">
+      <c r="C19" s="38" t="n">
         <f aca="false">B19+2</f>
         <v>30</v>
       </c>
-      <c r="D19" s="46" t="n">
+      <c r="D19" s="26" t="n">
         <f aca="false">B19</f>
         <v>28</v>
       </c>
-      <c r="E19" s="46" t="n">
+      <c r="E19" s="26" t="n">
         <f aca="false">C19</f>
         <v>30</v>
       </c>
@@ -60103,8 +60113,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60234,262 +60244,262 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.9878542510121"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.8461538461539"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="52" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="54" t="n">
+      <c r="E2" s="51" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="55" t="n">
+      <c r="B3" s="52" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="54" t="n">
+      <c r="E3" s="51" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
-      <c r="F3" s="56"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="58" t="n">
+      <c r="B4" s="55" t="n">
         <v>0.05</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="60" t="n">
+      <c r="E4" s="57" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="55" t="n">
+      <c r="B5" s="52" t="n">
         <v>20</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="54" t="n">
+      <c r="E5" s="51" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="55" t="n">
+      <c r="B6" s="52" t="n">
         <v>20</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="54" t="n">
+      <c r="E6" s="51" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="55" t="n">
+      <c r="B7" s="52" t="n">
         <v>1.5</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="54" t="n">
+      <c r="E7" s="51" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="55" t="n">
+      <c r="B8" s="52" t="n">
         <v>1.5</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="54" t="n">
+      <c r="E8" s="51" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="55" t="n">
+      <c r="B9" s="52" t="n">
         <v>9</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="54" t="n">
+      <c r="E9" s="51" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="62" t="n">
+      <c r="B10" s="59" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="E10" s="64" t="n">
+      <c r="E10" s="61" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="65" t="n">
+      <c r="B11" s="62" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="60" t="n">
+      <c r="E11" s="57" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="66" t="n">
+      <c r="B12" s="63" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="56" t="n">
+      <c r="E12" s="53" t="n">
         <f aca="false">B12/3</f>
         <v>3.33333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="66" t="n">
+      <c r="B13" s="63" t="n">
         <v>100</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="E13" s="56" t="n">
+      <c r="E13" s="53" t="n">
         <f aca="false">B13/3</f>
         <v>33.3333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="66" t="n">
+      <c r="B14" s="63" t="n">
         <v>10</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="E14" s="56" t="n">
+      <c r="E14" s="53" t="n">
         <f aca="false">B14/3</f>
         <v>3.33333333333333</v>
       </c>
@@ -60518,360 +60528,360 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="53" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="67" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="53" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="50" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="68" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="63" t="n">
+      <c r="B2" s="60" t="n">
         <v>4000</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="64" t="n">
+      <c r="E2" s="61" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="53" t="n">
+      <c r="B3" s="50" t="n">
         <v>4000</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="E3" s="54" t="n">
+      <c r="E3" s="51" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="53" t="n">
+      <c r="B4" s="50" t="n">
         <v>4000</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="54" t="n">
+      <c r="E4" s="51" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="53" t="n">
+      <c r="B5" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E5" s="54" t="n">
+      <c r="E5" s="51" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="53" t="n">
+      <c r="B6" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="54" t="n">
+      <c r="E6" s="51" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="B7" s="53" t="n">
+      <c r="B7" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="54" t="n">
+      <c r="E7" s="51" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="53" t="n">
+      <c r="B8" s="50" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="54" t="n">
+      <c r="E8" s="51" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="B9" s="53" t="n">
+      <c r="B9" s="50" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="E9" s="54" t="n">
+      <c r="E9" s="51" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="B10" s="53" t="n">
+      <c r="B10" s="50" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="E10" s="54" t="n">
+      <c r="E10" s="51" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="B11" s="53" t="n">
+      <c r="B11" s="50" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="54" t="n">
+      <c r="E11" s="51" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="B12" s="53" t="n">
+      <c r="B12" s="50" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="E12" s="54" t="n">
+      <c r="E12" s="51" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="B13" s="53" t="n">
+      <c r="B13" s="50" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="54" t="n">
+      <c r="E13" s="51" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="B14" s="53" t="n">
+      <c r="B14" s="50" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="54" t="n">
+      <c r="E14" s="51" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="B15" s="53" t="n">
+      <c r="B15" s="50" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="54" t="n">
+      <c r="E15" s="51" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="53" t="n">
+      <c r="B16" s="50" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D16" s="53" t="s">
+      <c r="D16" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="54" t="n">
+      <c r="E16" s="51" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="53" t="n">
+      <c r="B17" s="50" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="E17" s="54" t="n">
+      <c r="E17" s="51" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="53" t="n">
+      <c r="B18" s="50" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="E18" s="54" t="n">
+      <c r="E18" s="51" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="59" t="n">
+      <c r="B19" s="56" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D19" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="E19" s="60" t="n">
+      <c r="E19" s="57" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -60900,319 +60910,319 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="67" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="53" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="49.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="67" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="53" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="64" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="50.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="str">
+      <c r="A2" s="48" t="str">
         <f aca="false">truthStateParams!A2</f>
         <v>Q_grav</v>
       </c>
-      <c r="B2" s="52" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">truthStateParams!B2</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="53" t="str">
+      <c r="C2" s="50" t="str">
         <f aca="false">truthStateParams!C2</f>
         <v>m^2/s^3</v>
       </c>
-      <c r="D2" s="53" t="str">
+      <c r="D2" s="50" t="str">
         <f aca="false">truthStateParams!D2</f>
         <v>3-sigma non-gravitational process noise</v>
       </c>
-      <c r="E2" s="54" t="n">
+      <c r="E2" s="51" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="str">
+      <c r="A3" s="48" t="str">
         <f aca="false">truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
       </c>
-      <c r="B3" s="55" t="n">
+      <c r="B3" s="52" t="n">
         <f aca="false">truthStateParams!B3</f>
         <v>5</v>
       </c>
-      <c r="C3" s="52" t="str">
+      <c r="C3" s="49" t="str">
         <f aca="false">truthStateParams!C3</f>
         <v>deg/hr</v>
       </c>
-      <c r="D3" s="53" t="str">
+      <c r="D3" s="50" t="str">
         <f aca="false">truthStateParams!D3</f>
         <v>3-sigma steady-state gyro bias</v>
       </c>
-      <c r="E3" s="54" t="n">
+      <c r="E3" s="51" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="str">
+      <c r="A4" s="54" t="str">
         <f aca="false">truthStateParams!A4</f>
         <v>arw</v>
       </c>
-      <c r="B4" s="58" t="n">
+      <c r="B4" s="55" t="n">
         <f aca="false">truthStateParams!B4</f>
         <v>0.05</v>
       </c>
-      <c r="C4" s="59" t="str">
+      <c r="C4" s="56" t="str">
         <f aca="false">truthStateParams!C4</f>
         <v>deg/sqrt(hr)</v>
       </c>
-      <c r="D4" s="59" t="str">
+      <c r="D4" s="56" t="str">
         <f aca="false">truthStateParams!D4</f>
         <v>3-sigma angular random walk</v>
       </c>
-      <c r="E4" s="60" t="n">
+      <c r="E4" s="57" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
-      <c r="F4" s="73"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="str">
+      <c r="A5" s="48" t="str">
         <f aca="false">truthStateParams!A5</f>
         <v>sig_st_ss</v>
       </c>
-      <c r="B5" s="55" t="n">
+      <c r="B5" s="52" t="n">
         <f aca="false">truthStateParams!B5</f>
         <v>20</v>
       </c>
-      <c r="C5" s="53" t="str">
+      <c r="C5" s="50" t="str">
         <f aca="false">truthStateParams!C5</f>
         <v>arcsec/axis</v>
       </c>
-      <c r="D5" s="53" t="str">
+      <c r="D5" s="50" t="str">
         <f aca="false">truthStateParams!D5</f>
         <v>3-sigma steady-state star camera misalignment</v>
       </c>
-      <c r="E5" s="54" t="n">
+      <c r="E5" s="51" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
-      <c r="F5" s="73"/>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="str">
+      <c r="A6" s="48" t="str">
         <f aca="false">truthStateParams!A6</f>
         <v>sig_c_ss</v>
       </c>
-      <c r="B6" s="55" t="n">
+      <c r="B6" s="52" t="n">
         <f aca="false">truthStateParams!B6</f>
         <v>20</v>
       </c>
-      <c r="C6" s="53" t="str">
+      <c r="C6" s="50" t="str">
         <f aca="false">truthStateParams!C6</f>
         <v>arcsec/axis</v>
       </c>
-      <c r="D6" s="53" t="str">
+      <c r="D6" s="50" t="str">
         <f aca="false">truthStateParams!D6</f>
         <v>3-sigma steady-state terrain camera misalignment</v>
       </c>
-      <c r="E6" s="54" t="n">
+      <c r="E6" s="51" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="str">
+      <c r="A7" s="48" t="str">
         <f aca="false">truthStateParams!A7</f>
         <v>sig_meas_stx</v>
       </c>
-      <c r="B7" s="55" t="n">
+      <c r="B7" s="52" t="n">
         <f aca="false">truthStateParams!B7</f>
         <v>1.5</v>
       </c>
-      <c r="C7" s="53" t="str">
+      <c r="C7" s="50" t="str">
         <f aca="false">truthStateParams!C7</f>
         <v>arcsec</v>
       </c>
-      <c r="D7" s="53" t="str">
+      <c r="D7" s="50" t="str">
         <f aca="false">truthStateParams!D7</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E7" s="54" t="n">
+      <c r="E7" s="51" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="str">
+      <c r="A8" s="48" t="str">
         <f aca="false">truthStateParams!A8</f>
         <v>sig_meas_sty</v>
       </c>
-      <c r="B8" s="55" t="n">
+      <c r="B8" s="52" t="n">
         <f aca="false">truthStateParams!B8</f>
         <v>1.5</v>
       </c>
-      <c r="C8" s="53" t="str">
+      <c r="C8" s="50" t="str">
         <f aca="false">truthStateParams!C8</f>
         <v>arcsec</v>
       </c>
-      <c r="D8" s="53" t="str">
+      <c r="D8" s="50" t="str">
         <f aca="false">truthStateParams!D8</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E8" s="54" t="n">
+      <c r="E8" s="51" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="str">
+      <c r="A9" s="48" t="str">
         <f aca="false">truthStateParams!A9</f>
         <v>sig_meas_stz</v>
       </c>
-      <c r="B9" s="55" t="n">
+      <c r="B9" s="52" t="n">
         <f aca="false">truthStateParams!B9</f>
         <v>9</v>
       </c>
-      <c r="C9" s="53" t="str">
+      <c r="C9" s="50" t="str">
         <f aca="false">truthStateParams!C9</f>
         <v>arcsec</v>
       </c>
-      <c r="D9" s="53" t="str">
+      <c r="D9" s="50" t="str">
         <f aca="false">truthStateParams!D9</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E9" s="54" t="n">
+      <c r="E9" s="51" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="str">
+      <c r="A10" s="58" t="str">
         <f aca="false">truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
-      <c r="B10" s="62" t="n">
+      <c r="B10" s="59" t="n">
         <f aca="false">truthStateParams!B10</f>
         <v>3</v>
       </c>
-      <c r="C10" s="63" t="str">
+      <c r="C10" s="60" t="str">
         <f aca="false">truthStateParams!C10</f>
         <v>pixels</v>
       </c>
-      <c r="D10" s="63" t="str">
+      <c r="D10" s="60" t="str">
         <f aca="false">truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
-      <c r="E10" s="64" t="n">
+      <c r="E10" s="61" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="57" t="str">
+      <c r="A11" s="54" t="str">
         <f aca="false">truthStateParams!A11</f>
         <v>sig_cv</v>
       </c>
-      <c r="B11" s="65" t="n">
+      <c r="B11" s="62" t="n">
         <f aca="false">truthStateParams!B11</f>
         <v>3</v>
       </c>
-      <c r="C11" s="59" t="str">
+      <c r="C11" s="56" t="str">
         <f aca="false">truthStateParams!C11</f>
         <v>pixels</v>
       </c>
-      <c r="D11" s="59" t="str">
+      <c r="D11" s="56" t="str">
         <f aca="false">truthStateParams!D11</f>
         <v>3-sigma v component of pixel noise</v>
       </c>
-      <c r="E11" s="60" t="n">
+      <c r="E11" s="57" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="57" t="str">
+      <c r="A12" s="54" t="str">
         <f aca="false">truthStateParams!A12</f>
         <v>sig_idpos</v>
       </c>
-      <c r="B12" s="65" t="n">
+      <c r="B12" s="62" t="n">
         <f aca="false">truthStateParams!B12</f>
         <v>10</v>
       </c>
-      <c r="C12" s="59" t="str">
+      <c r="C12" s="56" t="str">
         <f aca="false">truthStateParams!C12</f>
         <v>m</v>
       </c>
-      <c r="D12" s="59" t="str">
+      <c r="D12" s="56" t="str">
         <f aca="false">truthStateParams!D12</f>
         <v>3-sigma change in inertial position measurement uncertainty</v>
       </c>
-      <c r="E12" s="60" t="n">
+      <c r="E12" s="57" t="n">
         <f aca="false">B12/3</f>
         <v>3.33333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="57" t="str">
+      <c r="A13" s="54" t="str">
         <f aca="false">truthStateParams!A13</f>
         <v>sig_loss</v>
       </c>
-      <c r="B13" s="65" t="n">
+      <c r="B13" s="62" t="n">
         <f aca="false">truthStateParams!B13</f>
         <v>100</v>
       </c>
-      <c r="C13" s="59" t="str">
+      <c r="C13" s="56" t="str">
         <f aca="false">truthStateParams!C13</f>
         <v>m</v>
       </c>
-      <c r="D13" s="59" t="str">
+      <c r="D13" s="56" t="str">
         <f aca="false">truthStateParams!D13</f>
         <v>3-sigma LOSS feature location uncertainty</v>
       </c>
-      <c r="E13" s="60" t="n">
+      <c r="E13" s="57" t="n">
         <f aca="false">B13/3</f>
         <v>33.3333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="57" t="str">
+      <c r="A14" s="54" t="str">
         <f aca="false">truthStateParams!A14</f>
         <v>sig_mdpos</v>
       </c>
-      <c r="B14" s="65" t="n">
+      <c r="B14" s="62" t="n">
         <f aca="false">truthStateParams!B14</f>
         <v>10</v>
       </c>
-      <c r="C14" s="59" t="str">
+      <c r="C14" s="56" t="str">
         <f aca="false">truthStateParams!C14</f>
         <v>m</v>
       </c>
-      <c r="D14" s="59" t="str">
+      <c r="D14" s="56" t="str">
         <f aca="false">truthStateParams!D14</f>
         <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
       </c>
-      <c r="E14" s="60" t="n">
+      <c r="E14" s="57" t="n">
         <f aca="false">B14/3</f>
         <v>3.33333333333333</v>
       </c>
@@ -61241,428 +61251,428 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="53" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="67" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="53" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="50" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="68" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="str">
+      <c r="A2" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
       </c>
-      <c r="B2" s="53" t="n">
+      <c r="B2" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
         <v>4000</v>
       </c>
-      <c r="C2" s="53" t="str">
+      <c r="C2" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
         <v>m</v>
       </c>
-      <c r="D2" s="53" t="str">
+      <c r="D2" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="75" t="n">
+      <c r="E2" s="72" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F2" s="73"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="str">
+      <c r="A3" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
       </c>
-      <c r="B3" s="53" t="n">
+      <c r="B3" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
         <v>4000</v>
       </c>
-      <c r="C3" s="53" t="str">
+      <c r="C3" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
         <v>m</v>
       </c>
-      <c r="D3" s="53" t="str">
+      <c r="D3" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="75" t="n">
+      <c r="E3" s="72" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="str">
+      <c r="A4" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
       </c>
-      <c r="B4" s="53" t="n">
+      <c r="B4" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
         <v>4000</v>
       </c>
-      <c r="C4" s="53" t="str">
+      <c r="C4" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="53" t="str">
+      <c r="D4" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="75" t="n">
+      <c r="E4" s="72" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F4" s="73"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="str">
+      <c r="A5" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
       </c>
-      <c r="B5" s="53" t="n">
+      <c r="B5" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
         <v>3</v>
       </c>
-      <c r="C5" s="53" t="str">
+      <c r="C5" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="53" t="str">
+      <c r="D5" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="75" t="n">
+      <c r="E5" s="72" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
-      <c r="F5" s="73"/>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="str">
+      <c r="A6" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
       </c>
-      <c r="B6" s="53" t="n">
+      <c r="B6" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
         <v>3</v>
       </c>
-      <c r="C6" s="53" t="str">
+      <c r="C6" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="53" t="str">
+      <c r="D6" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="75" t="n">
+      <c r="E6" s="72" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="51" t="str">
+      <c r="A7" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
       </c>
-      <c r="B7" s="53" t="n">
+      <c r="B7" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
         <v>3</v>
       </c>
-      <c r="C7" s="53" t="str">
+      <c r="C7" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="53" t="str">
+      <c r="D7" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="75" t="n">
+      <c r="E7" s="72" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="51" t="str">
+      <c r="A8" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
       </c>
-      <c r="B8" s="53" t="n">
+      <c r="B8" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B8</f>
         <v>0.0005</v>
       </c>
-      <c r="C8" s="53" t="str">
+      <c r="C8" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C8</f>
         <v>rad</v>
       </c>
-      <c r="D8" s="53" t="str">
+      <c r="D8" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="75" t="n">
+      <c r="E8" s="72" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="51" t="str">
+      <c r="A9" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
       </c>
-      <c r="B9" s="53" t="n">
+      <c r="B9" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B9</f>
         <v>0.0005</v>
       </c>
-      <c r="C9" s="53" t="str">
+      <c r="C9" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C9</f>
         <v>rad</v>
       </c>
-      <c r="D9" s="53" t="str">
+      <c r="D9" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="75" t="n">
+      <c r="E9" s="72" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="str">
+      <c r="A10" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
       </c>
-      <c r="B10" s="53" t="n">
+      <c r="B10" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B10</f>
         <v>0.0005</v>
       </c>
-      <c r="C10" s="53" t="str">
+      <c r="C10" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C10</f>
         <v>rad</v>
       </c>
-      <c r="D10" s="53" t="str">
+      <c r="D10" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="75" t="n">
+      <c r="E10" s="72" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51" t="str">
+      <c r="A11" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
       </c>
-      <c r="B11" s="53" t="n">
+      <c r="B11" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B11</f>
         <v>20</v>
       </c>
-      <c r="C11" s="53" t="str">
+      <c r="C11" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C11</f>
         <v>arcsec</v>
       </c>
-      <c r="D11" s="53" t="str">
+      <c r="D11" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="75" t="n">
+      <c r="E11" s="72" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51" t="str">
+      <c r="A12" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
       </c>
-      <c r="B12" s="53" t="n">
+      <c r="B12" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B12</f>
         <v>20</v>
       </c>
-      <c r="C12" s="53" t="str">
+      <c r="C12" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C12</f>
         <v>arcsec</v>
       </c>
-      <c r="D12" s="53" t="str">
+      <c r="D12" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="75" t="n">
+      <c r="E12" s="72" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="51" t="str">
+      <c r="A13" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
       </c>
-      <c r="B13" s="53" t="n">
+      <c r="B13" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B13</f>
         <v>20</v>
       </c>
-      <c r="C13" s="53" t="str">
+      <c r="C13" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C13</f>
         <v>arcsec</v>
       </c>
-      <c r="D13" s="53" t="str">
+      <c r="D13" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="75" t="n">
+      <c r="E13" s="72" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="51" t="str">
+      <c r="A14" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
       </c>
-      <c r="B14" s="53" t="n">
+      <c r="B14" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B14</f>
         <v>20</v>
       </c>
-      <c r="C14" s="53" t="str">
+      <c r="C14" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C14</f>
         <v>arcsec</v>
       </c>
-      <c r="D14" s="53" t="str">
+      <c r="D14" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="75" t="n">
+      <c r="E14" s="72" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="51" t="str">
+      <c r="A15" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
       </c>
-      <c r="B15" s="53" t="n">
+      <c r="B15" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B15</f>
         <v>20</v>
       </c>
-      <c r="C15" s="53" t="str">
+      <c r="C15" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C15</f>
         <v>arcsec</v>
       </c>
-      <c r="D15" s="53" t="str">
+      <c r="D15" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="75" t="n">
+      <c r="E15" s="72" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="51" t="str">
+      <c r="A16" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
       </c>
-      <c r="B16" s="53" t="n">
+      <c r="B16" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B16</f>
         <v>20</v>
       </c>
-      <c r="C16" s="53" t="str">
+      <c r="C16" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C16</f>
         <v>arcsec</v>
       </c>
-      <c r="D16" s="53" t="str">
+      <c r="D16" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="75" t="n">
+      <c r="E16" s="72" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="51" t="str">
+      <c r="A17" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B17" s="53" t="n">
+      <c r="B17" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B17</f>
         <v>5</v>
       </c>
-      <c r="C17" s="53" t="str">
+      <c r="C17" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C17</f>
         <v>deg/hr</v>
       </c>
-      <c r="D17" s="53" t="str">
+      <c r="D17" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="75" t="n">
+      <c r="E17" s="72" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="51" t="str">
+      <c r="A18" s="48" t="str">
         <f aca="false">truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B18" s="53" t="n">
+      <c r="B18" s="50" t="n">
         <f aca="false">truthStateInitialUncertainty!B18</f>
         <v>5</v>
       </c>
-      <c r="C18" s="53" t="str">
+      <c r="C18" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!C18</f>
         <v>deg/hr</v>
       </c>
-      <c r="D18" s="53" t="str">
+      <c r="D18" s="50" t="str">
         <f aca="false">truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="75" t="n">
+      <c r="E18" s="72" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="57" t="str">
+      <c r="A19" s="54" t="str">
         <f aca="false">truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B19" s="59" t="n">
+      <c r="B19" s="56" t="n">
         <f aca="false">truthStateInitialUncertainty!B19</f>
         <v>5</v>
       </c>
-      <c r="C19" s="59" t="str">
+      <c r="C19" s="56" t="str">
         <f aca="false">truthStateInitialUncertainty!C19</f>
         <v>deg/hr</v>
       </c>
-      <c r="D19" s="59" t="str">
+      <c r="D19" s="56" t="str">
         <f aca="false">truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="76" t="n">
+      <c r="E19" s="73" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -61693,292 +61703,292 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="77" t="n">
+      <c r="B2" s="74" t="n">
         <v>1.1E-009</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="78" t="n">
+      <c r="D2" s="60"/>
+      <c r="E2" s="75" t="n">
         <f aca="false">B2</f>
         <v>1.1E-009</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="79" t="n">
+      <c r="B3" s="76" t="n">
         <v>-2.45E-008</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="80" t="n">
+      <c r="D3" s="50"/>
+      <c r="E3" s="77" t="n">
         <f aca="false">B3</f>
         <v>-2.45E-008</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="79" t="n">
+      <c r="B4" s="76" t="n">
         <v>5.4E-009</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="80" t="n">
+      <c r="D4" s="50"/>
+      <c r="E4" s="77" t="n">
         <f aca="false">B4</f>
         <v>5.4E-009</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="79" t="n">
+      <c r="B5" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="80" t="n">
+      <c r="D5" s="50"/>
+      <c r="E5" s="77" t="n">
         <f aca="false">B5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="79" t="n">
+      <c r="B6" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="80" t="n">
+      <c r="D6" s="50"/>
+      <c r="E6" s="77" t="n">
         <f aca="false">B6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="79" t="n">
+      <c r="B7" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="80" t="n">
+      <c r="D7" s="50"/>
+      <c r="E7" s="77" t="n">
         <f aca="false">B7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="79" t="n">
+      <c r="B8" s="76" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="80" t="n">
+      <c r="D8" s="50"/>
+      <c r="E8" s="77" t="n">
         <f aca="false">B8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="53" t="n">
+      <c r="B9" s="50" t="n">
         <v>25</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="75" t="n">
+      <c r="D9" s="50"/>
+      <c r="E9" s="72" t="n">
         <f aca="false">B9*1000</f>
         <v>25000</v>
       </c>
-      <c r="F9" s="53"/>
+      <c r="F9" s="50"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="53" t="n">
+      <c r="B10" s="50" t="n">
         <v>47</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="75" t="n">
+      <c r="D10" s="50"/>
+      <c r="E10" s="72" t="n">
         <f aca="false">B10*1000</f>
         <v>47000</v>
       </c>
-      <c r="F10" s="53"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="53" t="n">
+      <c r="B11" s="50" t="n">
         <v>-32</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="75" t="n">
+      <c r="D11" s="50"/>
+      <c r="E11" s="72" t="n">
         <f aca="false">B11*1000</f>
         <v>-32000</v>
       </c>
-      <c r="F11" s="53"/>
+      <c r="F11" s="50"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="53" t="n">
+      <c r="B12" s="50" t="n">
         <v>16</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="75" t="n">
+      <c r="D12" s="50"/>
+      <c r="E12" s="72" t="n">
         <f aca="false">B12*1000</f>
         <v>16000</v>
       </c>
-      <c r="F12" s="53"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="53" t="n">
+      <c r="B13" s="50" t="n">
         <v>-29</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="75" t="n">
+      <c r="D13" s="50"/>
+      <c r="E13" s="72" t="n">
         <f aca="false">B13*1000</f>
         <v>-29000</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="50"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="53" t="n">
+      <c r="B14" s="50" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="75" t="n">
+      <c r="D14" s="50"/>
+      <c r="E14" s="72" t="n">
         <f aca="false">B14*1000</f>
         <v>13000</v>
       </c>
-      <c r="F14" s="53"/>
+      <c r="F14" s="50"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="53" t="n">
+      <c r="B15" s="50" t="n">
         <v>0.01</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="75" t="n">
+      <c r="D15" s="50"/>
+      <c r="E15" s="72" t="n">
         <f aca="false">B15</f>
         <v>0.01</v>
       </c>
-      <c r="F15" s="53"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="53" t="n">
+      <c r="B16" s="50" t="n">
         <v>-0.01</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="75" t="n">
+      <c r="D16" s="50"/>
+      <c r="E16" s="72" t="n">
         <f aca="false">B16</f>
         <v>-0.01</v>
       </c>
-      <c r="F16" s="53"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="59" t="n">
+      <c r="B17" s="56" t="n">
         <v>-0.01</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="76" t="n">
+      <c r="D17" s="56"/>
+      <c r="E17" s="73" t="n">
         <f aca="false">B17</f>
         <v>-0.01</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="50"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
working on validation of H
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1176,12 +1176,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.3846153846154"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="82.2672064777328"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="82.9109311740891"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1297,7 +1297,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>13</v>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="E7" s="13" t="n">
         <f aca="false">B7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,7 +1413,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4736842105263"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1535,8 +1535,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="79.1619433198381"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="79.8016194331984"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -52571,7 +52571,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60129,8 +60129,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60260,10 +60260,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.2753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60546,9 +60546,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="50" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="50" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="55.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="56.2388663967611"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -60928,10 +60928,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="50" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="64" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="50.5587044534413"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="50.9878542510121"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -61269,9 +61269,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="50" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="50" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="55.8097165991903"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="56.2388663967611"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="64" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -61717,11 +61717,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1457489878543"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.2388663967611"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
working towards covariance prop 1
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="203">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -448,175 +448,175 @@
     <t xml:space="preserve">vt</t>
   </si>
   <si>
-    <t xml:space="preserve">Q_grav</t>
+    <t xml:space="preserve">sig_b1_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">m^2/s^3</t>
+    <t xml:space="preserve">sec/sec</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma non-gravitational process noise</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 1</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_gyro_ss</t>
+    <t xml:space="preserve">sig_b2_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">deg/hr</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 2</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma steady-state gyro bias</t>
+    <t xml:space="preserve">sig_b3_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">arw</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 3</t>
   </si>
   <si>
-    <t xml:space="preserve">deg/sqrt(hr)</t>
+    <t xml:space="preserve">sig_b4_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma angular random walk</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 4</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_st_ss</t>
+    <t xml:space="preserve">sig_b5_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">arcsec/axis</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 5</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma steady-state star camera misalignment</t>
+    <t xml:space="preserve">sig_b6_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_c_ss</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 6</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma steady-state terrain camera misalignment</t>
+    <t xml:space="preserve">sig_b7_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_meas_stx</t>
+    <t xml:space="preserve">3-sigma bias propagation noise of asset 7</t>
   </si>
   <si>
-    <t xml:space="preserve">arcsec</t>
+    <t xml:space="preserve">Q_grav_x</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma star camera measurement uncertainty</t>
+    <t xml:space="preserve">m^2/sec^3</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_meas_sty</t>
+    <t xml:space="preserve">3-sigma of RSO x accelerations</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_meas_stz</t>
+    <t xml:space="preserve">Q_grav_y</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_cu</t>
+    <t xml:space="preserve">3-sigma of RSO y accelerations</t>
   </si>
   <si>
-    <t xml:space="preserve">pixels</t>
+    <t xml:space="preserve">Q_grav_z</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma u component of pixel noise</t>
+    <t xml:space="preserve">3-sigma of RSO z accelerations</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_cv</t>
+    <t xml:space="preserve">sig_ax_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma v component of pixel noise</t>
+    <t xml:space="preserve">3-sigma of RSO x atmo acceleration</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_idpos</t>
+    <t xml:space="preserve">sig_ay_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">m</t>
+    <t xml:space="preserve">4-sigma of RSO y atmo acceleration</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma change in inertial position measurement uncertainty</t>
+    <t xml:space="preserve">sig_az_ss</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_loss</t>
+    <t xml:space="preserve">5-sigma of RSO z atmo acceleration</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma LOSS feature location uncertainty</t>
+    <t xml:space="preserve">sig_b1</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_mdpos</t>
+    <t xml:space="preserve">3-sigma clocking bias of asset 1</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma change in lunar-referenced position measurement uncertainty</t>
+    <t xml:space="preserve">sig_b2</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_rsx</t>
+    <t xml:space="preserve">3-sigma clocking bias of asset 2</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma initial satellite position uncertainty</t>
+    <t xml:space="preserve">sig_b3</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_rsy</t>
+    <t xml:space="preserve">3-sigma clocking bias of asset 3</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_rsz</t>
+    <t xml:space="preserve">sig_b4</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_vsx</t>
+    <t xml:space="preserve">3-sigma clocking bias of asset 4</t>
   </si>
   <si>
-    <t xml:space="preserve">m/sec</t>
+    <t xml:space="preserve">sig_b5</t>
   </si>
   <si>
-    <t xml:space="preserve">3-sigma initial satellite velocity uncertainty</t>
+    <t xml:space="preserve">3-sigma clocking bias of asset 5</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_vsy</t>
+    <t xml:space="preserve">sig_b6</t>
   </si>
   <si>
-    <t xml:space="preserve">sig_vsz</t>
+    <t xml:space="preserve">3-sigma clocking bias of asset 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_b7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma clocking bias of asset 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma of RSO x position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma of RSO y position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_pz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma of RSO z position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_vx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma of RSO x velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_vy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma of RSO y velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sig_vz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-sigma of RSO z velocity</t>
   </si>
   <si>
     <t xml:space="preserve">sig_ax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-sigma initial satellite orientation uncertainty</t>
   </si>
   <si>
     <t xml:space="preserve">sig_ay</t>
   </si>
   <si>
     <t xml:space="preserve">sig_az</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_thstx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-sigma initial star camera misalignment uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_thsty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_thstz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_thcx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-sigma initial terrain camera misalignment uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_thcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_thcz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_gyrox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-sigma initial gyro bias uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_gyroy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sig_gyroz</t>
   </si>
   <si>
     <t xml:space="preserve">hrs2min</t>
@@ -830,7 +830,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1007,11 +1007,79 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1019,7 +1087,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1027,23 +1095,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1051,79 +1107,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1140,6 +1132,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1168,20 +1164,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.3481781376518"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="82.9109311740891"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="85.1578947368421"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1297,7 +1293,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>13</v>
@@ -1307,7 +1303,7 @@
       </c>
       <c r="E7" s="13" t="n">
         <f aca="false">B7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,6 +1384,8 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1406,22 +1404,22 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1470,7 +1468,7 @@
       <c r="A7" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B7" s="79" t="n">
+      <c r="B7" s="78" t="n">
         <f aca="false">398600.4418*(km2m^3)</f>
         <v>398600441800000</v>
       </c>
@@ -1526,8 +1524,8 @@
   </sheetPr>
   <dimension ref="1:59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1535,8 +1533,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="79.8016194331984"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="81.9473684210526"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -52564,14 +52562,14 @@
   </sheetPr>
   <dimension ref="1:19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60121,7 +60119,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -60129,8 +60127,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60250,24 +60248,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.7044534412956"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.9878542510122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -60284,242 +60282,244 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
         <v>136</v>
       </c>
       <c r="B2" s="49" t="n">
-        <f aca="false">0.00000016*3</f>
-        <v>4.8E-007</v>
-      </c>
-      <c r="C2" s="50" t="s">
+        <v>1E-007</v>
+      </c>
+      <c r="C2" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="51" t="n">
+      <c r="E2" s="50" t="n">
         <f aca="false">B2/3</f>
-        <v>1.6E-007</v>
+        <v>3.33333333333333E-008</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="52" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="49" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="E3" s="50" t="n">
+        <f aca="false">B3/3</f>
+        <v>3.33333333333333E-008</v>
+      </c>
+      <c r="F3" s="51"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="51" t="n">
-        <f aca="false">RADIANS(B3)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
-      <c r="F3" s="53"/>
+      <c r="B4" s="49" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="50" t="n">
+        <f aca="false">B4/3</f>
+        <v>3.33333333333333E-008</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="55" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C4" s="56" t="s">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="B5" s="49" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="E4" s="57" t="n">
-        <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
-        <v>4.84813681109536E-006</v>
+      <c r="E5" s="50" t="n">
+        <f aca="false">B5/3</f>
+        <v>3.33333333333333E-008</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="52" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" s="50" t="s">
+      <c r="B6" s="49" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="E6" s="50" t="n">
+        <f aca="false">B6/3</f>
+        <v>3.33333333333333E-008</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="51" t="n">
-        <f aca="false">RADIANS(B5)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+      <c r="B7" s="49" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="50" t="n">
+        <f aca="false">B7/3</f>
+        <v>3.33333333333333E-008</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="52" t="n">
-        <v>20</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" s="50" t="s">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="51" t="n">
-        <f aca="false">RADIANS(B6)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+      <c r="B8" s="49" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="50" t="n">
+        <f aca="false">B8/3</f>
+        <v>3.33333333333333E-008</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" s="52" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="C7" s="50" t="s">
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="B9" s="49" t="n">
+        <v>4.8E-007</v>
+      </c>
+      <c r="C9" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="51" t="n">
-        <f aca="false">RADIANS(B7)/3600/3</f>
-        <v>2.42406840554768E-006</v>
+      <c r="D9" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="50" t="n">
+        <f aca="false">B9/3</f>
+        <v>1.6E-007</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" s="52" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="50" t="s">
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="49" t="n">
+        <v>4.8E-007</v>
+      </c>
+      <c r="C10" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="E8" s="51" t="n">
-        <f aca="false">RADIANS(B8)/3600/3</f>
-        <v>2.42406840554768E-006</v>
+      <c r="D10" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="50" t="n">
+        <f aca="false">B10/3</f>
+        <v>1.6E-007</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="52" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9" s="50" t="s">
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="49" t="n">
+        <v>4.8E-007</v>
+      </c>
+      <c r="C11" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="51" t="n">
-        <f aca="false">RADIANS(B9)/3600/3</f>
-        <v>1.45444104332861E-005</v>
+      <c r="D11" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="50" t="n">
+        <f aca="false">B11/3</f>
+        <v>1.6E-007</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="59" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="61" t="n">
-        <f aca="false">B10/3</f>
-        <v>1</v>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="50" t="n">
+        <f aca="false">B12/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="54" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="62" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="56" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="57" t="n">
-        <f aca="false">B11/3</f>
-        <v>1</v>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="50" t="n">
+        <f aca="false">B13/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="63" t="n">
-        <v>10</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="50" t="s">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="53" t="n">
-        <f aca="false">B12/3</f>
-        <v>3.33333333333333</v>
+      <c r="B14" s="48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="50" t="n">
+        <f aca="false">B14/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="B13" s="63" t="n">
-        <v>100</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" s="53" t="n">
-        <f aca="false">B13/3</f>
-        <v>33.3333333333333</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="63" t="n">
-        <v>10</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" s="53" t="n">
-        <f aca="false">B14/3</f>
-        <v>3.33333333333333</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -60536,370 +60536,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="50" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="56.2388663967611"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="48" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="57.6315789473684"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="48" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="47" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="s">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="50" t="n">
+        <f aca="false">B2/3</f>
+        <v>0.000333333333333333</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="60" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="60" t="s">
+      <c r="E3" s="50" t="n">
+        <f aca="false">B3/3</f>
+        <v>0.000333333333333333</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="61" t="n">
-        <f aca="false">B2/3</f>
-        <v>1333.33333333333</v>
+      <c r="B4" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="50" t="n">
+        <f aca="false">B4/3</f>
+        <v>0.000333333333333333</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="50" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" s="51" t="n">
-        <f aca="false">B3/3</f>
-        <v>1333.33333333333</v>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="50" t="n">
+        <f aca="false">B5/3</f>
+        <v>0.000333333333333333</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B4" s="50" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="51" t="n">
-        <f aca="false">B4/3</f>
-        <v>1333.33333333333</v>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="50" t="n">
+        <f aca="false">B6/3</f>
+        <v>0.000333333333333333</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="E5" s="51" t="n">
-        <f aca="false">B5/3</f>
-        <v>1</v>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="50" t="n">
+        <f aca="false">B7/3</f>
+        <v>0.000333333333333333</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="E6" s="51" t="n">
-        <f aca="false">B6/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="E7" s="51" t="n">
-        <f aca="false">B7/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="50" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="C8" s="50" t="s">
+      <c r="B8" s="48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="E8" s="50" t="n">
+        <f aca="false">B8/3</f>
+        <v>0.000333333333333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="51" t="n">
-        <f aca="false">B8/3</f>
-        <v>0.000166666666666667</v>
+      <c r="B9" s="48" t="n">
+        <v>400</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="50" t="n">
+        <f aca="false">B9/3</f>
+        <v>133.333333333333</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="50" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="E9" s="51" t="n">
-        <f aca="false">B9/3</f>
-        <v>0.000166666666666667</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="B10" s="50" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="E10" s="51" t="n">
+      <c r="B10" s="48" t="n">
+        <v>400</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="50" t="n">
         <f aca="false">B10/3</f>
-        <v>0.000166666666666667</v>
+        <v>133.333333333333</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="B11" s="50" t="n">
-        <f aca="false">truthStateParams!$B$5</f>
-        <v>20</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="51" t="n">
-        <f aca="false">RADIANS(B11)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+      <c r="B11" s="48" t="n">
+        <v>400</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="50" t="n">
+        <f aca="false">B11/3</f>
+        <v>133.333333333333</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="B12" s="50" t="n">
-        <f aca="false">truthStateParams!$B$5</f>
-        <v>20</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="E12" s="51" t="n">
-        <f aca="false">RADIANS(B12)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+        <v>184</v>
+      </c>
+      <c r="B12" s="48" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="50" t="n">
+        <f aca="false">B12/3</f>
+        <v>33.3333333333333</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="B13" s="50" t="n">
-        <f aca="false">truthStateParams!$B$5</f>
-        <v>20</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="E13" s="51" t="n">
-        <f aca="false">RADIANS(B13)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+        <v>186</v>
+      </c>
+      <c r="B13" s="48" t="n">
+        <v>100</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" s="50" t="n">
+        <f aca="false">B13/3</f>
+        <v>33.3333333333333</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="B14" s="50" t="n">
-        <f aca="false">truthStateParams!$B$6</f>
-        <v>20</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D14" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="E14" s="51" t="n">
-        <f aca="false">RADIANS(B14)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+        <v>188</v>
+      </c>
+      <c r="B14" s="48" t="n">
+        <v>100</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="50" t="n">
+        <f aca="false">B14/3</f>
+        <v>33.3333333333333</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="B15" s="50" t="n">
-        <f aca="false">truthStateParams!$B$6</f>
-        <v>20</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="E15" s="51" t="n">
-        <f aca="false">RADIANS(B15)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+        <v>190</v>
+      </c>
+      <c r="B15" s="48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="50" t="n">
+        <f aca="false">B15/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="B16" s="50" t="n">
-        <f aca="false">truthStateParams!$B$6</f>
-        <v>20</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="50" t="s">
-        <v>186</v>
-      </c>
-      <c r="E16" s="51" t="n">
-        <f aca="false">RADIANS(B16)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="50" t="n">
+        <f aca="false">B16/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="B17" s="50" t="n">
-        <f aca="false">truthStateParams!$B$3</f>
-        <v>5</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="E17" s="51" t="n">
-        <f aca="false">RADIANS(B17)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" s="50" t="n">
-        <f aca="false">truthStateParams!$B$3</f>
-        <v>5</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="E18" s="51" t="n">
-        <f aca="false">RADIANS(B18)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="B19" s="56" t="n">
-        <f aca="false">truthStateParams!$B$3</f>
-        <v>5</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="E19" s="57" t="n">
-        <f aca="false">RADIANS(B19)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
+      <c r="B17" s="48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="50" t="n">
+        <f aca="false">B17/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -60918,329 +60873,395 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="64" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="50.9878542510121"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="48" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="52.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="48" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="48" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="F1" s="38"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="str">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="str">
         <f aca="false">truthStateParams!A2</f>
-        <v>Q_grav</v>
-      </c>
-      <c r="B2" s="49" t="n">
+        <v>sig_b1_ss</v>
+      </c>
+      <c r="B2" s="53" t="n">
         <f aca="false">truthStateParams!B2</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C2" s="12" t="str">
+        <f aca="false">truthStateParams!C2</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D2" s="12" t="str">
+        <f aca="false">truthStateParams!D2</f>
+        <v>3-sigma bias propagation noise of asset 1</v>
+      </c>
+      <c r="E2" s="13" t="n">
+        <f aca="false">B2/3</f>
+        <v>3.33333333333333E-008</v>
+      </c>
+      <c r="F2" s="54"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="str">
+        <f aca="false">truthStateParams!A3</f>
+        <v>sig_b2_ss</v>
+      </c>
+      <c r="B3" s="55" t="n">
+        <f aca="false">truthStateParams!B3</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C3" s="53" t="str">
+        <f aca="false">truthStateParams!C3</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D3" s="12" t="str">
+        <f aca="false">truthStateParams!D3</f>
+        <v>3-sigma bias propagation noise of asset 2</v>
+      </c>
+      <c r="E3" s="13" t="n">
+        <f aca="false">RADIANS(B3)/hr2sec/3</f>
+        <v>1.61604560369845E-013</v>
+      </c>
+      <c r="F3" s="54"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="str">
+        <f aca="false">truthStateParams!A4</f>
+        <v>sig_b3_ss</v>
+      </c>
+      <c r="B4" s="56" t="n">
+        <f aca="false">truthStateParams!B4</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C4" s="17" t="str">
+        <f aca="false">truthStateParams!C4</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D4" s="17" t="str">
+        <f aca="false">truthStateParams!D4</f>
+        <v>3-sigma bias propagation noise of asset 3</v>
+      </c>
+      <c r="E4" s="18" t="n">
+        <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
+        <v>9.69627362219072E-012</v>
+      </c>
+      <c r="F4" s="54"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="str">
+        <f aca="false">truthStateParams!A5</f>
+        <v>sig_b4_ss</v>
+      </c>
+      <c r="B5" s="55" t="n">
+        <f aca="false">truthStateParams!B5</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C5" s="12" t="str">
+        <f aca="false">truthStateParams!C5</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D5" s="12" t="str">
+        <f aca="false">truthStateParams!D5</f>
+        <v>3-sigma bias propagation noise of asset 4</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <f aca="false">RADIANS(B5)/3600/3</f>
+        <v>1.61604560369845E-013</v>
+      </c>
+      <c r="F5" s="54"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="str">
+        <f aca="false">truthStateParams!A6</f>
+        <v>sig_b5_ss</v>
+      </c>
+      <c r="B6" s="55" t="n">
+        <f aca="false">truthStateParams!B6</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C6" s="12" t="str">
+        <f aca="false">truthStateParams!C6</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D6" s="12" t="str">
+        <f aca="false">truthStateParams!D6</f>
+        <v>3-sigma bias propagation noise of asset 5</v>
+      </c>
+      <c r="E6" s="13" t="n">
+        <f aca="false">RADIANS(B6)/3600/3</f>
+        <v>1.61604560369845E-013</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="str">
+        <f aca="false">truthStateParams!A7</f>
+        <v>sig_b6_ss</v>
+      </c>
+      <c r="B7" s="55" t="n">
+        <f aca="false">truthStateParams!B7</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C7" s="12" t="str">
+        <f aca="false">truthStateParams!C7</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D7" s="12" t="str">
+        <f aca="false">truthStateParams!D7</f>
+        <v>3-sigma bias propagation noise of asset 6</v>
+      </c>
+      <c r="E7" s="13" t="n">
+        <f aca="false">RADIANS(B7)/3600/3</f>
+        <v>1.61604560369845E-013</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="str">
+        <f aca="false">truthStateParams!A8</f>
+        <v>sig_b7_ss</v>
+      </c>
+      <c r="B8" s="55" t="n">
+        <f aca="false">truthStateParams!B8</f>
+        <v>1E-007</v>
+      </c>
+      <c r="C8" s="12" t="str">
+        <f aca="false">truthStateParams!C8</f>
+        <v>sec/sec</v>
+      </c>
+      <c r="D8" s="12" t="str">
+        <f aca="false">truthStateParams!D8</f>
+        <v>3-sigma bias propagation noise of asset 7</v>
+      </c>
+      <c r="E8" s="13" t="n">
+        <f aca="false">RADIANS(B8)/3600/3</f>
+        <v>1.61604560369845E-013</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="str">
+        <f aca="false">truthStateParams!A9</f>
+        <v>Q_grav_x</v>
+      </c>
+      <c r="B9" s="55" t="n">
+        <f aca="false">truthStateParams!B9</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="50" t="str">
-        <f aca="false">truthStateParams!C2</f>
-        <v>m^2/s^3</v>
-      </c>
-      <c r="D2" s="50" t="str">
-        <f aca="false">truthStateParams!D2</f>
-        <v>3-sigma non-gravitational process noise</v>
-      </c>
-      <c r="E2" s="51" t="n">
-        <f aca="false">B2/3</f>
+      <c r="C9" s="12" t="str">
+        <f aca="false">truthStateParams!C9</f>
+        <v>m^2/sec^3</v>
+      </c>
+      <c r="D9" s="12" t="str">
+        <f aca="false">truthStateParams!D9</f>
+        <v>3-sigma of RSO x accelerations</v>
+      </c>
+      <c r="E9" s="13" t="n">
+        <f aca="false">RADIANS(B9)/3600/3</f>
+        <v>7.75701889775258E-013</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="str">
+        <f aca="false">truthStateParams!A10</f>
+        <v>Q_grav_y</v>
+      </c>
+      <c r="B10" s="57" t="n">
+        <f aca="false">truthStateParams!B10</f>
+        <v>4.8E-007</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f aca="false">truthStateParams!C10</f>
+        <v>m^2/sec^3</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f aca="false">truthStateParams!D10</f>
+        <v>3-sigma of RSO y accelerations</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <f aca="false">B10/3</f>
         <v>1.6E-007</v>
       </c>
-      <c r="F2" s="70"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="str">
-        <f aca="false">truthStateParams!A3</f>
-        <v>sig_gyro_ss</v>
-      </c>
-      <c r="B3" s="52" t="n">
-        <f aca="false">truthStateParams!B3</f>
-        <v>5</v>
-      </c>
-      <c r="C3" s="49" t="str">
-        <f aca="false">truthStateParams!C3</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D3" s="50" t="str">
-        <f aca="false">truthStateParams!D3</f>
-        <v>3-sigma steady-state gyro bias</v>
-      </c>
-      <c r="E3" s="51" t="n">
-        <f aca="false">RADIANS(B3)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
-      <c r="F3" s="70"/>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="str">
+        <f aca="false">truthStateParams!A11</f>
+        <v>Q_grav_z</v>
+      </c>
+      <c r="B11" s="58" t="n">
+        <f aca="false">truthStateParams!B11</f>
+        <v>4.8E-007</v>
+      </c>
+      <c r="C11" s="17" t="str">
+        <f aca="false">truthStateParams!C11</f>
+        <v>m^2/sec^3</v>
+      </c>
+      <c r="D11" s="17" t="str">
+        <f aca="false">truthStateParams!D11</f>
+        <v>3-sigma of RSO z accelerations</v>
+      </c>
+      <c r="E11" s="18" t="n">
+        <f aca="false">B11/3</f>
+        <v>1.6E-007</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54" t="str">
-        <f aca="false">truthStateParams!A4</f>
-        <v>arw</v>
-      </c>
-      <c r="B4" s="55" t="n">
-        <f aca="false">truthStateParams!B4</f>
-        <v>0.05</v>
-      </c>
-      <c r="C4" s="56" t="str">
-        <f aca="false">truthStateParams!C4</f>
-        <v>deg/sqrt(hr)</v>
-      </c>
-      <c r="D4" s="56" t="str">
-        <f aca="false">truthStateParams!D4</f>
-        <v>3-sigma angular random walk</v>
-      </c>
-      <c r="E4" s="57" t="n">
-        <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
-        <v>4.84813681109536E-006</v>
-      </c>
-      <c r="F4" s="70"/>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="str">
+        <f aca="false">truthStateParams!A9</f>
+        <v>Q_grav_x</v>
+      </c>
+      <c r="B12" s="58" t="n">
+        <f aca="false">truthStateParams!B9</f>
+        <v>4.8E-007</v>
+      </c>
+      <c r="C12" s="17" t="str">
+        <f aca="false">truthStateParams!C9</f>
+        <v>m^2/sec^3</v>
+      </c>
+      <c r="D12" s="17" t="str">
+        <f aca="false">truthStateParams!D9</f>
+        <v>3-sigma of RSO x accelerations</v>
+      </c>
+      <c r="E12" s="18" t="n">
+        <f aca="false">B12/3</f>
+        <v>1.6E-007</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="str">
-        <f aca="false">truthStateParams!A5</f>
-        <v>sig_st_ss</v>
-      </c>
-      <c r="B5" s="52" t="n">
-        <f aca="false">truthStateParams!B5</f>
-        <v>20</v>
-      </c>
-      <c r="C5" s="50" t="str">
-        <f aca="false">truthStateParams!C5</f>
-        <v>arcsec/axis</v>
-      </c>
-      <c r="D5" s="50" t="str">
-        <f aca="false">truthStateParams!D5</f>
-        <v>3-sigma steady-state star camera misalignment</v>
-      </c>
-      <c r="E5" s="51" t="n">
-        <f aca="false">RADIANS(B5)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
-      <c r="F5" s="70"/>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="str">
+        <f aca="false">truthStateParams!A10</f>
+        <v>Q_grav_y</v>
+      </c>
+      <c r="B13" s="58" t="n">
+        <f aca="false">truthStateParams!B10</f>
+        <v>4.8E-007</v>
+      </c>
+      <c r="C13" s="17" t="str">
+        <f aca="false">truthStateParams!C10</f>
+        <v>m^2/sec^3</v>
+      </c>
+      <c r="D13" s="17" t="str">
+        <f aca="false">truthStateParams!D10</f>
+        <v>3-sigma of RSO y accelerations</v>
+      </c>
+      <c r="E13" s="18" t="n">
+        <f aca="false">B13/3</f>
+        <v>1.6E-007</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="str">
-        <f aca="false">truthStateParams!A6</f>
-        <v>sig_c_ss</v>
-      </c>
-      <c r="B6" s="52" t="n">
-        <f aca="false">truthStateParams!B6</f>
-        <v>20</v>
-      </c>
-      <c r="C6" s="50" t="str">
-        <f aca="false">truthStateParams!C6</f>
-        <v>arcsec/axis</v>
-      </c>
-      <c r="D6" s="50" t="str">
-        <f aca="false">truthStateParams!D6</f>
-        <v>3-sigma steady-state terrain camera misalignment</v>
-      </c>
-      <c r="E6" s="51" t="n">
-        <f aca="false">RADIANS(B6)/3600/3</f>
-        <v>3.23209120739691E-005</v>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="str">
+        <f aca="false">truthStateParams!A11</f>
+        <v>Q_grav_z</v>
+      </c>
+      <c r="B14" s="58" t="n">
+        <f aca="false">truthStateParams!B11</f>
+        <v>4.8E-007</v>
+      </c>
+      <c r="C14" s="17" t="str">
+        <f aca="false">truthStateParams!C11</f>
+        <v>m^2/sec^3</v>
+      </c>
+      <c r="D14" s="17" t="str">
+        <f aca="false">truthStateParams!D11</f>
+        <v>3-sigma of RSO z accelerations</v>
+      </c>
+      <c r="E14" s="18" t="n">
+        <f aca="false">B14/3</f>
+        <v>1.6E-007</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="str">
-        <f aca="false">truthStateParams!A7</f>
-        <v>sig_meas_stx</v>
-      </c>
-      <c r="B7" s="52" t="n">
-        <f aca="false">truthStateParams!B7</f>
-        <v>1.5</v>
-      </c>
-      <c r="C7" s="50" t="str">
-        <f aca="false">truthStateParams!C7</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D7" s="50" t="str">
-        <f aca="false">truthStateParams!D7</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E7" s="51" t="n">
-        <f aca="false">RADIANS(B7)/3600/3</f>
-        <v>2.42406840554768E-006</v>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="str">
+        <f aca="false">truthStateParams!A12</f>
+        <v>sig_ax_ss</v>
+      </c>
+      <c r="B15" s="58" t="n">
+        <f aca="false">truthStateParams!B12</f>
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="17" t="str">
+        <f aca="false">truthStateParams!C12</f>
+        <v>m/s^2</v>
+      </c>
+      <c r="D15" s="17" t="str">
+        <f aca="false">truthStateParams!D12</f>
+        <v>3-sigma of RSO x atmo acceleration</v>
+      </c>
+      <c r="E15" s="18" t="n">
+        <f aca="false">B15/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="str">
-        <f aca="false">truthStateParams!A8</f>
-        <v>sig_meas_sty</v>
-      </c>
-      <c r="B8" s="52" t="n">
-        <f aca="false">truthStateParams!B8</f>
-        <v>1.5</v>
-      </c>
-      <c r="C8" s="50" t="str">
-        <f aca="false">truthStateParams!C8</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D8" s="50" t="str">
-        <f aca="false">truthStateParams!D8</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E8" s="51" t="n">
-        <f aca="false">RADIANS(B8)/3600/3</f>
-        <v>2.42406840554768E-006</v>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="str">
+        <f aca="false">truthStateParams!A13</f>
+        <v>sig_ay_ss</v>
+      </c>
+      <c r="B16" s="58" t="n">
+        <f aca="false">truthStateParams!B13</f>
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="17" t="str">
+        <f aca="false">truthStateParams!C13</f>
+        <v>m/s^2</v>
+      </c>
+      <c r="D16" s="17" t="str">
+        <f aca="false">truthStateParams!D13</f>
+        <v>4-sigma of RSO y atmo acceleration</v>
+      </c>
+      <c r="E16" s="18" t="n">
+        <f aca="false">B16/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="str">
-        <f aca="false">truthStateParams!A9</f>
-        <v>sig_meas_stz</v>
-      </c>
-      <c r="B9" s="52" t="n">
-        <f aca="false">truthStateParams!B9</f>
-        <v>9</v>
-      </c>
-      <c r="C9" s="50" t="str">
-        <f aca="false">truthStateParams!C9</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D9" s="50" t="str">
-        <f aca="false">truthStateParams!D9</f>
-        <v>3-sigma star camera measurement uncertainty</v>
-      </c>
-      <c r="E9" s="51" t="n">
-        <f aca="false">RADIANS(B9)/3600/3</f>
-        <v>1.45444104332861E-005</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="58" t="str">
-        <f aca="false">truthStateParams!A10</f>
-        <v>sig_cu</v>
-      </c>
-      <c r="B10" s="59" t="n">
-        <f aca="false">truthStateParams!B10</f>
-        <v>3</v>
-      </c>
-      <c r="C10" s="60" t="str">
-        <f aca="false">truthStateParams!C10</f>
-        <v>pixels</v>
-      </c>
-      <c r="D10" s="60" t="str">
-        <f aca="false">truthStateParams!D10</f>
-        <v>3-sigma u component of pixel noise</v>
-      </c>
-      <c r="E10" s="61" t="n">
-        <f aca="false">B10/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="54" t="str">
-        <f aca="false">truthStateParams!A11</f>
-        <v>sig_cv</v>
-      </c>
-      <c r="B11" s="62" t="n">
-        <f aca="false">truthStateParams!B11</f>
-        <v>3</v>
-      </c>
-      <c r="C11" s="56" t="str">
-        <f aca="false">truthStateParams!C11</f>
-        <v>pixels</v>
-      </c>
-      <c r="D11" s="56" t="str">
-        <f aca="false">truthStateParams!D11</f>
-        <v>3-sigma v component of pixel noise</v>
-      </c>
-      <c r="E11" s="57" t="n">
-        <f aca="false">B11/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="54" t="str">
-        <f aca="false">truthStateParams!A12</f>
-        <v>sig_idpos</v>
-      </c>
-      <c r="B12" s="62" t="n">
-        <f aca="false">truthStateParams!B12</f>
-        <v>10</v>
-      </c>
-      <c r="C12" s="56" t="str">
-        <f aca="false">truthStateParams!C12</f>
-        <v>m</v>
-      </c>
-      <c r="D12" s="56" t="str">
-        <f aca="false">truthStateParams!D12</f>
-        <v>3-sigma change in inertial position measurement uncertainty</v>
-      </c>
-      <c r="E12" s="57" t="n">
-        <f aca="false">B12/3</f>
-        <v>3.33333333333333</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="54" t="str">
-        <f aca="false">truthStateParams!A13</f>
-        <v>sig_loss</v>
-      </c>
-      <c r="B13" s="62" t="n">
-        <f aca="false">truthStateParams!B13</f>
-        <v>100</v>
-      </c>
-      <c r="C13" s="56" t="str">
-        <f aca="false">truthStateParams!C13</f>
-        <v>m</v>
-      </c>
-      <c r="D13" s="56" t="str">
-        <f aca="false">truthStateParams!D13</f>
-        <v>3-sigma LOSS feature location uncertainty</v>
-      </c>
-      <c r="E13" s="57" t="n">
-        <f aca="false">B13/3</f>
-        <v>33.3333333333333</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="54" t="str">
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="str">
         <f aca="false">truthStateParams!A14</f>
-        <v>sig_mdpos</v>
-      </c>
-      <c r="B14" s="62" t="n">
+        <v>sig_az_ss</v>
+      </c>
+      <c r="B17" s="58" t="n">
         <f aca="false">truthStateParams!B14</f>
-        <v>10</v>
-      </c>
-      <c r="C14" s="56" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="17" t="str">
         <f aca="false">truthStateParams!C14</f>
-        <v>m</v>
-      </c>
-      <c r="D14" s="56" t="str">
+        <v>m/s^2</v>
+      </c>
+      <c r="D17" s="17" t="str">
         <f aca="false">truthStateParams!D14</f>
-        <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
-      </c>
-      <c r="E14" s="57" t="n">
-        <f aca="false">B14/3</f>
-        <v>3.33333333333333</v>
+        <v>5-sigma of RSO z atmo acceleration</v>
+      </c>
+      <c r="E17" s="18" t="n">
+        <f aca="false">B17/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -61261,437 +61282,407 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="50" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="56.2388663967611"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="64" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="50" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="6.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="57.6315789473684"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="60" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="59" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="64" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="str">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A2</f>
-        <v>sig_rsx</v>
-      </c>
-      <c r="B2" s="50" t="n">
+        <v>sig_b1</v>
+      </c>
+      <c r="B2" s="59" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
-        <v>4000</v>
-      </c>
-      <c r="C2" s="50" t="str">
+        <v>0.001</v>
+      </c>
+      <c r="C2" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
-        <v>m</v>
-      </c>
-      <c r="D2" s="50" t="str">
+        <v>sec</v>
+      </c>
+      <c r="D2" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!D2</f>
-        <v>3-sigma initial satellite position uncertainty</v>
-      </c>
-      <c r="E2" s="72" t="n">
+        <v>3-sigma clocking bias of asset 1</v>
+      </c>
+      <c r="E2" s="66" t="n">
         <f aca="false">B2/3</f>
-        <v>1333.33333333333</v>
-      </c>
-      <c r="F2" s="70"/>
+        <v>0.000333333333333333</v>
+      </c>
+      <c r="F2" s="67"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="str">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A3</f>
-        <v>sig_rsy</v>
-      </c>
-      <c r="B3" s="50" t="n">
+        <v>sig_b2</v>
+      </c>
+      <c r="B3" s="59" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
-        <v>4000</v>
-      </c>
-      <c r="C3" s="50" t="str">
+        <v>0.001</v>
+      </c>
+      <c r="C3" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
-        <v>m</v>
-      </c>
-      <c r="D3" s="50" t="str">
+        <v>sec</v>
+      </c>
+      <c r="D3" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!D3</f>
-        <v>3-sigma initial satellite position uncertainty</v>
-      </c>
-      <c r="E3" s="72" t="n">
+        <v>3-sigma clocking bias of asset 2</v>
+      </c>
+      <c r="E3" s="66" t="n">
         <f aca="false">B3/3</f>
-        <v>1333.33333333333</v>
-      </c>
-      <c r="F3" s="70"/>
+        <v>0.000333333333333333</v>
+      </c>
+      <c r="F3" s="67"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="str">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A4</f>
-        <v>sig_rsz</v>
-      </c>
-      <c r="B4" s="50" t="n">
+        <v>sig_b3</v>
+      </c>
+      <c r="B4" s="59" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
-        <v>4000</v>
-      </c>
-      <c r="C4" s="50" t="str">
+        <v>0.001</v>
+      </c>
+      <c r="C4" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
-        <v>m</v>
-      </c>
-      <c r="D4" s="50" t="str">
+        <v>sec</v>
+      </c>
+      <c r="D4" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!D4</f>
-        <v>3-sigma initial satellite position uncertainty</v>
-      </c>
-      <c r="E4" s="72" t="n">
+        <v>3-sigma clocking bias of asset 3</v>
+      </c>
+      <c r="E4" s="66" t="n">
         <f aca="false">B4/3</f>
-        <v>1333.33333333333</v>
-      </c>
-      <c r="F4" s="70"/>
+        <v>0.000333333333333333</v>
+      </c>
+      <c r="F4" s="67"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="str">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A5</f>
-        <v>sig_vsx</v>
-      </c>
-      <c r="B5" s="50" t="n">
+        <v>sig_b4</v>
+      </c>
+      <c r="B5" s="59" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="50" t="str">
+        <v>0.001</v>
+      </c>
+      <c r="C5" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
-        <v>m/sec</v>
-      </c>
-      <c r="D5" s="50" t="str">
+        <v>sec</v>
+      </c>
+      <c r="D5" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!D5</f>
-        <v>3-sigma initial satellite velocity uncertainty</v>
-      </c>
-      <c r="E5" s="72" t="n">
+        <v>3-sigma clocking bias of asset 4</v>
+      </c>
+      <c r="E5" s="66" t="n">
         <f aca="false">B5/3</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="70"/>
+        <v>0.000333333333333333</v>
+      </c>
+      <c r="F5" s="67"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="str">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A6</f>
-        <v>sig_vsy</v>
-      </c>
-      <c r="B6" s="50" t="n">
+        <v>sig_b5</v>
+      </c>
+      <c r="B6" s="59" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
-        <v>3</v>
-      </c>
-      <c r="C6" s="50" t="str">
+        <v>0.001</v>
+      </c>
+      <c r="C6" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
-        <v>m/sec</v>
-      </c>
-      <c r="D6" s="50" t="str">
+        <v>sec</v>
+      </c>
+      <c r="D6" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!D6</f>
-        <v>3-sigma initial satellite velocity uncertainty</v>
-      </c>
-      <c r="E6" s="72" t="n">
+        <v>3-sigma clocking bias of asset 5</v>
+      </c>
+      <c r="E6" s="66" t="n">
         <f aca="false">B6/3</f>
-        <v>1</v>
+        <v>0.000333333333333333</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="str">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A7</f>
-        <v>sig_vsz</v>
-      </c>
-      <c r="B7" s="50" t="n">
+        <v>sig_b6</v>
+      </c>
+      <c r="B7" s="59" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
-        <v>3</v>
-      </c>
-      <c r="C7" s="50" t="str">
+        <v>0.001</v>
+      </c>
+      <c r="C7" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
-        <v>m/sec</v>
-      </c>
-      <c r="D7" s="50" t="str">
+        <v>sec</v>
+      </c>
+      <c r="D7" s="59" t="str">
         <f aca="false">truthStateInitialUncertainty!D7</f>
-        <v>3-sigma initial satellite velocity uncertainty</v>
-      </c>
-      <c r="E7" s="72" t="n">
+        <v>3-sigma clocking bias of asset 6</v>
+      </c>
+      <c r="E7" s="66" t="n">
         <f aca="false">B7/3</f>
-        <v>1</v>
+        <v>0.000333333333333333</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="str">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="65" t="str">
         <f aca="false">truthStateInitialUncertainty!A8</f>
+        <v>sig_b7</v>
+      </c>
+      <c r="B8" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B8</f>
+        <v>0.001</v>
+      </c>
+      <c r="C8" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C8</f>
+        <v>sec</v>
+      </c>
+      <c r="D8" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D8</f>
+        <v>3-sigma clocking bias of asset 7</v>
+      </c>
+      <c r="E8" s="66" t="n">
+        <f aca="false">B8/3</f>
+        <v>0.000333333333333333</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A9</f>
+        <v>sig_px</v>
+      </c>
+      <c r="B9" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B9</f>
+        <v>400</v>
+      </c>
+      <c r="C9" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C9</f>
+        <v>km</v>
+      </c>
+      <c r="D9" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D9</f>
+        <v>3-sigma of RSO x position</v>
+      </c>
+      <c r="E9" s="66" t="n">
+        <f aca="false">B9/3</f>
+        <v>133.333333333333</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A10</f>
+        <v>sig_py</v>
+      </c>
+      <c r="B10" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B10</f>
+        <v>400</v>
+      </c>
+      <c r="C10" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C10</f>
+        <v>km</v>
+      </c>
+      <c r="D10" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D10</f>
+        <v>3-sigma of RSO y position</v>
+      </c>
+      <c r="E10" s="66" t="n">
+        <f aca="false">B10/3</f>
+        <v>133.333333333333</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A11</f>
+        <v>sig_pz</v>
+      </c>
+      <c r="B11" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B11</f>
+        <v>400</v>
+      </c>
+      <c r="C11" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C11</f>
+        <v>km</v>
+      </c>
+      <c r="D11" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D11</f>
+        <v>3-sigma of RSO z position</v>
+      </c>
+      <c r="E11" s="66" t="n">
+        <f aca="false">B11/3</f>
+        <v>133.333333333333</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A12</f>
+        <v>sig_vx</v>
+      </c>
+      <c r="B12" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B12</f>
+        <v>100</v>
+      </c>
+      <c r="C12" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C12</f>
+        <v>km/s</v>
+      </c>
+      <c r="D12" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D12</f>
+        <v>3-sigma of RSO x velocity</v>
+      </c>
+      <c r="E12" s="66" t="n">
+        <f aca="false">B12/3</f>
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A13</f>
+        <v>sig_vy</v>
+      </c>
+      <c r="B13" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B13</f>
+        <v>100</v>
+      </c>
+      <c r="C13" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C13</f>
+        <v>km/s</v>
+      </c>
+      <c r="D13" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D13</f>
+        <v>3-sigma of RSO y velocity</v>
+      </c>
+      <c r="E13" s="66" t="n">
+        <f aca="false">B13/3</f>
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A14</f>
+        <v>sig_vz</v>
+      </c>
+      <c r="B14" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B14</f>
+        <v>100</v>
+      </c>
+      <c r="C14" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C14</f>
+        <v>km/s</v>
+      </c>
+      <c r="D14" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D14</f>
+        <v>3-sigma of RSO z velocity</v>
+      </c>
+      <c r="E14" s="66" t="n">
+        <f aca="false">B14/3</f>
+        <v>33.3333333333333</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A15</f>
         <v>sig_ax</v>
       </c>
-      <c r="B8" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B8</f>
-        <v>0.0005</v>
-      </c>
-      <c r="C8" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C8</f>
-        <v>rad</v>
-      </c>
-      <c r="D8" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D8</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
-      </c>
-      <c r="E8" s="72" t="n">
-        <f aca="false">B8/3</f>
-        <v>0.000166666666666667</v>
+      <c r="B15" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B15</f>
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C15</f>
+        <v>m/s^2</v>
+      </c>
+      <c r="D15" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D15</f>
+        <v>3-sigma of RSO x atmo acceleration</v>
+      </c>
+      <c r="E15" s="66" t="n">
+        <f aca="false">B15/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A9</f>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A16</f>
         <v>sig_ay</v>
       </c>
-      <c r="B9" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B9</f>
-        <v>0.0005</v>
-      </c>
-      <c r="C9" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C9</f>
-        <v>rad</v>
-      </c>
-      <c r="D9" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D9</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
-      </c>
-      <c r="E9" s="72" t="n">
-        <f aca="false">B9/3</f>
-        <v>0.000166666666666667</v>
+      <c r="B16" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B16</f>
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C16</f>
+        <v>m/s^2</v>
+      </c>
+      <c r="D16" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D16</f>
+        <v>4-sigma of RSO y atmo acceleration</v>
+      </c>
+      <c r="E16" s="66" t="n">
+        <f aca="false">B16/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A10</f>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65" t="str">
+        <f aca="false">truthStateInitialUncertainty!A17</f>
         <v>sig_az</v>
       </c>
-      <c r="B10" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B10</f>
-        <v>0.0005</v>
-      </c>
-      <c r="C10" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C10</f>
-        <v>rad</v>
-      </c>
-      <c r="D10" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D10</f>
-        <v>3-sigma initial satellite orientation uncertainty</v>
-      </c>
-      <c r="E10" s="72" t="n">
-        <f aca="false">B10/3</f>
-        <v>0.000166666666666667</v>
+      <c r="B17" s="59" t="n">
+        <f aca="false">truthStateInitialUncertainty!B17</f>
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!C17</f>
+        <v>m/s^2</v>
+      </c>
+      <c r="D17" s="59" t="str">
+        <f aca="false">truthStateInitialUncertainty!D17</f>
+        <v>5-sigma of RSO z atmo acceleration</v>
+      </c>
+      <c r="E17" s="66" t="n">
+        <f aca="false">B17/3</f>
+        <v>0.166666666666667</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A11</f>
-        <v>sig_thstx</v>
-      </c>
-      <c r="B11" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B11</f>
-        <v>20</v>
-      </c>
-      <c r="C11" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C11</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D11" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D11</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E11" s="72" t="n">
-        <f aca="false">RADIANS(B11)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="66"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A12</f>
-        <v>sig_thsty</v>
-      </c>
-      <c r="B12" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B12</f>
-        <v>20</v>
-      </c>
-      <c r="C12" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C12</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D12" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D12</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E12" s="72" t="n">
-        <f aca="false">RADIANS(B12)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A13</f>
-        <v>sig_thstz</v>
-      </c>
-      <c r="B13" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B13</f>
-        <v>20</v>
-      </c>
-      <c r="C13" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C13</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D13" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D13</f>
-        <v>3-sigma initial star camera misalignment uncertainty</v>
-      </c>
-      <c r="E13" s="72" t="n">
-        <f aca="false">RADIANS(B13)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A14</f>
-        <v>sig_thcx</v>
-      </c>
-      <c r="B14" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B14</f>
-        <v>20</v>
-      </c>
-      <c r="C14" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C14</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D14" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D14</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E14" s="72" t="n">
-        <f aca="false">RADIANS(B14)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A15</f>
-        <v>sig_thcy</v>
-      </c>
-      <c r="B15" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B15</f>
-        <v>20</v>
-      </c>
-      <c r="C15" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C15</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D15" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D15</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E15" s="72" t="n">
-        <f aca="false">RADIANS(B15)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A16</f>
-        <v>sig_thcz</v>
-      </c>
-      <c r="B16" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B16</f>
-        <v>20</v>
-      </c>
-      <c r="C16" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C16</f>
-        <v>arcsec</v>
-      </c>
-      <c r="D16" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D16</f>
-        <v>3-sigma initial terrain camera misalignment uncertainty</v>
-      </c>
-      <c r="E16" s="72" t="n">
-        <f aca="false">RADIANS(B16)/3600/3</f>
-        <v>3.23209120739691E-005</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A17</f>
-        <v>sig_gyrox</v>
-      </c>
-      <c r="B17" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B17</f>
-        <v>5</v>
-      </c>
-      <c r="C17" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C17</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D17" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D17</f>
-        <v>3-sigma initial gyro bias uncertainty</v>
-      </c>
-      <c r="E17" s="72" t="n">
-        <f aca="false">RADIANS(B17)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="48" t="str">
-        <f aca="false">truthStateInitialUncertainty!A18</f>
-        <v>sig_gyroy</v>
-      </c>
-      <c r="B18" s="50" t="n">
-        <f aca="false">truthStateInitialUncertainty!B18</f>
-        <v>5</v>
-      </c>
-      <c r="C18" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!C18</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D18" s="50" t="str">
-        <f aca="false">truthStateInitialUncertainty!D18</f>
-        <v>3-sigma initial gyro bias uncertainty</v>
-      </c>
-      <c r="E18" s="72" t="n">
-        <f aca="false">RADIANS(B18)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="54" t="str">
-        <f aca="false">truthStateInitialUncertainty!A19</f>
-        <v>sig_gyroz</v>
-      </c>
-      <c r="B19" s="56" t="n">
-        <f aca="false">truthStateInitialUncertainty!B19</f>
-        <v>5</v>
-      </c>
-      <c r="C19" s="56" t="str">
-        <f aca="false">truthStateInitialUncertainty!C19</f>
-        <v>deg/hr</v>
-      </c>
-      <c r="D19" s="56" t="str">
-        <f aca="false">truthStateInitialUncertainty!D19</f>
-        <v>3-sigma initial gyro bias uncertainty</v>
-      </c>
-      <c r="E19" s="73" t="n">
-        <f aca="false">RADIANS(B19)/hr2sec/3</f>
-        <v>8.08022801849227E-006</v>
-      </c>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="68"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="66"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -61711,7 +61702,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -61720,292 +61711,292 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.2388663967611"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.6315789473684"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="70" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="74" t="n">
+      <c r="B2" s="72" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="75" t="n">
+      <c r="D2" s="71"/>
+      <c r="E2" s="73" t="n">
         <f aca="false">B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="76" t="n">
+      <c r="B3" s="74" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="77" t="n">
+      <c r="D3" s="59"/>
+      <c r="E3" s="75" t="n">
         <f aca="false">B3</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="76" t="n">
+      <c r="B4" s="74" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="77" t="n">
+      <c r="D4" s="59"/>
+      <c r="E4" s="75" t="n">
         <f aca="false">B4</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="76" t="n">
+      <c r="B5" s="74" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="77" t="n">
+      <c r="D5" s="59"/>
+      <c r="E5" s="75" t="n">
         <f aca="false">B5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="76" t="n">
+      <c r="B6" s="74" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="77" t="n">
+      <c r="D6" s="59"/>
+      <c r="E6" s="75" t="n">
         <f aca="false">B6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="76" t="n">
+      <c r="B7" s="74" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="77" t="n">
+      <c r="D7" s="59"/>
+      <c r="E7" s="75" t="n">
         <f aca="false">B7</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="76" t="n">
+      <c r="B8" s="74" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="77" t="n">
+      <c r="D8" s="59"/>
+      <c r="E8" s="75" t="n">
         <f aca="false">B8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="50" t="n">
+      <c r="B9" s="59" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="72" t="n">
+      <c r="D9" s="59"/>
+      <c r="E9" s="66" t="n">
         <f aca="false">B9*1000</f>
         <v>1000</v>
       </c>
-      <c r="F9" s="50"/>
+      <c r="F9" s="59"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="50" t="n">
+      <c r="B10" s="59" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="72" t="n">
+      <c r="D10" s="59"/>
+      <c r="E10" s="66" t="n">
         <f aca="false">B10*1000</f>
         <v>2000</v>
       </c>
-      <c r="F10" s="50"/>
+      <c r="F10" s="59"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="50" t="n">
+      <c r="B11" s="59" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="72" t="n">
+      <c r="D11" s="59"/>
+      <c r="E11" s="66" t="n">
         <f aca="false">B11*1000</f>
         <v>3000</v>
       </c>
-      <c r="F11" s="50"/>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="50" t="n">
+      <c r="B12" s="59" t="n">
         <v>0.1</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="72" t="n">
+      <c r="D12" s="59"/>
+      <c r="E12" s="66" t="n">
         <f aca="false">B12*1000</f>
         <v>100</v>
       </c>
-      <c r="F12" s="50"/>
+      <c r="F12" s="59"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="50" t="n">
+      <c r="B13" s="59" t="n">
         <v>0.2</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="72" t="n">
+      <c r="D13" s="59"/>
+      <c r="E13" s="66" t="n">
         <f aca="false">B13*1000</f>
         <v>200</v>
       </c>
-      <c r="F13" s="50"/>
+      <c r="F13" s="59"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="50" t="n">
+      <c r="B14" s="59" t="n">
         <v>0.3</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="72" t="n">
+      <c r="D14" s="59"/>
+      <c r="E14" s="66" t="n">
         <f aca="false">B14*1000</f>
         <v>300</v>
       </c>
-      <c r="F14" s="50"/>
+      <c r="F14" s="59"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="50" t="n">
+      <c r="B15" s="59" t="n">
         <v>0.01</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="72" t="n">
+      <c r="D15" s="59"/>
+      <c r="E15" s="66" t="n">
         <f aca="false">B15</f>
         <v>0.01</v>
       </c>
-      <c r="F15" s="50"/>
+      <c r="F15" s="59"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="50" t="n">
+      <c r="B16" s="59" t="n">
         <v>0.02</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="72" t="n">
+      <c r="D16" s="59"/>
+      <c r="E16" s="66" t="n">
         <f aca="false">B16</f>
         <v>0.02</v>
       </c>
-      <c r="F16" s="50"/>
+      <c r="F16" s="59"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="56" t="n">
+      <c r="B17" s="69" t="n">
         <v>0.03</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="56"/>
-      <c r="E17" s="73" t="n">
+      <c r="D17" s="69"/>
+      <c r="E17" s="76" t="n">
         <f aca="false">B17</f>
         <v>0.03</v>
       </c>
-      <c r="F17" s="50"/>
+      <c r="F17" s="59"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
began writing final part of code. Residual Covariance is singular.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -679,6 +679,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -701,11 +702,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1144,12 +1147,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.93522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1356,7 +1359,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="20" t="n">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>13</v>
@@ -1366,7 +1369,7 @@
       </c>
       <c r="E12" s="22" t="n">
         <f aca="false">B12</f>
-        <v>200</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1396,7 +1399,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1515,11 +1518,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.2712550607288"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -52554,7 +52557,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60113,7 +60116,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60236,17 +60239,16 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.86234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.34817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6194331983806"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.9635627530364"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60272,7 +60274,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>139</v>
@@ -60282,7 +60284,7 @@
       </c>
       <c r="E2" s="50" t="n">
         <f aca="false">B2/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60290,7 +60292,7 @@
         <v>141</v>
       </c>
       <c r="B3" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>139</v>
@@ -60300,7 +60302,7 @@
       </c>
       <c r="E3" s="50" t="n">
         <f aca="false">B3/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F3" s="51"/>
     </row>
@@ -60309,7 +60311,7 @@
         <v>143</v>
       </c>
       <c r="B4" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>139</v>
@@ -60319,7 +60321,7 @@
       </c>
       <c r="E4" s="50" t="n">
         <f aca="false">B4/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60327,7 +60329,7 @@
         <v>145</v>
       </c>
       <c r="B5" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>139</v>
@@ -60337,7 +60339,7 @@
       </c>
       <c r="E5" s="50" t="n">
         <f aca="false">B5/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60345,7 +60347,7 @@
         <v>147</v>
       </c>
       <c r="B6" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>139</v>
@@ -60355,7 +60357,7 @@
       </c>
       <c r="E6" s="50" t="n">
         <f aca="false">B6/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60363,7 +60365,7 @@
         <v>149</v>
       </c>
       <c r="B7" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>139</v>
@@ -60373,7 +60375,7 @@
       </c>
       <c r="E7" s="50" t="n">
         <f aca="false">B7/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60381,7 +60383,7 @@
         <v>151</v>
       </c>
       <c r="B8" s="49" t="n">
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>139</v>
@@ -60391,7 +60393,7 @@
       </c>
       <c r="E8" s="50" t="n">
         <f aca="false">B8/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60524,7 +60526,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D70" activeCellId="0" sqref="D70"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -60532,9 +60534,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="21" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="21" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="29.2145748987854"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="29.4574898785425"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -60561,7 +60563,7 @@
       </c>
       <c r="B2" s="49" t="n">
         <f aca="false">truthStateParams!B2</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>6</v>
@@ -60571,7 +60573,7 @@
       </c>
       <c r="E2" s="50" t="n">
         <f aca="false">B2/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60580,7 +60582,7 @@
       </c>
       <c r="B3" s="49" t="n">
         <f aca="false">truthStateParams!B3</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>6</v>
@@ -60590,7 +60592,7 @@
       </c>
       <c r="E3" s="50" t="n">
         <f aca="false">B3/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60599,7 +60601,7 @@
       </c>
       <c r="B4" s="49" t="n">
         <f aca="false">truthStateParams!B4</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>6</v>
@@ -60609,7 +60611,7 @@
       </c>
       <c r="E4" s="50" t="n">
         <f aca="false">B4/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60618,7 +60620,7 @@
       </c>
       <c r="B5" s="49" t="n">
         <f aca="false">truthStateParams!B5</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>6</v>
@@ -60628,7 +60630,7 @@
       </c>
       <c r="E5" s="50" t="n">
         <f aca="false">B5/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60637,7 +60639,7 @@
       </c>
       <c r="B6" s="49" t="n">
         <f aca="false">truthStateParams!B6</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>6</v>
@@ -60647,7 +60649,7 @@
       </c>
       <c r="E6" s="50" t="n">
         <f aca="false">B6/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60656,7 +60658,7 @@
       </c>
       <c r="B7" s="49" t="n">
         <f aca="false">truthStateParams!B7</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>6</v>
@@ -60666,7 +60668,7 @@
       </c>
       <c r="E7" s="50" t="n">
         <f aca="false">B7/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -60675,7 +60677,7 @@
       </c>
       <c r="B8" s="49" t="n">
         <f aca="false">truthStateParams!B8</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>6</v>
@@ -60685,7 +60687,7 @@
       </c>
       <c r="E8" s="50" t="n">
         <f aca="false">B8/3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60877,12 +60879,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="8.86234817813765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="8.34817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="10.6194331983806"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="33.9635627530364"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -60911,7 +60913,7 @@
       </c>
       <c r="B2" s="53" t="n">
         <f aca="false">truthStateParams!B2</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C2" s="12" t="str">
         <f aca="false">truthStateParams!C2</f>
@@ -60923,7 +60925,7 @@
       </c>
       <c r="E2" s="54" t="n">
         <f aca="false">truthStateParams!E2</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F2" s="55"/>
     </row>
@@ -60934,7 +60936,7 @@
       </c>
       <c r="B3" s="53" t="n">
         <f aca="false">truthStateParams!B3</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C3" s="12" t="str">
         <f aca="false">truthStateParams!C3</f>
@@ -60946,7 +60948,7 @@
       </c>
       <c r="E3" s="54" t="n">
         <f aca="false">truthStateParams!E3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F3" s="55"/>
     </row>
@@ -60957,7 +60959,7 @@
       </c>
       <c r="B4" s="53" t="n">
         <f aca="false">truthStateParams!B4</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C4" s="12" t="str">
         <f aca="false">truthStateParams!C4</f>
@@ -60969,7 +60971,7 @@
       </c>
       <c r="E4" s="54" t="n">
         <f aca="false">truthStateParams!E4</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F4" s="55"/>
     </row>
@@ -60980,7 +60982,7 @@
       </c>
       <c r="B5" s="53" t="n">
         <f aca="false">truthStateParams!B5</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C5" s="12" t="str">
         <f aca="false">truthStateParams!C5</f>
@@ -60992,7 +60994,7 @@
       </c>
       <c r="E5" s="54" t="n">
         <f aca="false">truthStateParams!E5</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F5" s="55"/>
     </row>
@@ -61003,7 +61005,7 @@
       </c>
       <c r="B6" s="53" t="n">
         <f aca="false">truthStateParams!B6</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C6" s="12" t="str">
         <f aca="false">truthStateParams!C6</f>
@@ -61015,7 +61017,7 @@
       </c>
       <c r="E6" s="54" t="n">
         <f aca="false">truthStateParams!E6</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61025,7 +61027,7 @@
       </c>
       <c r="B7" s="53" t="n">
         <f aca="false">truthStateParams!B7</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C7" s="12" t="str">
         <f aca="false">truthStateParams!C7</f>
@@ -61037,7 +61039,7 @@
       </c>
       <c r="E7" s="54" t="n">
         <f aca="false">truthStateParams!E7</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61047,7 +61049,7 @@
       </c>
       <c r="B8" s="53" t="n">
         <f aca="false">truthStateParams!B8</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C8" s="12" t="str">
         <f aca="false">truthStateParams!C8</f>
@@ -61059,7 +61061,7 @@
       </c>
       <c r="E8" s="54" t="n">
         <f aca="false">truthStateParams!E8</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61242,9 +61244,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="21" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="21" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="29.2145748987854"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="29.4574898785425"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -61273,7 +61275,7 @@
       </c>
       <c r="B2" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C2" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
@@ -61285,7 +61287,7 @@
       </c>
       <c r="E2" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E2</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F2" s="55"/>
     </row>
@@ -61296,7 +61298,7 @@
       </c>
       <c r="B3" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C3" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
@@ -61308,7 +61310,7 @@
       </c>
       <c r="E3" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E3</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F3" s="55"/>
     </row>
@@ -61319,7 +61321,7 @@
       </c>
       <c r="B4" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C4" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
@@ -61331,7 +61333,7 @@
       </c>
       <c r="E4" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E4</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F4" s="55"/>
     </row>
@@ -61342,7 +61344,7 @@
       </c>
       <c r="B5" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C5" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
@@ -61354,7 +61356,7 @@
       </c>
       <c r="E5" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E5</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
       <c r="F5" s="55"/>
     </row>
@@ -61365,7 +61367,7 @@
       </c>
       <c r="B6" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C6" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
@@ -61377,7 +61379,7 @@
       </c>
       <c r="E6" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E6</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61387,7 +61389,7 @@
       </c>
       <c r="B7" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C7" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
@@ -61399,7 +61401,7 @@
       </c>
       <c r="E7" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E7</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61409,7 +61411,7 @@
       </c>
       <c r="B8" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!B8</f>
-        <v>6E-008</v>
+        <v>3E-008</v>
       </c>
       <c r="C8" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C8</f>
@@ -61421,7 +61423,7 @@
       </c>
       <c r="E8" s="54" t="n">
         <f aca="false">truthStateInitialUncertainty!E8</f>
-        <v>2E-008</v>
+        <v>1E-008</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61663,8 +61665,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated units and R matrix, in progress 1
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,8 @@
     <sheet name="Constants" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" name="ac" vbProcedure="false">Constants!$B$15</definedName>
+    <definedName function="false" hidden="false" name="bc" vbProcedure="false">Constants!$B$14</definedName>
     <definedName function="false" hidden="false" name="days2hrs" vbProcedure="false">Constants!$B$6</definedName>
     <definedName function="false" hidden="false" name="g2mps2" vbProcedure="false">Constants!$B$5</definedName>
     <definedName function="false" hidden="false" name="hr2min" vbProcedure="false">Constants!$B$2</definedName>
@@ -27,7 +29,9 @@
     <definedName function="false" hidden="false" name="km2m" vbProcedure="false">Constants!$B$11</definedName>
     <definedName function="false" hidden="false" name="min2sec" vbProcedure="false">Constants!$B$3</definedName>
     <definedName function="false" hidden="false" name="Na" vbProcedure="false">general!$B$9</definedName>
+    <definedName function="false" hidden="false" name="pc" vbProcedure="false">Constants!$B$12</definedName>
     <definedName function="false" hidden="false" name="SpeedOfLight" vbProcedure="false">Constants!$B$8</definedName>
+    <definedName function="false" hidden="false" name="vc" vbProcedure="false">Constants!$B$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="216">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -281,7 +285,7 @@
     <t xml:space="preserve">b1</t>
   </si>
   <si>
-    <t xml:space="preserve">s</t>
+    <t xml:space="preserve">ns</t>
   </si>
   <si>
     <t xml:space="preserve">clock bias for asset 1</t>
@@ -362,7 +366,7 @@
     <t xml:space="preserve">ax</t>
   </si>
   <si>
-    <t xml:space="preserve">m/s^2</t>
+    <t xml:space="preserve">nm/s^2</t>
   </si>
   <si>
     <t xml:space="preserve">x component of atmospheric acceleration</t>
@@ -455,6 +459,9 @@
     <t xml:space="preserve">vt</t>
   </si>
   <si>
+    <t xml:space="preserve">units</t>
+  </si>
+  <si>
     <t xml:space="preserve">sig_b1_ss</t>
   </si>
   <si>
@@ -506,6 +513,9 @@
     <t xml:space="preserve">3-sigma of RSO x accelerations</t>
   </si>
   <si>
+    <t xml:space="preserve">cm^2/sec^3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q_grav_y</t>
   </si>
   <si>
@@ -524,6 +534,9 @@
     <t xml:space="preserve">3-sigma of RSO x atmo acceleration</t>
   </si>
   <si>
+    <t xml:space="preserve">deci nm/s^2</t>
+  </si>
+  <si>
     <t xml:space="preserve">sig_ay_ss</t>
   </si>
   <si>
@@ -534,6 +547,9 @@
   </si>
   <si>
     <t xml:space="preserve">3-sigma of RSO z atmo acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units2</t>
   </si>
   <si>
     <t xml:space="preserve">sig_b1</t>
@@ -584,6 +600,9 @@
     <t xml:space="preserve">3-sigma of RSO x position</t>
   </si>
   <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
     <t xml:space="preserve">sig_py</t>
   </si>
   <si>
@@ -600,6 +619,9 @@
   </si>
   <si>
     <t xml:space="preserve">3-sigma of RSO x velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm/s</t>
   </si>
   <si>
     <t xml:space="preserve">sig_vy</t>
@@ -621,6 +643,12 @@
   </si>
   <si>
     <t xml:space="preserve">sig_az</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/s^2</t>
   </si>
   <si>
     <t xml:space="preserve">hrs2min</t>
@@ -652,23 +680,38 @@
   <si>
     <t xml:space="preserve">km2m</t>
   </si>
+  <si>
+    <t xml:space="preserve">posCover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">velCover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biaCover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atmCover</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="11">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000E+00"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0000000000"/>
-    <numFmt numFmtId="171" formatCode="0.00E+00"/>
-    <numFmt numFmtId="172" formatCode="0.0000000000"/>
-    <numFmt numFmtId="173" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.00E+00"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="0.000E+00"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="173" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="174" formatCode="0.0000000"/>
+    <numFmt numFmtId="175" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000000000"/>
+    <numFmt numFmtId="177" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -716,7 +759,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -801,13 +844,6 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -834,7 +870,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -927,31 +963,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -959,31 +983,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -995,23 +999,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1031,7 +1023,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1039,23 +1055,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1079,11 +1115,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1091,11 +1127,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1115,8 +1151,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1138,18 +1178,18 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.2429149797571"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1385,16 +1425,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1408,7 +1448,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1416,7 +1456,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>60</v>
@@ -1424,7 +1464,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
@@ -1433,7 +1473,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>9.81</v>
@@ -1441,7 +1481,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>24</v>
@@ -1449,7 +1489,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B7" s="70" t="n">
         <f aca="false">398600.4418*(km2m^3)</f>
@@ -1458,7 +1498,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">299792.458*km2m</f>
@@ -1467,7 +1507,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>3500</v>
@@ -1475,7 +1515,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>300</v>
@@ -1483,10 +1523,42 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="71" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" s="71" t="n">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="71" t="n">
+        <v>10000000000</v>
       </c>
     </row>
   </sheetData>
@@ -1508,33 +1580,33 @@
   <dimension ref="1:59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
+      <selection pane="topLeft" activeCell="D65" activeCellId="0" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.21457489878543"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.96356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0"/>
@@ -2557,21 +2629,21 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="28" t="n">
+      <c r="B2" s="26" t="n">
         <v>7912.33967</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="29" t="n">
-        <f aca="false">B2*1000</f>
+      <c r="E2" s="27" t="n">
+        <f aca="false">B2*km2m*pc</f>
         <v>7912339.67</v>
       </c>
       <c r="F2" s="0"/>
@@ -3594,11 +3666,11 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="30" t="n">
+      <c r="B3" s="26" t="n">
         <v>2836.1046</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -3607,8 +3679,8 @@
       <c r="D3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="29" t="n">
-        <f aca="false">B3*1000</f>
+      <c r="E3" s="27" t="n">
+        <f aca="false">B3*km2m*pc</f>
         <v>2836104.6</v>
       </c>
       <c r="F3" s="0"/>
@@ -4631,21 +4703,21 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="31" t="n">
+      <c r="B4" s="26" t="n">
         <v>500.0817</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="32" t="n">
-        <f aca="false">B4*1000</f>
+      <c r="E4" s="27" t="n">
+        <f aca="false">B4*km2m*pc</f>
         <v>500081.7</v>
       </c>
       <c r="F4" s="0"/>
@@ -5668,22 +5740,22 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="30" t="n">
+      <c r="B5" s="26" t="n">
         <v>-2.3535</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="29" t="n">
-        <f aca="false">B5*1000</f>
-        <v>-2353.5</v>
+      <c r="E5" s="27" t="n">
+        <f aca="false">B5*km2m*vc</f>
+        <v>-235350</v>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -6705,11 +6777,11 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="30" t="n">
+      <c r="B6" s="26" t="n">
         <v>6.368</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -6718,9 +6790,9 @@
       <c r="D6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="29" t="n">
-        <f aca="false">B6*1000</f>
-        <v>6368</v>
+      <c r="E6" s="27" t="n">
+        <f aca="false">B6*km2m*vc</f>
+        <v>636800</v>
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -7742,22 +7814,22 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="31" t="n">
+      <c r="B7" s="26" t="n">
         <v>-1.1228565</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="32" t="n">
-        <f aca="false">B7*1000</f>
-        <v>-1122.8565</v>
+      <c r="E7" s="27" t="n">
+        <f aca="false">B7*km2m*vc</f>
+        <v>-112285.65</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -8779,11 +8851,11 @@
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="30" t="n">
+      <c r="B8" s="26" t="n">
         <v>7600</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -8792,8 +8864,8 @@
       <c r="D8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="29" t="n">
-        <f aca="false">B8*1000</f>
+      <c r="E8" s="27" t="n">
+        <f aca="false">B8*km2m*pc</f>
         <v>7600000</v>
       </c>
       <c r="F8" s="0"/>
@@ -9816,11 +9888,11 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="30" t="n">
+      <c r="B9" s="26" t="n">
         <v>3589</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -9829,8 +9901,8 @@
       <c r="D9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="29" t="n">
-        <f aca="false">B9*1000</f>
+      <c r="E9" s="27" t="n">
+        <f aca="false">B9*km2m*pc</f>
         <v>3589000</v>
       </c>
       <c r="F9" s="0"/>
@@ -10853,21 +10925,21 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="31" t="n">
+      <c r="B10" s="26" t="n">
         <v>-500</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="32" t="n">
-        <f aca="false">B10*1000</f>
+      <c r="E10" s="27" t="n">
+        <f aca="false">B10*km2m*pc</f>
         <v>-500000</v>
       </c>
       <c r="F10" s="0"/>
@@ -11890,29 +11962,29 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="12" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="30" t="n">
+      <c r="B11" s="26" t="n">
         <v>-2.839</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="29" t="n">
-        <f aca="false">B11*1000</f>
-        <v>-2839</v>
+      <c r="E11" s="27" t="n">
+        <f aca="false">B11*km2m*vc</f>
+        <v>-283900</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="30" t="n">
+      <c r="B12" s="26" t="n">
         <v>6.17</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -11921,9 +11993,9 @@
       <c r="D12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="29" t="n">
-        <f aca="false">B12*1000</f>
-        <v>6170</v>
+      <c r="E12" s="27" t="n">
+        <f aca="false">B12*km2m*vc</f>
+        <v>617000</v>
       </c>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -12945,22 +13017,22 @@
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="31" t="n">
+      <c r="B13" s="26" t="n">
         <v>-1.12</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="32" t="n">
-        <f aca="false">B13*1000</f>
-        <v>-1120</v>
+      <c r="E13" s="27" t="n">
+        <f aca="false">B13*km2m*vc</f>
+        <v>-112000</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -13982,11 +14054,11 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="30" t="n">
+      <c r="B14" s="26" t="n">
         <v>7993.22895176268</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -13995,8 +14067,8 @@
       <c r="D14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="29" t="n">
-        <f aca="false">B14*1000</f>
+      <c r="E14" s="27" t="n">
+        <f aca="false">B14*km2m*pc</f>
         <v>7993228.95176268</v>
       </c>
       <c r="F14" s="0"/>
@@ -15019,11 +15091,11 @@
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="30" t="n">
+      <c r="B15" s="26" t="n">
         <v>2319.63567604595</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -15032,8 +15104,8 @@
       <c r="D15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="29" t="n">
-        <f aca="false">B15*1000</f>
+      <c r="E15" s="27" t="n">
+        <f aca="false">B15*km2m*pc</f>
         <v>2319635.67604595</v>
       </c>
       <c r="F15" s="0"/>
@@ -16056,21 +16128,21 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="31" t="n">
+      <c r="B16" s="26" t="n">
         <v>1275.25350954771</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="32" t="n">
-        <f aca="false">B16*1000</f>
+      <c r="E16" s="27" t="n">
+        <f aca="false">B16*km2m*pc</f>
         <v>1275253.50954771</v>
       </c>
       <c r="F16" s="0"/>
@@ -17093,22 +17165,22 @@
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="30" t="n">
+      <c r="B17" s="26" t="n">
         <v>-2.15792847166078</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="29" t="n">
-        <f aca="false">B17*1000</f>
-        <v>-2157.92847166078</v>
+      <c r="E17" s="27" t="n">
+        <f aca="false">B17*km2m*vc</f>
+        <v>-215792.847166078</v>
       </c>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
@@ -18130,11 +18202,11 @@
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="30" t="n">
+      <c r="B18" s="26" t="n">
         <v>5.94339709534114</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -18143,9 +18215,9 @@
       <c r="D18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="29" t="n">
-        <f aca="false">B18*1000</f>
-        <v>5943.39709534114</v>
+      <c r="E18" s="27" t="n">
+        <f aca="false">B18*km2m*vc</f>
+        <v>594339.709534114</v>
       </c>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
@@ -19167,22 +19239,22 @@
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="31" t="n">
+      <c r="B19" s="26" t="n">
         <v>-2.7149898983448</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="32" t="n">
-        <f aca="false">B19*1000</f>
-        <v>-2714.9898983448</v>
+      <c r="E19" s="27" t="n">
+        <f aca="false">B19*km2m*vc</f>
+        <v>-271498.98983448</v>
       </c>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
@@ -20208,7 +20280,7 @@
       <c r="A20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="30" t="n">
+      <c r="B20" s="26" t="n">
         <v>8292.2152142172</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -20217,8 +20289,8 @@
       <c r="D20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="33" t="n">
-        <f aca="false">B20*1000</f>
+      <c r="E20" s="27" t="n">
+        <f aca="false">B20*km2m*pc</f>
         <v>8292215.2142172</v>
       </c>
       <c r="F20" s="0"/>
@@ -21245,7 +21317,7 @@
       <c r="A21" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="30" t="n">
+      <c r="B21" s="26" t="n">
         <v>8.95303314393977E-014</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -21254,8 +21326,8 @@
       <c r="D21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="29" t="n">
-        <f aca="false">B21*1000</f>
+      <c r="E21" s="27" t="n">
+        <f aca="false">B21*km2m*pc</f>
         <v>8.95303314393977E-011</v>
       </c>
       <c r="F21" s="0"/>
@@ -22279,20 +22351,20 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="31" t="n">
+      <c r="B22" s="26" t="n">
         <v>1462.14127210772</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="32" t="n">
-        <f aca="false">B22*1000</f>
+      <c r="E22" s="27" t="n">
+        <f aca="false">B22*km2m*pc</f>
         <v>1462141.27210772</v>
       </c>
       <c r="F22" s="0"/>
@@ -23319,18 +23391,18 @@
       <c r="A23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="30" t="n">
+      <c r="B23" s="26" t="n">
         <v>-1.19491895657397</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="29" t="n">
-        <f aca="false">B23*1000</f>
-        <v>-1194.91895657397</v>
+      <c r="E23" s="27" t="n">
+        <f aca="false">B23*km2m*vc</f>
+        <v>-119491.895657397</v>
       </c>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
@@ -24356,7 +24428,7 @@
       <c r="A24" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="30" t="n">
+      <c r="B24" s="26" t="n">
         <v>4.14954554750836E-016</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -24365,9 +24437,9 @@
       <c r="D24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="29" t="n">
-        <f aca="false">B24*1000</f>
-        <v>4.14954554750836E-013</v>
+      <c r="E24" s="27" t="n">
+        <f aca="false">B24*km2m*vc</f>
+        <v>4.14954554750836E-011</v>
       </c>
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
@@ -25390,21 +25462,21 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="31" t="n">
+      <c r="B25" s="26" t="n">
         <v>-6.77672215433451</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="32" t="n">
-        <f aca="false">B25*1000</f>
-        <v>-6776.72215433451</v>
+      <c r="E25" s="27" t="n">
+        <f aca="false">B25*km2m*vc</f>
+        <v>-677672.215433451</v>
       </c>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
@@ -26430,7 +26502,7 @@
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="30" t="n">
+      <c r="B26" s="26" t="n">
         <v>8292.2152142172</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -26439,8 +26511,8 @@
       <c r="D26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="29" t="n">
-        <f aca="false">B26*1000</f>
+      <c r="E26" s="27" t="n">
+        <f aca="false">B26*km2m*pc</f>
         <v>8292215.2142172</v>
       </c>
       <c r="F26" s="0"/>
@@ -27467,7 +27539,7 @@
       <c r="A27" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="30" t="n">
+      <c r="B27" s="26" t="n">
         <v>617.927602837498</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -27476,8 +27548,8 @@
       <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="29" t="n">
-        <f aca="false">B27*1000</f>
+      <c r="E27" s="27" t="n">
+        <f aca="false">B27*km2m*pc</f>
         <v>617927.602837498</v>
       </c>
       <c r="F27" s="0"/>
@@ -28501,20 +28573,20 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="31" t="n">
+      <c r="B28" s="26" t="n">
         <v>1325.1500206589</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="32" t="n">
-        <f aca="false">B28*1000</f>
+      <c r="E28" s="27" t="n">
+        <f aca="false">B28*km2m*pc</f>
         <v>1325150.0206589</v>
       </c>
       <c r="F28" s="0"/>
@@ -29541,18 +29613,18 @@
       <c r="A29" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="30" t="n">
+      <c r="B29" s="26" t="n">
         <v>-1.19491895657397</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="29" t="n">
-        <f aca="false">B29*1000</f>
-        <v>-1194.91895657397</v>
+      <c r="E29" s="27" t="n">
+        <f aca="false">B29*km2m*vc</f>
+        <v>-119491.895657397</v>
       </c>
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>
@@ -30578,7 +30650,7 @@
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="30" t="n">
+      <c r="B30" s="26" t="n">
         <v>2.86396653716454</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -30587,9 +30659,9 @@
       <c r="D30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="29" t="n">
-        <f aca="false">B30*1000</f>
-        <v>2863.96653716454</v>
+      <c r="E30" s="27" t="n">
+        <f aca="false">B30*km2m*vc</f>
+        <v>286396.653716454</v>
       </c>
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
@@ -31612,21 +31684,21 @@
       <c r="AMJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="31" t="n">
+      <c r="B31" s="26" t="n">
         <v>-6.14179605905715</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="32" t="n">
-        <f aca="false">B31*1000</f>
-        <v>-6141.79605905715</v>
+      <c r="E31" s="27" t="n">
+        <f aca="false">B31*km2m*vc</f>
+        <v>-614179.605905715</v>
       </c>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -32652,7 +32724,7 @@
       <c r="A32" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="30" t="n">
+      <c r="B32" s="26" t="n">
         <v>8059.7117971281</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -32661,8 +32733,8 @@
       <c r="D32" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="29" t="n">
-        <f aca="false">B32*1000</f>
+      <c r="E32" s="27" t="n">
+        <f aca="false">B32*km2m*pc</f>
         <v>8059711.7971281</v>
       </c>
       <c r="F32" s="0"/>
@@ -33689,7 +33761,7 @@
       <c r="A33" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="30" t="n">
+      <c r="B33" s="26" t="n">
         <v>-1339.01096535455</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -33698,8 +33770,8 @@
       <c r="D33" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="29" t="n">
-        <f aca="false">B33*1000</f>
+      <c r="E33" s="27" t="n">
+        <f aca="false">B33*km2m*pc</f>
         <v>-1339010.96535455</v>
       </c>
       <c r="F33" s="0"/>
@@ -34723,20 +34795,20 @@
       <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="31" t="n">
+      <c r="B34" s="26" t="n">
         <v>-2036.36579238367</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="32" t="n">
-        <f aca="false">B34*1000</f>
+      <c r="E34" s="27" t="n">
+        <f aca="false">B34*km2m*pc</f>
         <v>-2036365.79238367</v>
       </c>
       <c r="F34" s="0"/>
@@ -35763,18 +35835,18 @@
       <c r="A35" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="30" t="n">
+      <c r="B35" s="26" t="n">
         <v>1.94606884149104</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="29" t="n">
-        <f aca="false">B35*1000</f>
-        <v>1946.06884149104</v>
+      <c r="E35" s="27" t="n">
+        <f aca="false">B35*km2m*vc</f>
+        <v>194606.884149104</v>
       </c>
       <c r="F35" s="0"/>
       <c r="G35" s="0"/>
@@ -36800,7 +36872,7 @@
       <c r="A36" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="30" t="n">
+      <c r="B36" s="26" t="n">
         <v>4.76007007933894</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -36809,9 +36881,9 @@
       <c r="D36" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="29" t="n">
-        <f aca="false">B36*1000</f>
-        <v>4760.07007933894</v>
+      <c r="E36" s="27" t="n">
+        <f aca="false">B36*km2m*vc</f>
+        <v>476007.007933894</v>
       </c>
       <c r="F36" s="0"/>
       <c r="G36" s="0"/>
@@ -37834,21 +37906,21 @@
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="31" t="n">
+      <c r="B37" s="26" t="n">
         <v>-4.57234550026438</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="32" t="n">
-        <f aca="false">B37*1000</f>
-        <v>-4572.34550026438</v>
+      <c r="E37" s="27" t="n">
+        <f aca="false">B37*km2m*vc</f>
+        <v>-457234.550026438</v>
       </c>
       <c r="F37" s="0"/>
       <c r="G37" s="0"/>
@@ -38874,7 +38946,7 @@
       <c r="A38" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="30" t="n">
+      <c r="B38" s="26" t="n">
         <v>-5836.97295524894</v>
       </c>
       <c r="C38" s="12" t="s">
@@ -38883,8 +38955,8 @@
       <c r="D38" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="29" t="n">
-        <f aca="false">B38*1000</f>
+      <c r="E38" s="27" t="n">
+        <f aca="false">B38*km2m*pc</f>
         <v>-5836972.95524894</v>
       </c>
       <c r="F38" s="0"/>
@@ -39911,7 +39983,7 @@
       <c r="A39" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="30" t="n">
+      <c r="B39" s="26" t="n">
         <v>3769.19293812876</v>
       </c>
       <c r="C39" s="12" t="s">
@@ -39920,8 +39992,8 @@
       <c r="D39" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E39" s="29" t="n">
-        <f aca="false">B39*1000</f>
+      <c r="E39" s="27" t="n">
+        <f aca="false">B39*km2m*pc</f>
         <v>3769192.93812876</v>
       </c>
       <c r="F39" s="0"/>
@@ -40945,20 +41017,20 @@
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="31" t="n">
+      <c r="B40" s="26" t="n">
         <v>4756.21925202663</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E40" s="32" t="n">
-        <f aca="false">B40*1000</f>
+      <c r="E40" s="27" t="n">
+        <f aca="false">B40*km2m*pc</f>
         <v>4756219.25202663</v>
       </c>
       <c r="F40" s="0"/>
@@ -41985,18 +42057,18 @@
       <c r="A41" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="30" t="n">
+      <c r="B41" s="26" t="n">
         <v>-4.09973571358502</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="29" t="n">
-        <f aca="false">B41*1000</f>
-        <v>-4099.73571358502</v>
+      <c r="E41" s="27" t="n">
+        <f aca="false">B41*km2m*vc</f>
+        <v>-409973.571358502</v>
       </c>
       <c r="F41" s="0"/>
       <c r="G41" s="0"/>
@@ -43022,7 +43094,7 @@
       <c r="A42" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="30" t="n">
+      <c r="B42" s="26" t="n">
         <v>-5.48399666550907</v>
       </c>
       <c r="C42" s="12" t="s">
@@ -43031,9 +43103,9 @@
       <c r="D42" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="29" t="n">
-        <f aca="false">B42*1000</f>
-        <v>-5483.99666550907</v>
+      <c r="E42" s="27" t="n">
+        <f aca="false">B42*km2m*vc</f>
+        <v>-548399.666550907</v>
       </c>
       <c r="F42" s="0"/>
       <c r="G42" s="0"/>
@@ -44056,21 +44128,21 @@
       <c r="AMJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="31" t="n">
+      <c r="B43" s="26" t="n">
         <v>0.685377356840007</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="32" t="n">
-        <f aca="false">B43*1000</f>
-        <v>685.377356840007</v>
+      <c r="E43" s="27" t="n">
+        <f aca="false">B43*km2m*vc</f>
+        <v>68537.7356840007</v>
       </c>
       <c r="F43" s="0"/>
       <c r="G43" s="0"/>
@@ -45092,12 +45164,12 @@
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="34" t="n">
-        <v>5.47E-008</v>
+      <c r="B44" s="28" t="n">
+        <v>25</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>80</v>
@@ -45105,9 +45177,9 @@
       <c r="D44" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="33" t="n">
-        <f aca="false">B44</f>
-        <v>5.47E-008</v>
+      <c r="E44" s="28" t="n">
+        <f aca="false">B44/1000000000*bc</f>
+        <v>25</v>
       </c>
       <c r="F44" s="0"/>
       <c r="G44" s="0"/>
@@ -46129,12 +46201,12 @@
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="34" t="n">
-        <v>3.23E-009</v>
+      <c r="B45" s="28" t="n">
+        <v>3.23</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>80</v>
@@ -46142,9 +46214,9 @@
       <c r="D45" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="29" t="n">
-        <f aca="false">B45</f>
-        <v>3.23E-009</v>
+      <c r="E45" s="28" t="n">
+        <f aca="false">B45/1000000000*bc</f>
+        <v>3.23</v>
       </c>
       <c r="F45" s="0"/>
       <c r="G45" s="0"/>
@@ -47166,12 +47238,12 @@
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="34" t="n">
-        <v>-2E-009</v>
+      <c r="B46" s="28" t="n">
+        <v>-2</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>80</v>
@@ -47179,9 +47251,9 @@
       <c r="D46" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="29" t="n">
-        <f aca="false">B46</f>
-        <v>-2E-009</v>
+      <c r="E46" s="28" t="n">
+        <f aca="false">B46/1000000000*bc</f>
+        <v>-2</v>
       </c>
       <c r="F46" s="0"/>
       <c r="G46" s="0"/>
@@ -48203,12 +48275,12 @@
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="34" t="n">
-        <v>0</v>
+      <c r="B47" s="28" t="n">
+        <v>-12</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>80</v>
@@ -48216,9 +48288,9 @@
       <c r="D47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="29" t="n">
-        <f aca="false">B47</f>
-        <v>0</v>
+      <c r="E47" s="28" t="n">
+        <f aca="false">B47/1000000000*bc</f>
+        <v>-12</v>
       </c>
       <c r="F47" s="0"/>
       <c r="G47" s="0"/>
@@ -49240,12 +49312,12 @@
       <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="34" t="n">
-        <v>0</v>
+      <c r="B48" s="28" t="n">
+        <v>24</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>80</v>
@@ -49253,9 +49325,9 @@
       <c r="D48" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="29" t="n">
-        <f aca="false">B48</f>
-        <v>0</v>
+      <c r="E48" s="28" t="n">
+        <f aca="false">B48/1000000000*bc</f>
+        <v>24</v>
       </c>
       <c r="F48" s="0"/>
       <c r="G48" s="0"/>
@@ -50277,12 +50349,12 @@
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="34" t="n">
-        <v>0</v>
+      <c r="B49" s="28" t="n">
+        <v>-20</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>80</v>
@@ -50290,9 +50362,9 @@
       <c r="D49" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="29" t="n">
-        <f aca="false">B49</f>
-        <v>0</v>
+      <c r="E49" s="28" t="n">
+        <f aca="false">B49/1000000000*bc</f>
+        <v>-20</v>
       </c>
       <c r="F49" s="0"/>
       <c r="G49" s="0"/>
@@ -51314,22 +51386,22 @@
       <c r="AMI49" s="0"/>
       <c r="AMJ49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="17" t="s">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" s="17" t="s">
+      <c r="B50" s="28" t="n">
+        <v>6</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E50" s="32" t="n">
-        <f aca="false">B50</f>
-        <v>0</v>
+      <c r="E50" s="28" t="n">
+        <f aca="false">B50/1000000000*bc</f>
+        <v>6</v>
       </c>
       <c r="F50" s="0"/>
       <c r="G50" s="0"/>
@@ -52351,148 +52423,148 @@
       <c r="AMI50" s="0"/>
       <c r="AMJ50" s="0"/>
     </row>
-    <row r="51" s="38" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="36" t="s">
+    <row r="51" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="36" t="n">
+      <c r="B51" s="29" t="n">
         <v>7142.8</v>
       </c>
-      <c r="C51" s="36" t="s">
+      <c r="C51" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="37" t="n">
-        <f aca="false">B51*1000</f>
+      <c r="E51" s="27" t="n">
+        <f aca="false">B51*km2m*pc</f>
         <v>7142800</v>
       </c>
     </row>
-    <row r="52" s="39" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="38" t="s">
+    <row r="52" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="38" t="n">
+      <c r="B52" s="30" t="n">
         <v>4456.8</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E52" s="37" t="n">
-        <f aca="false">B52*1000</f>
+      <c r="E52" s="27" t="n">
+        <f aca="false">B52*km2m*pc</f>
         <v>4456800</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="40" t="s">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="40" t="n">
+      <c r="B53" s="29" t="n">
         <v>127.434</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="40" t="s">
+      <c r="D53" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E53" s="41" t="n">
-        <f aca="false">B53*1000</f>
+      <c r="E53" s="27" t="n">
+        <f aca="false">B53*km2m*pc</f>
         <v>127434</v>
       </c>
       <c r="F53" s="0"/>
       <c r="G53" s="0"/>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="36" t="s">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="36" t="n">
+      <c r="B54" s="29" t="n">
         <v>-3.637</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="37" t="n">
-        <f aca="false">B54*1000</f>
-        <v>-3637</v>
+      <c r="E54" s="27" t="n">
+        <f aca="false">B54*km2m*vc</f>
+        <v>-363700</v>
       </c>
       <c r="F54" s="0"/>
       <c r="G54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="38" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="38" t="n">
+      <c r="B55" s="30" t="n">
         <v>5.812</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D55" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="E55" s="37" t="n">
-        <f aca="false">B55*1000</f>
-        <v>5812</v>
+      <c r="E55" s="27" t="n">
+        <f aca="false">B55*km2m*vc</f>
+        <v>581200</v>
       </c>
       <c r="F55" s="0"/>
       <c r="G55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="40" t="s">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="40" t="n">
+      <c r="B56" s="29" t="n">
         <v>-0.5906</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E56" s="41" t="n">
-        <f aca="false">B56*1000</f>
-        <v>-590.6</v>
-      </c>
-      <c r="F56" s="36"/>
-      <c r="G56" s="43"/>
+      <c r="E56" s="27" t="n">
+        <f aca="false">B56*km2m*vc</f>
+        <v>-59060</v>
+      </c>
+      <c r="F56" s="29"/>
+      <c r="G56" s="32"/>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="s">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="8" t="n">
-        <v>-0.0007</v>
-      </c>
-      <c r="C57" s="8" t="s">
+      <c r="B57" s="12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C57" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E57" s="44" t="n">
-        <f aca="false">B57</f>
-        <v>-0.0007</v>
+      <c r="E57" s="28" t="n">
+        <f aca="false">B57/1000000000*ac</f>
+        <v>1</v>
       </c>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
         <v>109</v>
       </c>
       <c r="B58" s="12" t="n">
-        <v>0.0001</v>
+        <v>0.2</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>107</v>
@@ -52500,29 +52572,29 @@
       <c r="D58" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E58" s="13" t="n">
-        <f aca="false">B58</f>
-        <v>0.0001</v>
+      <c r="E58" s="28" t="n">
+        <f aca="false">B58/1000000000*ac</f>
+        <v>2</v>
       </c>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="17" t="s">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="17" t="n">
-        <v>-4E-005</v>
-      </c>
-      <c r="C59" s="17" t="s">
+      <c r="B59" s="12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E59" s="18" t="n">
-        <f aca="false">B59</f>
-        <v>-4E-005</v>
+      <c r="E59" s="28" t="n">
+        <f aca="false">B59/1000000000*ac</f>
+        <v>3</v>
       </c>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
@@ -52552,24 +52624,24 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="31" t="s">
         <v>117</v>
       </c>
       <c r="F1" s="0"/>
@@ -53592,65 +53664,65 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+    <row r="2" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="27" t="n">
+      <c r="B2" s="33" t="n">
         <f aca="false">IF(Na&gt;=1,1,0)</f>
         <v>1</v>
       </c>
-      <c r="C2" s="27" t="n">
+      <c r="C2" s="33" t="n">
         <f aca="false">B2+2</f>
         <v>3</v>
       </c>
-      <c r="D2" s="27" t="n">
+      <c r="D2" s="33" t="n">
         <f aca="false">B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="27" t="n">
+      <c r="E2" s="33" t="n">
         <f aca="false">C2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+    <row r="3" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="27" t="n">
+      <c r="B3" s="33" t="n">
         <f aca="false">C2+1</f>
         <v>4</v>
       </c>
-      <c r="C3" s="27" t="n">
+      <c r="C3" s="33" t="n">
         <f aca="false">B3+2</f>
         <v>6</v>
       </c>
-      <c r="D3" s="27" t="n">
+      <c r="D3" s="33" t="n">
         <f aca="false">B3</f>
         <v>4</v>
       </c>
-      <c r="E3" s="27" t="n">
+      <c r="E3" s="33" t="n">
         <f aca="false">C3</f>
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="27" t="n">
+      <c r="B4" s="33" t="n">
         <f aca="false">IF(Na&gt;=2,C3+1,0)</f>
         <v>7</v>
       </c>
-      <c r="C4" s="27" t="n">
+      <c r="C4" s="33" t="n">
         <f aca="false">B4+2</f>
         <v>9</v>
       </c>
-      <c r="D4" s="27" t="n">
+      <c r="D4" s="33" t="n">
         <f aca="false">B4</f>
         <v>7</v>
       </c>
-      <c r="E4" s="27" t="n">
+      <c r="E4" s="33" t="n">
         <f aca="false">C4</f>
         <v>9</v>
       </c>
@@ -54675,22 +54747,22 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="27" t="n">
+      <c r="B5" s="33" t="n">
         <f aca="false">C4+1</f>
         <v>10</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="33" t="n">
         <f aca="false">B5+2</f>
         <v>12</v>
       </c>
-      <c r="D5" s="27" t="n">
+      <c r="D5" s="33" t="n">
         <f aca="false">B5</f>
         <v>10</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="E5" s="33" t="n">
         <f aca="false">C5</f>
         <v>12</v>
       </c>
@@ -55714,65 +55786,65 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+    <row r="6" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="27" t="n">
+      <c r="B6" s="33" t="n">
         <f aca="false">IF(Na&gt;=3,C5+1,0)</f>
         <v>13</v>
       </c>
-      <c r="C6" s="27" t="n">
+      <c r="C6" s="33" t="n">
         <f aca="false">B6+2</f>
         <v>15</v>
       </c>
-      <c r="D6" s="27" t="n">
+      <c r="D6" s="33" t="n">
         <f aca="false">B6</f>
         <v>13</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="33" t="n">
         <f aca="false">C6</f>
         <v>15</v>
       </c>
     </row>
-    <row r="7" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+    <row r="7" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="27" t="n">
+      <c r="B7" s="33" t="n">
         <f aca="false">C6+1</f>
         <v>16</v>
       </c>
-      <c r="C7" s="27" t="n">
+      <c r="C7" s="33" t="n">
         <f aca="false">B7+2</f>
         <v>18</v>
       </c>
-      <c r="D7" s="27" t="n">
+      <c r="D7" s="33" t="n">
         <f aca="false">B7</f>
         <v>16</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="33" t="n">
         <f aca="false">C7</f>
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="27" t="n">
+      <c r="B8" s="33" t="n">
         <f aca="false">IF(Na&gt;=4,C7+1,0)</f>
         <v>19</v>
       </c>
-      <c r="C8" s="27" t="n">
+      <c r="C8" s="33" t="n">
         <f aca="false">B8+2</f>
         <v>21</v>
       </c>
-      <c r="D8" s="27" t="n">
+      <c r="D8" s="33" t="n">
         <f aca="false">B8</f>
         <v>19</v>
       </c>
-      <c r="E8" s="27" t="n">
+      <c r="E8" s="33" t="n">
         <f aca="false">C8</f>
         <v>21</v>
       </c>
@@ -56797,22 +56869,22 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="27" t="n">
+      <c r="B9" s="33" t="n">
         <f aca="false">C8+1</f>
         <v>22</v>
       </c>
-      <c r="C9" s="27" t="n">
+      <c r="C9" s="33" t="n">
         <f aca="false">B9+2</f>
         <v>24</v>
       </c>
-      <c r="D9" s="27" t="n">
+      <c r="D9" s="33" t="n">
         <f aca="false">B9</f>
         <v>22</v>
       </c>
-      <c r="E9" s="27" t="n">
+      <c r="E9" s="33" t="n">
         <f aca="false">C9</f>
         <v>24</v>
       </c>
@@ -57836,65 +57908,65 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+    <row r="10" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="27" t="n">
+      <c r="B10" s="33" t="n">
         <f aca="false">IF(Na&gt;=5,C9+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="27" t="n">
+      <c r="C10" s="33" t="n">
         <f aca="false">B10+2</f>
         <v>2</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="33" t="n">
         <f aca="false">B10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="27" t="n">
+      <c r="E10" s="33" t="n">
         <f aca="false">C10</f>
         <v>2</v>
       </c>
     </row>
-    <row r="11" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="s">
+    <row r="11" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="27" t="n">
+      <c r="B11" s="33" t="n">
         <f aca="false">C10+1</f>
         <v>3</v>
       </c>
-      <c r="C11" s="27" t="n">
+      <c r="C11" s="33" t="n">
         <f aca="false">B11+2</f>
         <v>5</v>
       </c>
-      <c r="D11" s="27" t="n">
+      <c r="D11" s="33" t="n">
         <f aca="false">B11</f>
         <v>3</v>
       </c>
-      <c r="E11" s="27" t="n">
+      <c r="E11" s="33" t="n">
         <f aca="false">C11</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="27" t="n">
+      <c r="B12" s="33" t="n">
         <f aca="false">IF(Na&gt;=6,C11+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="27" t="n">
+      <c r="C12" s="33" t="n">
         <f aca="false">B12+2</f>
         <v>2</v>
       </c>
-      <c r="D12" s="27" t="n">
+      <c r="D12" s="33" t="n">
         <f aca="false">B12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="27" t="n">
+      <c r="E12" s="33" t="n">
         <f aca="false">C12</f>
         <v>2</v>
       </c>
@@ -58919,22 +58991,22 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="27" t="n">
+      <c r="B13" s="33" t="n">
         <f aca="false">C12+1</f>
         <v>3</v>
       </c>
-      <c r="C13" s="27" t="n">
+      <c r="C13" s="33" t="n">
         <f aca="false">B13+2</f>
         <v>5</v>
       </c>
-      <c r="D13" s="27" t="n">
+      <c r="D13" s="33" t="n">
         <f aca="false">B13</f>
         <v>3</v>
       </c>
-      <c r="E13" s="27" t="n">
+      <c r="E13" s="33" t="n">
         <f aca="false">C13</f>
         <v>5</v>
       </c>
@@ -59958,128 +60030,128 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+    <row r="14" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="27" t="n">
+      <c r="B14" s="33" t="n">
         <f aca="false">IF(Na&gt;=7,C13+1,0)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="27" t="n">
+      <c r="C14" s="33" t="n">
         <f aca="false">B14+2</f>
         <v>2</v>
       </c>
-      <c r="D14" s="27" t="n">
+      <c r="D14" s="33" t="n">
         <f aca="false">B14</f>
         <v>0</v>
       </c>
-      <c r="E14" s="27" t="n">
+      <c r="E14" s="33" t="n">
         <f aca="false">C14</f>
         <v>2</v>
       </c>
     </row>
-    <row r="15" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="s">
+    <row r="15" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="27" t="n">
+      <c r="B15" s="33" t="n">
         <f aca="false">C14+1</f>
         <v>3</v>
       </c>
-      <c r="C15" s="27" t="n">
+      <c r="C15" s="33" t="n">
         <f aca="false">B15+2</f>
         <v>5</v>
       </c>
-      <c r="D15" s="27" t="n">
+      <c r="D15" s="33" t="n">
         <f aca="false">B15</f>
         <v>3</v>
       </c>
-      <c r="E15" s="27" t="n">
+      <c r="E15" s="33" t="n">
         <f aca="false">C15</f>
         <v>5</v>
       </c>
     </row>
-    <row r="16" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="s">
+    <row r="16" s="33" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="27" t="n">
+      <c r="B16" s="33" t="n">
         <f aca="false">1+6*Na</f>
         <v>25</v>
       </c>
-      <c r="C16" s="27" t="n">
+      <c r="C16" s="33" t="n">
         <f aca="false">7*Na</f>
         <v>28</v>
       </c>
-      <c r="D16" s="27" t="n">
+      <c r="D16" s="33" t="n">
         <f aca="false">B16</f>
         <v>25</v>
       </c>
-      <c r="E16" s="27" t="n">
+      <c r="E16" s="33" t="n">
         <f aca="false">C16</f>
         <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="39" t="n">
+      <c r="B17" s="31" t="n">
         <f aca="false">C16+1</f>
         <v>29</v>
       </c>
-      <c r="C17" s="39" t="n">
+      <c r="C17" s="31" t="n">
         <f aca="false">B17+2</f>
         <v>31</v>
       </c>
-      <c r="D17" s="27" t="n">
+      <c r="D17" s="33" t="n">
         <f aca="false">B17</f>
         <v>29</v>
       </c>
-      <c r="E17" s="27" t="n">
+      <c r="E17" s="33" t="n">
         <f aca="false">C17</f>
         <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="39" t="n">
+      <c r="B18" s="31" t="n">
         <f aca="false">C17+1</f>
         <v>32</v>
       </c>
-      <c r="C18" s="39" t="n">
+      <c r="C18" s="31" t="n">
         <f aca="false">B18+2</f>
         <v>34</v>
       </c>
-      <c r="D18" s="27" t="n">
+      <c r="D18" s="33" t="n">
         <f aca="false">B18</f>
         <v>32</v>
       </c>
-      <c r="E18" s="27" t="n">
+      <c r="E18" s="33" t="n">
         <f aca="false">C18</f>
         <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="B19" s="39" t="n">
+      <c r="B19" s="31" t="n">
         <f aca="false">C18+1</f>
         <v>35</v>
       </c>
-      <c r="C19" s="39" t="n">
+      <c r="C19" s="31" t="n">
         <f aca="false">B19+2</f>
         <v>37</v>
       </c>
-      <c r="D19" s="27" t="n">
+      <c r="D19" s="33" t="n">
         <f aca="false">B19</f>
         <v>35</v>
       </c>
-      <c r="E19" s="27" t="n">
+      <c r="E19" s="33" t="n">
         <f aca="false">C19</f>
         <v>37</v>
       </c>
@@ -60111,7 +60183,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60234,7 +60306,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -60242,261 +60314,303 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.1983805668016"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1619433198381"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="49" t="n">
-        <v>3E-008</v>
+        <v>139</v>
+      </c>
+      <c r="B2" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="50" t="n">
-        <f aca="false">B2/3</f>
-        <v>1E-008</v>
+        <v>140</v>
+      </c>
+      <c r="E2" s="40" t="n">
+        <f aca="false">B2/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="49" t="n">
-        <v>3E-008</v>
+        <v>141</v>
+      </c>
+      <c r="B3" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" s="50" t="n">
-        <f aca="false">B3/3</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F3" s="51"/>
+        <v>142</v>
+      </c>
+      <c r="E3" s="40" t="n">
+        <f aca="false">B3/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="49" t="n">
-        <v>3E-008</v>
+        <v>143</v>
+      </c>
+      <c r="B4" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="50" t="n">
-        <f aca="false">B4/3</f>
-        <v>1E-008</v>
+        <v>144</v>
+      </c>
+      <c r="E4" s="40" t="n">
+        <f aca="false">B4/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="49" t="n">
-        <v>3E-008</v>
+        <v>145</v>
+      </c>
+      <c r="B5" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="50" t="n">
-        <f aca="false">B5/3</f>
-        <v>1E-008</v>
+        <v>146</v>
+      </c>
+      <c r="E5" s="40" t="n">
+        <f aca="false">B5/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B6" s="49" t="n">
-        <v>3E-008</v>
+        <v>147</v>
+      </c>
+      <c r="B6" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E6" s="50" t="n">
-        <f aca="false">B6/3</f>
-        <v>1E-008</v>
+        <v>148</v>
+      </c>
+      <c r="E6" s="40" t="n">
+        <f aca="false">B6/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="49" t="n">
-        <v>3E-008</v>
+        <v>149</v>
+      </c>
+      <c r="B7" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="50" t="n">
-        <f aca="false">B7/3</f>
-        <v>1E-008</v>
+        <v>150</v>
+      </c>
+      <c r="E7" s="40" t="n">
+        <f aca="false">B7/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="49" t="n">
-        <v>3E-008</v>
+        <v>151</v>
+      </c>
+      <c r="B8" s="39" t="n">
+        <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="50" t="n">
-        <f aca="false">B8/3</f>
-        <v>1E-008</v>
+        <v>152</v>
+      </c>
+      <c r="E8" s="40" t="n">
+        <f aca="false">B8/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="49" t="n">
+        <v>153</v>
+      </c>
+      <c r="B9" s="42" t="n">
         <v>4.8E-007</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="50" t="n">
-        <f aca="false">B9/3</f>
-        <v>1.6E-007</v>
+        <v>155</v>
+      </c>
+      <c r="E9" s="43" t="n">
+        <f aca="false">B9/3*vc^2</f>
+        <v>0.0016</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="49" t="n">
+        <v>157</v>
+      </c>
+      <c r="B10" s="42" t="n">
         <v>4.8E-007</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D10" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="43" t="n">
+        <f aca="false">B10/3*vc^2</f>
+        <v>0.0016</v>
+      </c>
+      <c r="F10" s="38" t="s">
         <v>156</v>
-      </c>
-      <c r="E10" s="50" t="n">
-        <f aca="false">B10/3</f>
-        <v>1.6E-007</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" s="49" t="n">
+        <v>159</v>
+      </c>
+      <c r="B11" s="42" t="n">
         <v>4.8E-007</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="E11" s="50" t="n">
-        <f aca="false">B11/3</f>
-        <v>1.6E-007</v>
+        <v>160</v>
+      </c>
+      <c r="E11" s="43" t="n">
+        <f aca="false">B11/3*vc^2</f>
+        <v>0.0016</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="49" t="n">
-        <v>1E-009</v>
+        <v>161</v>
+      </c>
+      <c r="B12" s="39" t="n">
+        <v>1</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="50" t="n">
-        <f aca="false">B12/3</f>
-        <v>3.33333333333333E-010</v>
+        <v>162</v>
+      </c>
+      <c r="E12" s="44" t="n">
+        <f aca="false">B12/3/1000000000*ac</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="49" t="n">
-        <v>1E-009</v>
+        <v>164</v>
+      </c>
+      <c r="B13" s="39" t="n">
+        <v>1</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="50" t="n">
-        <f aca="false">B13/3</f>
-        <v>3.33333333333333E-010</v>
+        <v>165</v>
+      </c>
+      <c r="E13" s="44" t="n">
+        <f aca="false">B13/3/1000000000*ac</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="49" t="n">
-        <v>1E-009</v>
+        <v>166</v>
+      </c>
+      <c r="B14" s="39" t="n">
+        <v>1</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E14" s="50" t="n">
-        <f aca="false">B14/3</f>
-        <v>3.33333333333333E-010</v>
+        <v>167</v>
+      </c>
+      <c r="E14" s="44" t="n">
+        <f aca="false">B14/3/1000000000*ac</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -60515,178 +60629,202 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="29.6720647773279"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="9.51417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="7.97165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.1214574898785"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="45" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="37" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="49" t="n">
+        <v>169</v>
+      </c>
+      <c r="B2" s="39" t="n">
         <f aca="false">truthStateParams!B2</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="50" t="n">
-        <f aca="false">B2/3</f>
-        <v>1E-008</v>
+        <v>170</v>
+      </c>
+      <c r="E2" s="45" t="n">
+        <f aca="false">B2/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="49" t="n">
+        <v>171</v>
+      </c>
+      <c r="B3" s="39" t="n">
         <f aca="false">truthStateParams!B3</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" s="50" t="n">
-        <f aca="false">B3/3</f>
-        <v>1E-008</v>
+        <v>172</v>
+      </c>
+      <c r="E3" s="45" t="n">
+        <f aca="false">B3/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="49" t="n">
+        <v>173</v>
+      </c>
+      <c r="B4" s="39" t="n">
         <f aca="false">truthStateParams!B4</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" s="50" t="n">
-        <f aca="false">B4/3</f>
-        <v>1E-008</v>
+        <v>174</v>
+      </c>
+      <c r="E4" s="45" t="n">
+        <f aca="false">B4/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" s="49" t="n">
+        <v>175</v>
+      </c>
+      <c r="B5" s="39" t="n">
         <f aca="false">truthStateParams!B5</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="E5" s="50" t="n">
-        <f aca="false">B5/3</f>
-        <v>1E-008</v>
+        <v>176</v>
+      </c>
+      <c r="E5" s="45" t="n">
+        <f aca="false">B5/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="49" t="n">
+        <v>177</v>
+      </c>
+      <c r="B6" s="39" t="n">
         <f aca="false">truthStateParams!B6</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="E6" s="50" t="n">
-        <f aca="false">B6/3</f>
-        <v>1E-008</v>
+        <v>178</v>
+      </c>
+      <c r="E6" s="45" t="n">
+        <f aca="false">B6/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7" s="49" t="n">
+        <v>179</v>
+      </c>
+      <c r="B7" s="39" t="n">
         <f aca="false">truthStateParams!B7</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="50" t="n">
-        <f aca="false">B7/3</f>
-        <v>1E-008</v>
+        <v>180</v>
+      </c>
+      <c r="E7" s="45" t="n">
+        <f aca="false">B7/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" s="49" t="n">
+        <v>181</v>
+      </c>
+      <c r="B8" s="39" t="n">
         <f aca="false">truthStateParams!B8</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="50" t="n">
-        <f aca="false">B8/3</f>
-        <v>1E-008</v>
+        <v>182</v>
+      </c>
+      <c r="E8" s="45" t="n">
+        <f aca="false">B8/3/1000000000*bc</f>
+        <v>10</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="21" t="n">
+        <v>183</v>
+      </c>
+      <c r="B9" s="46" t="n">
         <f aca="false">0.00000006*SpeedOfLight/km2m</f>
         <v>0.01798754748</v>
       </c>
@@ -60694,18 +60832,21 @@
         <v>30</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="50" t="n">
-        <f aca="false">B9/3*km2m</f>
+        <v>184</v>
+      </c>
+      <c r="E9" s="45" t="n">
+        <f aca="false">B9/3*km2m*pc</f>
         <v>5.99584916</v>
       </c>
+      <c r="F9" s="21" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" s="21" t="n">
+        <v>186</v>
+      </c>
+      <c r="B10" s="46" t="n">
         <f aca="false">0.00000006*SpeedOfLight/km2m</f>
         <v>0.01798754748</v>
       </c>
@@ -60713,18 +60854,21 @@
         <v>30</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="E10" s="50" t="n">
-        <f aca="false">B10/3*km2m</f>
+        <v>187</v>
+      </c>
+      <c r="E10" s="45" t="n">
+        <f aca="false">B10/3*km2m*pc</f>
         <v>5.99584916</v>
       </c>
+      <c r="F10" s="21" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="B11" s="21" t="n">
+        <v>188</v>
+      </c>
+      <c r="B11" s="46" t="n">
         <f aca="false">0.00000006*SpeedOfLight/km2m</f>
         <v>0.01798754748</v>
       </c>
@@ -60732,122 +60876,143 @@
         <v>30</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E11" s="50" t="n">
-        <f aca="false">B11/3*km2m</f>
+        <v>189</v>
+      </c>
+      <c r="E11" s="45" t="n">
+        <f aca="false">B11/3*km2m*pc</f>
         <v>5.99584916</v>
       </c>
+      <c r="F11" s="21" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="B12" s="49" t="n">
+        <v>190</v>
+      </c>
+      <c r="B12" s="46" t="n">
         <v>0.000153</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="E12" s="50" t="n">
-        <f aca="false">B12/3*km2m</f>
-        <v>0.051</v>
+        <v>191</v>
+      </c>
+      <c r="E12" s="44" t="n">
+        <f aca="false">B12/3*km2m*vc</f>
+        <v>5.1</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="B13" s="49" t="n">
+        <v>193</v>
+      </c>
+      <c r="B13" s="46" t="n">
         <v>0.000153</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="E13" s="50" t="n">
-        <f aca="false">B13/3*km2m</f>
-        <v>0.051</v>
+        <v>194</v>
+      </c>
+      <c r="E13" s="44" t="n">
+        <f aca="false">B13/3*km2m*vc</f>
+        <v>5.1</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="B14" s="49" t="n">
+        <v>195</v>
+      </c>
+      <c r="B14" s="46" t="n">
         <v>0.000153</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="E14" s="50" t="n">
-        <f aca="false">B14/3*km2m</f>
-        <v>0.051</v>
+        <v>196</v>
+      </c>
+      <c r="E14" s="44" t="n">
+        <f aca="false">B14/3*km2m*vc</f>
+        <v>5.1</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="49" t="n">
+        <v>197</v>
+      </c>
+      <c r="B15" s="39" t="n">
         <f aca="false">truthStateParams!B12</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" s="50" t="n">
-        <f aca="false">B15/3</f>
-        <v>3.33333333333333E-010</v>
+        <v>162</v>
+      </c>
+      <c r="E15" s="45" t="n">
+        <f aca="false">B15/3/1000000000*ac</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="B16" s="49" t="n">
+        <v>198</v>
+      </c>
+      <c r="B16" s="39" t="n">
         <f aca="false">truthStateParams!B13</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="50" t="n">
-        <f aca="false">B16/3</f>
-        <v>3.33333333333333E-010</v>
+        <v>165</v>
+      </c>
+      <c r="E16" s="45" t="n">
+        <f aca="false">B16/3/1000000000*ac</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>163</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="B17" s="49" t="n">
+        <v>199</v>
+      </c>
+      <c r="B17" s="39" t="n">
         <f aca="false">truthStateParams!B14</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>107</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E17" s="50" t="n">
-        <f aca="false">B17/3</f>
-        <v>3.33333333333333E-010</v>
+        <v>167</v>
+      </c>
+      <c r="E17" s="45" t="n">
+        <f aca="false">B17/3/1000000000*ac</f>
+        <v>3.33333333333333</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -60869,150 +61034,150 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="45" width="9.73279352226721"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="21" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="36.1983805668016"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="45" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="str">
         <f aca="false">truthStateParams!A2</f>
         <v>sig_b1_ss</v>
       </c>
-      <c r="B2" s="53" t="n">
+      <c r="B2" s="51" t="n">
         <f aca="false">truthStateParams!B2</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C2" s="12" t="str">
         <f aca="false">truthStateParams!C2</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D2" s="12" t="str">
         <f aca="false">truthStateParams!D2</f>
         <v>3-sigma bias propagation noise of asset 1</v>
       </c>
-      <c r="E2" s="54" t="n">
+      <c r="E2" s="28" t="n">
         <f aca="false">truthStateParams!E2</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F2" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="str">
         <f aca="false">truthStateParams!A3</f>
         <v>sig_b2_ss</v>
       </c>
-      <c r="B3" s="53" t="n">
+      <c r="B3" s="51" t="n">
         <f aca="false">truthStateParams!B3</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C3" s="12" t="str">
         <f aca="false">truthStateParams!C3</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D3" s="12" t="str">
         <f aca="false">truthStateParams!D3</f>
         <v>3-sigma bias propagation noise of asset 2</v>
       </c>
-      <c r="E3" s="54" t="n">
+      <c r="E3" s="28" t="n">
         <f aca="false">truthStateParams!E3</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F3" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="str">
         <f aca="false">truthStateParams!A4</f>
         <v>sig_b3_ss</v>
       </c>
-      <c r="B4" s="53" t="n">
+      <c r="B4" s="51" t="n">
         <f aca="false">truthStateParams!B4</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C4" s="12" t="str">
         <f aca="false">truthStateParams!C4</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D4" s="12" t="str">
         <f aca="false">truthStateParams!D4</f>
         <v>3-sigma bias propagation noise of asset 3</v>
       </c>
-      <c r="E4" s="54" t="n">
+      <c r="E4" s="28" t="n">
         <f aca="false">truthStateParams!E4</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F4" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="str">
         <f aca="false">truthStateParams!A5</f>
         <v>sig_b4_ss</v>
       </c>
-      <c r="B5" s="53" t="n">
+      <c r="B5" s="51" t="n">
         <f aca="false">truthStateParams!B5</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C5" s="12" t="str">
         <f aca="false">truthStateParams!C5</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D5" s="12" t="str">
         <f aca="false">truthStateParams!D5</f>
         <v>3-sigma bias propagation noise of asset 4</v>
       </c>
-      <c r="E5" s="54" t="n">
+      <c r="E5" s="28" t="n">
         <f aca="false">truthStateParams!E5</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F5" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="str">
         <f aca="false">truthStateParams!A6</f>
         <v>sig_b5_ss</v>
       </c>
-      <c r="B6" s="53" t="n">
+      <c r="B6" s="51" t="n">
         <f aca="false">truthStateParams!B6</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C6" s="12" t="str">
         <f aca="false">truthStateParams!C6</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D6" s="12" t="str">
         <f aca="false">truthStateParams!D6</f>
         <v>3-sigma bias propagation noise of asset 5</v>
       </c>
-      <c r="E6" s="54" t="n">
+      <c r="E6" s="28" t="n">
         <f aca="false">truthStateParams!E6</f>
-        <v>1E-008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61020,21 +61185,21 @@
         <f aca="false">truthStateParams!A7</f>
         <v>sig_b6_ss</v>
       </c>
-      <c r="B7" s="53" t="n">
+      <c r="B7" s="51" t="n">
         <f aca="false">truthStateParams!B7</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C7" s="12" t="str">
         <f aca="false">truthStateParams!C7</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D7" s="12" t="str">
         <f aca="false">truthStateParams!D7</f>
         <v>3-sigma bias propagation noise of asset 6</v>
       </c>
-      <c r="E7" s="54" t="n">
+      <c r="E7" s="28" t="n">
         <f aca="false">truthStateParams!E7</f>
-        <v>1E-008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61042,21 +61207,21 @@
         <f aca="false">truthStateParams!A8</f>
         <v>sig_b7_ss</v>
       </c>
-      <c r="B8" s="53" t="n">
+      <c r="B8" s="51" t="n">
         <f aca="false">truthStateParams!B8</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12" t="str">
         <f aca="false">truthStateParams!C8</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D8" s="12" t="str">
         <f aca="false">truthStateParams!D8</f>
         <v>3-sigma bias propagation noise of asset 7</v>
       </c>
-      <c r="E8" s="54" t="n">
+      <c r="E8" s="28" t="n">
         <f aca="false">truthStateParams!E8</f>
-        <v>1E-008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61076,9 +61241,9 @@
         <f aca="false">truthStateParams!D9</f>
         <v>3-sigma of RSO x accelerations</v>
       </c>
-      <c r="E9" s="54" t="n">
+      <c r="E9" s="27" t="n">
         <f aca="false">truthStateParams!E9</f>
-        <v>1.6E-007</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61098,9 +61263,9 @@
         <f aca="false">truthStateParams!D10</f>
         <v>3-sigma of RSO y accelerations</v>
       </c>
-      <c r="E10" s="54" t="n">
+      <c r="E10" s="27" t="n">
         <f aca="false">truthStateParams!E10</f>
-        <v>1.6E-007</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61120,9 +61285,9 @@
         <f aca="false">truthStateParams!D11</f>
         <v>3-sigma of RSO z accelerations</v>
       </c>
-      <c r="E11" s="54" t="n">
+      <c r="E11" s="27" t="n">
         <f aca="false">truthStateParams!E11</f>
-        <v>1.6E-007</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61130,21 +61295,21 @@
         <f aca="false">truthStateParams!A12</f>
         <v>sig_ax_ss</v>
       </c>
-      <c r="B12" s="53" t="n">
+      <c r="B12" s="51" t="n">
         <f aca="false">truthStateParams!B12</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C12" s="12" t="str">
         <f aca="false">truthStateParams!C12</f>
-        <v>m/s^2</v>
+        <v>nm/s^2</v>
       </c>
       <c r="D12" s="12" t="str">
         <f aca="false">truthStateParams!D12</f>
         <v>3-sigma of RSO x atmo acceleration</v>
       </c>
-      <c r="E12" s="54" t="n">
+      <c r="E12" s="28" t="n">
         <f aca="false">truthStateParams!E12</f>
-        <v>3.33333333333333E-010</v>
+        <v>3.33333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61152,21 +61317,21 @@
         <f aca="false">truthStateParams!A13</f>
         <v>sig_ay_ss</v>
       </c>
-      <c r="B13" s="53" t="n">
+      <c r="B13" s="51" t="n">
         <f aca="false">truthStateParams!B13</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C13" s="12" t="str">
         <f aca="false">truthStateParams!C13</f>
-        <v>m/s^2</v>
+        <v>nm/s^2</v>
       </c>
       <c r="D13" s="12" t="str">
         <f aca="false">truthStateParams!D13</f>
         <v>3-sigma of RSO y atmo acceleration</v>
       </c>
-      <c r="E13" s="54" t="n">
+      <c r="E13" s="28" t="n">
         <f aca="false">truthStateParams!E13</f>
-        <v>3.33333333333333E-010</v>
+        <v>3.33333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61174,21 +61339,21 @@
         <f aca="false">truthStateParams!A14</f>
         <v>sig_az_ss</v>
       </c>
-      <c r="B14" s="53" t="n">
+      <c r="B14" s="51" t="n">
         <f aca="false">truthStateParams!B14</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C14" s="12" t="str">
         <f aca="false">truthStateParams!C14</f>
-        <v>m/s^2</v>
+        <v>nm/s^2</v>
       </c>
       <c r="D14" s="12" t="str">
         <f aca="false">truthStateParams!D14</f>
         <v>3-sigma of RSO z atmo acceleration</v>
       </c>
-      <c r="E14" s="54" t="n">
+      <c r="E14" s="28" t="n">
         <f aca="false">truthStateParams!E14</f>
-        <v>3.33333333333333E-010</v>
+        <v>3.33333333333333</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61196,21 +61361,21 @@
       <c r="B15" s="53"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="54"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
       <c r="B16" s="53"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="54"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
       <c r="B17" s="53"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="54"/>
+      <c r="E17" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -61231,150 +61396,150 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.1214574898785"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="9.73279352226721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="7.97165991902834"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="45" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="21" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="49" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="39"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="str">
         <f aca="false">truthStateInitialUncertainty!A2</f>
         <v>sig_b1</v>
       </c>
-      <c r="B2" s="54" t="n">
+      <c r="B2" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C2" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D2" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D2</f>
         <v>3-sigma clocking bias of asset 1</v>
       </c>
-      <c r="E2" s="54" t="n">
+      <c r="E2" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E2</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F2" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="str">
         <f aca="false">truthStateInitialUncertainty!A3</f>
         <v>sig_b2</v>
       </c>
-      <c r="B3" s="54" t="n">
+      <c r="B3" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C3" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D3" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D3</f>
         <v>3-sigma clocking bias of asset 2</v>
       </c>
-      <c r="E3" s="54" t="n">
+      <c r="E3" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E3</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F3" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="str">
         <f aca="false">truthStateInitialUncertainty!A4</f>
         <v>sig_b3</v>
       </c>
-      <c r="B4" s="54" t="n">
+      <c r="B4" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C4" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D4" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D4</f>
         <v>3-sigma clocking bias of asset 3</v>
       </c>
-      <c r="E4" s="54" t="n">
+      <c r="E4" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E4</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F4" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="str">
         <f aca="false">truthStateInitialUncertainty!A5</f>
         <v>sig_b4</v>
       </c>
-      <c r="B5" s="54" t="n">
+      <c r="B5" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C5" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D5" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D5</f>
         <v>3-sigma clocking bias of asset 4</v>
       </c>
-      <c r="E5" s="54" t="n">
+      <c r="E5" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E5</f>
-        <v>1E-008</v>
-      </c>
-      <c r="F5" s="55"/>
+        <v>10</v>
+      </c>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="str">
         <f aca="false">truthStateInitialUncertainty!A6</f>
         <v>sig_b5</v>
       </c>
-      <c r="B6" s="54" t="n">
+      <c r="B6" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C6" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D6" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D6</f>
         <v>3-sigma clocking bias of asset 5</v>
       </c>
-      <c r="E6" s="54" t="n">
+      <c r="E6" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E6</f>
-        <v>1E-008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61382,21 +61547,21 @@
         <f aca="false">truthStateInitialUncertainty!A7</f>
         <v>sig_b6</v>
       </c>
-      <c r="B7" s="54" t="n">
+      <c r="B7" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C7" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D7" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D7</f>
         <v>3-sigma clocking bias of asset 6</v>
       </c>
-      <c r="E7" s="54" t="n">
+      <c r="E7" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E7</f>
-        <v>1E-008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61404,21 +61569,21 @@
         <f aca="false">truthStateInitialUncertainty!A8</f>
         <v>sig_b7</v>
       </c>
-      <c r="B8" s="54" t="n">
+      <c r="B8" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B8</f>
-        <v>3E-008</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C8</f>
-        <v>sec</v>
+        <v>ns</v>
       </c>
       <c r="D8" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D8</f>
         <v>3-sigma clocking bias of asset 7</v>
       </c>
-      <c r="E8" s="54" t="n">
+      <c r="E8" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!E8</f>
-        <v>1E-008</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61426,7 +61591,7 @@
         <f aca="false">truthStateInitialUncertainty!A9</f>
         <v>sig_px</v>
       </c>
-      <c r="B9" s="54" t="n">
+      <c r="B9" s="27" t="n">
         <f aca="false">truthStateInitialUncertainty!B9</f>
         <v>0.01798754748</v>
       </c>
@@ -61438,7 +61603,7 @@
         <f aca="false">truthStateInitialUncertainty!D9</f>
         <v>3-sigma of RSO x position</v>
       </c>
-      <c r="E9" s="54" t="n">
+      <c r="E9" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E9</f>
         <v>5.99584916</v>
       </c>
@@ -61448,7 +61613,7 @@
         <f aca="false">truthStateInitialUncertainty!A10</f>
         <v>sig_py</v>
       </c>
-      <c r="B10" s="54" t="n">
+      <c r="B10" s="27" t="n">
         <f aca="false">truthStateInitialUncertainty!B10</f>
         <v>0.01798754748</v>
       </c>
@@ -61460,7 +61625,7 @@
         <f aca="false">truthStateInitialUncertainty!D10</f>
         <v>3-sigma of RSO y position</v>
       </c>
-      <c r="E10" s="54" t="n">
+      <c r="E10" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E10</f>
         <v>5.99584916</v>
       </c>
@@ -61470,7 +61635,7 @@
         <f aca="false">truthStateInitialUncertainty!A11</f>
         <v>sig_pz</v>
       </c>
-      <c r="B11" s="54" t="n">
+      <c r="B11" s="27" t="n">
         <f aca="false">truthStateInitialUncertainty!B11</f>
         <v>0.01798754748</v>
       </c>
@@ -61482,7 +61647,7 @@
         <f aca="false">truthStateInitialUncertainty!D11</f>
         <v>3-sigma of RSO z position</v>
       </c>
-      <c r="E11" s="54" t="n">
+      <c r="E11" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E11</f>
         <v>5.99584916</v>
       </c>
@@ -61492,7 +61657,7 @@
         <f aca="false">truthStateInitialUncertainty!A12</f>
         <v>sig_vx</v>
       </c>
-      <c r="B12" s="54" t="n">
+      <c r="B12" s="27" t="n">
         <f aca="false">truthStateInitialUncertainty!B12</f>
         <v>0.000153</v>
       </c>
@@ -61504,9 +61669,9 @@
         <f aca="false">truthStateInitialUncertainty!D12</f>
         <v>3-sigma of RSO x velocity</v>
       </c>
-      <c r="E12" s="54" t="n">
+      <c r="E12" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E12</f>
-        <v>0.051</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61514,7 +61679,7 @@
         <f aca="false">truthStateInitialUncertainty!A13</f>
         <v>sig_vy</v>
       </c>
-      <c r="B13" s="54" t="n">
+      <c r="B13" s="27" t="n">
         <f aca="false">truthStateInitialUncertainty!B13</f>
         <v>0.000153</v>
       </c>
@@ -61526,9 +61691,9 @@
         <f aca="false">truthStateInitialUncertainty!D13</f>
         <v>3-sigma of RSO y velocity</v>
       </c>
-      <c r="E13" s="54" t="n">
+      <c r="E13" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E13</f>
-        <v>0.051</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61536,7 +61701,7 @@
         <f aca="false">truthStateInitialUncertainty!A14</f>
         <v>sig_vz</v>
       </c>
-      <c r="B14" s="54" t="n">
+      <c r="B14" s="27" t="n">
         <f aca="false">truthStateInitialUncertainty!B14</f>
         <v>0.000153</v>
       </c>
@@ -61548,9 +61713,9 @@
         <f aca="false">truthStateInitialUncertainty!D14</f>
         <v>3-sigma of RSO z velocity</v>
       </c>
-      <c r="E14" s="54" t="n">
+      <c r="E14" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E14</f>
-        <v>0.051</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61558,21 +61723,21 @@
         <f aca="false">truthStateInitialUncertainty!A15</f>
         <v>sig_ax</v>
       </c>
-      <c r="B15" s="54" t="n">
+      <c r="B15" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B15</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C15" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C15</f>
-        <v>m/s^2</v>
+        <v>nm/s^2</v>
       </c>
       <c r="D15" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D15</f>
         <v>3-sigma of RSO x atmo acceleration</v>
       </c>
-      <c r="E15" s="54" t="n">
+      <c r="E15" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E15</f>
-        <v>3.33333333333333E-010</v>
+        <v>3.33333333333333</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61580,21 +61745,21 @@
         <f aca="false">truthStateInitialUncertainty!A16</f>
         <v>sig_ay</v>
       </c>
-      <c r="B16" s="54" t="n">
+      <c r="B16" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B16</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C16" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C16</f>
-        <v>m/s^2</v>
+        <v>nm/s^2</v>
       </c>
       <c r="D16" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D16</f>
         <v>3-sigma of RSO y atmo acceleration</v>
       </c>
-      <c r="E16" s="54" t="n">
+      <c r="E16" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E16</f>
-        <v>3.33333333333333E-010</v>
+        <v>3.33333333333333</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61602,28 +61767,28 @@
         <f aca="false">truthStateInitialUncertainty!A17</f>
         <v>sig_az</v>
       </c>
-      <c r="B17" s="54" t="n">
+      <c r="B17" s="28" t="n">
         <f aca="false">truthStateInitialUncertainty!B17</f>
-        <v>1E-009</v>
+        <v>1</v>
       </c>
       <c r="C17" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!C17</f>
-        <v>m/s^2</v>
+        <v>nm/s^2</v>
       </c>
       <c r="D17" s="12" t="str">
         <f aca="false">truthStateInitialUncertainty!D17</f>
         <v>3-sigma of RSO z atmo acceleration</v>
       </c>
-      <c r="E17" s="54" t="n">
+      <c r="E17" s="55" t="n">
         <f aca="false">truthStateInitialUncertainty!E17</f>
-        <v>3.33333333333333E-010</v>
+        <v>3.33333333333333</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -61660,8 +61825,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.9878542510121"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -61690,7 +61855,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D2" s="60"/>
       <c r="E2" s="62" t="n">
@@ -61706,7 +61871,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D3" s="63"/>
       <c r="E3" s="65" t="n">
@@ -61722,7 +61887,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="65" t="n">
@@ -61738,7 +61903,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="65" t="n">
@@ -61754,7 +61919,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D6" s="63"/>
       <c r="E6" s="65" t="n">
@@ -61770,7 +61935,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="65" t="n">
@@ -61786,7 +61951,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="65" t="n">
@@ -61904,7 +62069,7 @@
         <v>0.01</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D15" s="63"/>
       <c r="E15" s="66" t="n">
@@ -61921,7 +62086,7 @@
         <v>0.02</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="66" t="n">
@@ -61938,7 +62103,7 @@
         <v>0.03</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D17" s="67"/>
       <c r="E17" s="68" t="n">

</xml_diff>

<commit_message>
attempted processing kalman updates one at a time.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1223,17 +1223,17 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="A9:B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.5951417004049"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1385,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>13</v>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="E9" s="9" t="n">
         <f aca="false">B9</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1422,7 +1422,7 @@
       </c>
       <c r="B11" s="17" t="n">
         <f aca="false">9+Na</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="E11" s="18" t="n">
         <f aca="false">B11</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,13 +1532,13 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="A9:B9 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1684,7 +1684,7 @@
   <dimension ref="1:59"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D65" activeCellId="1" sqref="A9:B9 D65"/>
+      <selection pane="topLeft" activeCell="D65" activeCellId="0" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1692,8 +1692,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.5991902834008"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -52722,13 +52722,13 @@
   <dimension ref="1:19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="1" sqref="A9:B9 C72"/>
+      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -55896,19 +55896,19 @@
       </c>
       <c r="B6" s="34" t="n">
         <f aca="false">IF(Na&gt;=3,C5+1,0)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C6" s="34" t="n">
         <f aca="false">B6+2</f>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D6" s="34" t="n">
         <f aca="false">B6</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E6" s="34" t="n">
         <f aca="false">C6</f>
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" s="34" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55917,19 +55917,19 @@
       </c>
       <c r="B7" s="34" t="n">
         <f aca="false">C6+1</f>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C7" s="34" t="n">
         <f aca="false">B7+2</f>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D7" s="34" t="n">
         <f aca="false">B7</f>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E7" s="34" t="n">
         <f aca="false">C7</f>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55938,19 +55938,19 @@
       </c>
       <c r="B8" s="34" t="n">
         <f aca="false">IF(Na&gt;=4,C7+1,0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C8" s="34" t="n">
         <f aca="false">B8+2</f>
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D8" s="34" t="n">
         <f aca="false">B8</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E8" s="34" t="n">
         <f aca="false">C8</f>
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -56978,19 +56978,19 @@
       </c>
       <c r="B9" s="34" t="n">
         <f aca="false">C8+1</f>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C9" s="34" t="n">
         <f aca="false">B9+2</f>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D9" s="34" t="n">
         <f aca="false">B9</f>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E9" s="34" t="n">
         <f aca="false">C9</f>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -58018,19 +58018,19 @@
       </c>
       <c r="B10" s="34" t="n">
         <f aca="false">IF(Na&gt;=5,C9+1,0)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C10" s="34" t="n">
         <f aca="false">B10+2</f>
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D10" s="34" t="n">
         <f aca="false">B10</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E10" s="34" t="n">
         <f aca="false">C10</f>
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" s="34" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58039,19 +58039,19 @@
       </c>
       <c r="B11" s="34" t="n">
         <f aca="false">C10+1</f>
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C11" s="34" t="n">
         <f aca="false">B11+2</f>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D11" s="34" t="n">
         <f aca="false">B11</f>
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E11" s="34" t="n">
         <f aca="false">C11</f>
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58060,19 +58060,19 @@
       </c>
       <c r="B12" s="34" t="n">
         <f aca="false">IF(Na&gt;=6,C11+1,0)</f>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C12" s="34" t="n">
         <f aca="false">B12+2</f>
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D12" s="34" t="n">
         <f aca="false">B12</f>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E12" s="34" t="n">
         <f aca="false">C12</f>
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -59100,19 +59100,19 @@
       </c>
       <c r="B13" s="34" t="n">
         <f aca="false">C12+1</f>
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C13" s="34" t="n">
         <f aca="false">B13+2</f>
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="D13" s="34" t="n">
         <f aca="false">B13</f>
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="E13" s="34" t="n">
         <f aca="false">C13</f>
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -60140,19 +60140,19 @@
       </c>
       <c r="B14" s="34" t="n">
         <f aca="false">IF(Na&gt;=7,C13+1,0)</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C14" s="34" t="n">
         <f aca="false">B14+2</f>
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D14" s="34" t="n">
         <f aca="false">B14</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E14" s="34" t="n">
         <f aca="false">C14</f>
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" s="34" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60161,19 +60161,19 @@
       </c>
       <c r="B15" s="34" t="n">
         <f aca="false">C14+1</f>
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C15" s="34" t="n">
         <f aca="false">B15+2</f>
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="D15" s="34" t="n">
         <f aca="false">B15</f>
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E15" s="34" t="n">
         <f aca="false">C15</f>
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" s="34" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60182,19 +60182,19 @@
       </c>
       <c r="B16" s="34" t="n">
         <f aca="false">1+6*Na</f>
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C16" s="34" t="n">
         <f aca="false">7*Na</f>
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D16" s="34" t="n">
         <f aca="false">B16</f>
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E16" s="34" t="n">
         <f aca="false">C16</f>
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60203,19 +60203,19 @@
       </c>
       <c r="B17" s="32" t="n">
         <f aca="false">C16+1</f>
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C17" s="32" t="n">
         <f aca="false">B17+2</f>
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D17" s="34" t="n">
         <f aca="false">B17</f>
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E17" s="34" t="n">
         <f aca="false">C17</f>
-        <v>52</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60224,19 +60224,19 @@
       </c>
       <c r="B18" s="32" t="n">
         <f aca="false">C17+1</f>
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C18" s="32" t="n">
         <f aca="false">B18+2</f>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D18" s="34" t="n">
         <f aca="false">B18</f>
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="E18" s="34" t="n">
         <f aca="false">C18</f>
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60245,19 +60245,19 @@
       </c>
       <c r="B19" s="32" t="n">
         <f aca="false">C18+1</f>
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C19" s="32" t="n">
         <f aca="false">B19+2</f>
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D19" s="34" t="n">
         <f aca="false">B19</f>
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="E19" s="34" t="n">
         <f aca="false">C19</f>
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -60279,7 +60279,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="A9:B9 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -60316,7 +60316,7 @@
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">Na</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">B2</f>
@@ -60324,7 +60324,7 @@
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">C2</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60333,19 +60333,19 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">C2+1</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">B3+2</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">B3</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">C3</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60354,19 +60354,19 @@
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">C3+1</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">B4+2</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">B4</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">C4</f>
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -60375,19 +60375,19 @@
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">C4+1</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5+2</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">B5</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">C5</f>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -60409,17 +60409,17 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="A9:B9 D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5060728744939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -60717,113 +60717,113 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="23" t="s">
         <v>173</v>
       </c>
       <c r="B15" s="45" t="n">
         <f aca="false">60-B2</f>
         <v>30</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="23" t="n">
         <f aca="false">B15/3/1000000000*bc</f>
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="23" t="s">
         <v>174</v>
       </c>
       <c r="B16" s="45" t="n">
         <f aca="false">60-B3</f>
         <v>30</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="23" t="n">
         <f aca="false">B16/3/1000000000*bc</f>
         <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="23" t="s">
         <v>175</v>
       </c>
       <c r="B17" s="45" t="n">
         <f aca="false">60-B4</f>
         <v>30</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="23" t="n">
         <f aca="false">B17/3/1000000000*bc</f>
         <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="23" t="s">
         <v>176</v>
       </c>
       <c r="B18" s="45" t="n">
         <f aca="false">60-B5</f>
         <v>30</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="23" t="n">
         <f aca="false">B18/3/1000000000*bc</f>
         <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B19" s="45" t="n">
         <f aca="false">60-B6</f>
         <v>30</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="23" t="n">
         <f aca="false">B19/3/1000000000*bc</f>
         <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="23" t="s">
         <v>178</v>
       </c>
       <c r="B20" s="45" t="n">
         <f aca="false">60-B7</f>
         <v>30</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="23" t="n">
         <f aca="false">B20/3/1000000000*bc</f>
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="23" t="s">
         <v>179</v>
       </c>
       <c r="B21" s="45" t="n">
         <f aca="false">60-B8</f>
         <v>30</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="23" t="n">
         <f aca="false">B21/3/1000000000*bc</f>
         <v>10</v>
       </c>
@@ -60847,17 +60847,17 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="A9:B9 E22"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="21" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="46" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -61249,17 +61249,17 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="1" sqref="A9:B9 D30"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="10.5060728744939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="21" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="46" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -61744,15 +61744,15 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="A9:B9 E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="21" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="46" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="21" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="21" width="9.10526315789474"/>
@@ -62165,7 +62165,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="A9:B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -62173,8 +62173,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
initial push for merginf the measurements
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Documents\OptimalEstimation\Montgomery_SpaceDomainAwareness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janss\repos\Montgomery_SpaceDomainAwareness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187DA87A-62E7-488E-B6AF-6CB198932AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF885BC-7A5A-4536-87C4-F0C448E5AE14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="987" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="224">
   <si>
     <t>Name</t>
   </si>
@@ -694,12 +694,48 @@
   <si>
     <t>atmCover</t>
   </si>
+  <si>
+    <t>RaDec_Kalman_update_enable</t>
+  </si>
+  <si>
+    <t>sig_bias_alpha</t>
+  </si>
+  <si>
+    <t>µrad</t>
+  </si>
+  <si>
+    <t>3-sigma right accension bias</t>
+  </si>
+  <si>
+    <t>sig_bias_delta</t>
+  </si>
+  <si>
+    <t>3-sigma declination bias</t>
+  </si>
+  <si>
+    <t>sig_meas_alpha</t>
+  </si>
+  <si>
+    <t>3-sigma right accension measurement uncertainty</t>
+  </si>
+  <si>
+    <t>sig_meas_delta</t>
+  </si>
+  <si>
+    <t>3-sigma declination measurement uncertainty</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>bias_radec</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
@@ -709,6 +745,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.0000"/>
     <numFmt numFmtId="171" formatCode="#,##0.000"/>
     <numFmt numFmtId="172" formatCode="0.000000000E+00"/>
+    <numFmt numFmtId="173" formatCode="0.0000000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -876,7 +913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,6 +1136,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1481,24 +1520,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.06640625" style="1"/>
-    <col min="2" max="2" width="7.9296875" style="1"/>
-    <col min="3" max="3" width="7.46484375" style="1"/>
-    <col min="4" max="4" width="46.9296875" style="1"/>
-    <col min="5" max="5" width="13.3984375" style="1"/>
-    <col min="6" max="6" width="29.33203125" style="1"/>
-    <col min="7" max="1025" width="8.59765625" style="1"/>
+    <col min="1" max="1" width="30" style="1"/>
+    <col min="2" max="2" width="8" style="1"/>
+    <col min="3" max="3" width="7.42578125" style="1"/>
+    <col min="4" max="4" width="47" style="1"/>
+    <col min="5" max="5" width="13.42578125" style="1"/>
+    <col min="6" max="6" width="29.28515625" style="1"/>
+    <col min="7" max="1025" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1529,11 +1568,11 @@
         <v>7</v>
       </c>
       <c r="E2" s="9">
-        <f t="shared" ref="E2:E17" si="0">B2</f>
+        <f t="shared" ref="E2:E18" si="0">B2</f>
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -1551,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1608,7 @@
         <v>15360</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -1587,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -1605,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -1641,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
@@ -1659,7 +1698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
@@ -1677,13 +1716,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="17">
-        <f>9+Na</f>
-        <v>16</v>
+        <f>9+3*Na</f>
+        <v>30</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -1693,10 +1732,10 @@
       </c>
       <c r="E11" s="18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>27</v>
       </c>
@@ -1714,7 +1753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>29</v>
       </c>
@@ -1726,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>30</v>
       </c>
@@ -1738,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>31</v>
       </c>
@@ -1750,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
@@ -1762,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>33</v>
       </c>
@@ -1772,6 +1811,18 @@
       <c r="E17" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1788,14 +1839,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625"/>
-    <col min="2" max="2" width="26.796875"/>
-    <col min="3" max="1025" width="8.59765625"/>
+    <col min="1" max="1" width="10.5703125"/>
+    <col min="2" max="2" width="26.85546875"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
@@ -1803,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>198</v>
       </c>
@@ -1811,7 +1862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -1819,7 +1870,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -1828,7 +1879,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -1836,7 +1887,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -1844,7 +1895,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -1853,7 +1904,7 @@
         <v>398600441800000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>204</v>
       </c>
@@ -1862,7 +1913,7 @@
         <v>299792458</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>205</v>
       </c>
@@ -1870,7 +1921,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>206</v>
       </c>
@@ -1878,7 +1929,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>207</v>
       </c>
@@ -1886,7 +1937,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -1894,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>209</v>
       </c>
@@ -1902,7 +1953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>210</v>
       </c>
@@ -1910,7 +1961,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -1928,21 +1979,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK59"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.19921875" style="1"/>
-    <col min="2" max="2" width="8.86328125" style="1"/>
-    <col min="3" max="3" width="8.59765625" style="1"/>
-    <col min="4" max="4" width="44.265625" style="1"/>
-    <col min="5" max="5" width="24.53125" style="1"/>
-    <col min="6" max="1025" width="8.59765625" style="1"/>
+    <col min="1" max="1" width="6.140625" style="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="8.5703125" style="1"/>
+    <col min="4" max="4" width="44.28515625" style="1"/>
+    <col min="5" max="5" width="24.5703125" style="1"/>
+    <col min="6" max="1025" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +3029,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -4015,7 +4066,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>37</v>
       </c>
@@ -5052,7 +5103,7 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>39</v>
       </c>
@@ -6089,7 +6140,7 @@
       <c r="AMI4"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>41</v>
       </c>
@@ -7126,7 +7177,7 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>44</v>
       </c>
@@ -8163,7 +8214,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>46</v>
       </c>
@@ -9200,7 +9251,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>48</v>
       </c>
@@ -10237,7 +10288,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>49</v>
       </c>
@@ -11274,7 +11325,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>50</v>
       </c>
@@ -12311,7 +12362,7 @@
       <c r="AMI10"/>
       <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1024" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>51</v>
       </c>
@@ -12329,7 +12380,7 @@
         <v>-323313.65091647406</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
@@ -13366,7 +13417,7 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>53</v>
       </c>
@@ -14403,7 +14454,7 @@
       <c r="AMI13"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>54</v>
       </c>
@@ -15440,7 +15491,7 @@
       <c r="AMI14"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>55</v>
       </c>
@@ -16477,7 +16528,7 @@
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>56</v>
       </c>
@@ -17514,7 +17565,7 @@
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>57</v>
       </c>
@@ -18551,7 +18602,7 @@
       <c r="AMI17"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>58</v>
       </c>
@@ -19588,7 +19639,7 @@
       <c r="AMI18"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>59</v>
       </c>
@@ -20625,7 +20676,7 @@
       <c r="AMI19"/>
       <c r="AMJ19"/>
     </row>
-    <row r="20" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>60</v>
       </c>
@@ -21662,7 +21713,7 @@
       <c r="AMI20"/>
       <c r="AMJ20"/>
     </row>
-    <row r="21" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>61</v>
       </c>
@@ -22699,7 +22750,7 @@
       <c r="AMI21"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>62</v>
       </c>
@@ -23736,7 +23787,7 @@
       <c r="AMI22"/>
       <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>63</v>
       </c>
@@ -24773,7 +24824,7 @@
       <c r="AMI23"/>
       <c r="AMJ23"/>
     </row>
-    <row r="24" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>64</v>
       </c>
@@ -25810,7 +25861,7 @@
       <c r="AMI24"/>
       <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>65</v>
       </c>
@@ -26847,7 +26898,7 @@
       <c r="AMI25"/>
       <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>66</v>
       </c>
@@ -27884,7 +27935,7 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>67</v>
       </c>
@@ -28921,7 +28972,7 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>68</v>
       </c>
@@ -29958,7 +30009,7 @@
       <c r="AMI28"/>
       <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>69</v>
       </c>
@@ -30995,7 +31046,7 @@
       <c r="AMI29"/>
       <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
         <v>70</v>
       </c>
@@ -32032,7 +32083,7 @@
       <c r="AMI30"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
         <v>71</v>
       </c>
@@ -33069,7 +33120,7 @@
       <c r="AMI31"/>
       <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
         <v>72</v>
       </c>
@@ -34106,7 +34157,7 @@
       <c r="AMI32"/>
       <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
         <v>73</v>
       </c>
@@ -35143,7 +35194,7 @@
       <c r="AMI33"/>
       <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
         <v>74</v>
       </c>
@@ -36180,7 +36231,7 @@
       <c r="AMI34"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>75</v>
       </c>
@@ -37217,7 +37268,7 @@
       <c r="AMI35"/>
       <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
         <v>76</v>
       </c>
@@ -38254,7 +38305,7 @@
       <c r="AMI36"/>
       <c r="AMJ36"/>
     </row>
-    <row r="37" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>77</v>
       </c>
@@ -39291,7 +39342,7 @@
       <c r="AMI37"/>
       <c r="AMJ37"/>
     </row>
-    <row r="38" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>78</v>
       </c>
@@ -40328,7 +40379,7 @@
       <c r="AMI38"/>
       <c r="AMJ38"/>
     </row>
-    <row r="39" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>79</v>
       </c>
@@ -41365,7 +41416,7 @@
       <c r="AMI39"/>
       <c r="AMJ39"/>
     </row>
-    <row r="40" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>80</v>
       </c>
@@ -42402,7 +42453,7 @@
       <c r="AMI40"/>
       <c r="AMJ40"/>
     </row>
-    <row r="41" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
         <v>81</v>
       </c>
@@ -43439,7 +43490,7 @@
       <c r="AMI41"/>
       <c r="AMJ41"/>
     </row>
-    <row r="42" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>82</v>
       </c>
@@ -44476,7 +44527,7 @@
       <c r="AMI42"/>
       <c r="AMJ42"/>
     </row>
-    <row r="43" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>83</v>
       </c>
@@ -45513,7 +45564,7 @@
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>84</v>
       </c>
@@ -46550,7 +46601,7 @@
       <c r="AMI44"/>
       <c r="AMJ44"/>
     </row>
-    <row r="45" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>87</v>
       </c>
@@ -47587,7 +47638,7 @@
       <c r="AMI45"/>
       <c r="AMJ45"/>
     </row>
-    <row r="46" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>89</v>
       </c>
@@ -48624,7 +48675,7 @@
       <c r="AMI46"/>
       <c r="AMJ46"/>
     </row>
-    <row r="47" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>91</v>
       </c>
@@ -49661,7 +49712,7 @@
       <c r="AMI47"/>
       <c r="AMJ47"/>
     </row>
-    <row r="48" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>93</v>
       </c>
@@ -50698,7 +50749,7 @@
       <c r="AMI48"/>
       <c r="AMJ48"/>
     </row>
-    <row r="49" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>95</v>
       </c>
@@ -51735,7 +51786,7 @@
       <c r="AMI49"/>
       <c r="AMJ49"/>
     </row>
-    <row r="50" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>97</v>
       </c>
@@ -52772,7 +52823,7 @@
       <c r="AMI50"/>
       <c r="AMJ50"/>
     </row>
-    <row r="51" spans="1:1024" s="34" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1024" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>99</v>
       </c>
@@ -52790,7 +52841,7 @@
         <v>8388094.8404114405</v>
       </c>
     </row>
-    <row r="52" spans="1:1024" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1024" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
         <v>101</v>
       </c>
@@ -52808,7 +52859,7 @@
         <v>-733863.20711629605</v>
       </c>
     </row>
-    <row r="53" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
         <v>103</v>
       </c>
@@ -52828,7 +52879,7 @@
       <c r="F53"/>
       <c r="G53"/>
     </row>
-    <row r="54" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
         <v>105</v>
       </c>
@@ -52848,7 +52899,7 @@
       <c r="F54"/>
       <c r="G54"/>
     </row>
-    <row r="55" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A55" s="34" t="s">
         <v>107</v>
       </c>
@@ -52868,7 +52919,7 @@
       <c r="F55"/>
       <c r="G55"/>
     </row>
-    <row r="56" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>109</v>
       </c>
@@ -52888,7 +52939,7 @@
       <c r="F56" s="33"/>
       <c r="G56" s="36"/>
     </row>
-    <row r="57" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>111</v>
       </c>
@@ -52908,7 +52959,7 @@
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
     </row>
-    <row r="58" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>114</v>
       </c>
@@ -52928,7 +52979,7 @@
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="1:1024" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>116</v>
       </c>
@@ -52960,10 +53011,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1025" width="9.1328125"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -52976,21 +53024,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.796875"/>
-    <col min="2" max="3" width="8.59765625"/>
-    <col min="4" max="5" width="16.46484375"/>
-    <col min="6" max="1025" width="8.59765625"/>
+    <col min="1" max="1" width="10.85546875"/>
+    <col min="2" max="3" width="8.5703125"/>
+    <col min="4" max="5" width="16.42578125"/>
+    <col min="6" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>118</v>
       </c>
@@ -53007,7 +53055,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -53019,7 +53067,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:E5" si="0">B2</f>
+        <f t="shared" ref="D2:E3" si="0">B2</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -53027,17 +53075,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <f>C2+1</f>
         <v>8</v>
       </c>
       <c r="C3">
-        <f>B3+2</f>
-        <v>10</v>
+        <f>B3+2*Na-1</f>
+        <v>21</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -53045,49 +53093,70 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4">
         <f>C3+1</f>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <f>B4+2</f>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>B4</f>
+        <v>22</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>C4</f>
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5">
         <f>C4+1</f>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <f>B5+2</f>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f>B5</f>
+        <v>25</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>C5</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6">
+        <f>C5+1</f>
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <f>B6+2</f>
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <f>B6</f>
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <f>C6</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -53098,24 +53167,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMK21"/>
+  <dimension ref="A1:AMK25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" style="1"/>
-    <col min="2" max="2" width="8.33203125" style="1"/>
-    <col min="3" max="3" width="10.796875" style="1"/>
-    <col min="4" max="4" width="37.73046875" style="1"/>
-    <col min="5" max="5" width="16.46484375" style="1"/>
-    <col min="6" max="6" width="12.53125" style="1"/>
-    <col min="7" max="1025" width="8.59765625" style="1"/>
+    <col min="1" max="1" width="10.5703125" style="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1"/>
+    <col min="4" max="4" width="37.7109375" style="1"/>
+    <col min="5" max="5" width="16.42578125" style="1"/>
+    <col min="6" max="6" width="12.5703125" style="1"/>
+    <col min="7" max="1025" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -53135,7 +53204,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>128</v>
       </c>
@@ -53156,7 +53225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>130</v>
       </c>
@@ -53177,7 +53246,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>132</v>
       </c>
@@ -53198,7 +53267,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>134</v>
       </c>
@@ -53219,7 +53288,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>136</v>
       </c>
@@ -53240,7 +53309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>138</v>
       </c>
@@ -53261,7 +53330,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>140</v>
       </c>
@@ -53282,7 +53351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>142</v>
       </c>
@@ -53303,7 +53372,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>146</v>
       </c>
@@ -53324,7 +53393,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>148</v>
       </c>
@@ -53345,7 +53414,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>150</v>
       </c>
@@ -53366,7 +53435,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>153</v>
       </c>
@@ -53387,7 +53456,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>155</v>
       </c>
@@ -53408,7 +53477,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>157</v>
       </c>
@@ -53424,7 +53493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>158</v>
       </c>
@@ -53440,7 +53509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>159</v>
       </c>
@@ -53456,7 +53525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>160</v>
       </c>
@@ -53472,7 +53541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>161</v>
       </c>
@@ -53488,7 +53557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>162</v>
       </c>
@@ -53504,7 +53573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>163</v>
       </c>
@@ -53518,6 +53587,90 @@
       <c r="E21" s="23">
         <f t="shared" si="2"/>
         <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" s="76">
+        <v>500</v>
+      </c>
+      <c r="C22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E22" s="77">
+        <f t="shared" ref="E22:E23" si="3">B22*10^-6/3</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="76">
+        <v>500</v>
+      </c>
+      <c r="C23" t="s">
+        <v>214</v>
+      </c>
+      <c r="D23" t="s">
+        <v>217</v>
+      </c>
+      <c r="E23" s="77">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="76">
+        <v>500</v>
+      </c>
+      <c r="C24" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E24" s="77">
+        <f>B24*10^-6/3</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="76">
+        <v>500</v>
+      </c>
+      <c r="C25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" s="77">
+        <f t="shared" ref="E25" si="4">B25*10^-6/3</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -53528,24 +53681,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="21"/>
-    <col min="2" max="2" width="9.9296875" style="21"/>
+    <col min="1" max="1" width="9.28515625" style="21"/>
+    <col min="2" max="2" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="21"/>
     <col min="4" max="4" width="32" style="21"/>
-    <col min="5" max="5" width="16.46484375" style="48"/>
-    <col min="6" max="6" width="20.265625" style="21"/>
-    <col min="7" max="1025" width="9.06640625" style="21"/>
+    <col min="5" max="5" width="16.42578125" style="48"/>
+    <col min="6" max="6" width="20.28515625" style="21"/>
+    <col min="7" max="1025" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -53565,7 +53718,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>165</v>
       </c>
@@ -53587,7 +53740,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>167</v>
       </c>
@@ -53609,7 +53762,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>169</v>
       </c>
@@ -53631,7 +53784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>171</v>
       </c>
@@ -53653,7 +53806,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>173</v>
       </c>
@@ -53675,7 +53828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>175</v>
       </c>
@@ -53697,7 +53850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>177</v>
       </c>
@@ -53719,7 +53872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>179</v>
       </c>
@@ -53741,7 +53894,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>182</v>
       </c>
@@ -53763,7 +53916,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>184</v>
       </c>
@@ -53785,7 +53938,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>186</v>
       </c>
@@ -53806,7 +53959,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>189</v>
       </c>
@@ -53827,7 +53980,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>191</v>
       </c>
@@ -53848,7 +54001,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>193</v>
       </c>
@@ -53870,7 +54023,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>194</v>
       </c>
@@ -53892,7 +54045,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>195</v>
       </c>
@@ -53912,6 +54065,90 @@
       </c>
       <c r="F17" s="21" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="76">
+        <v>500</v>
+      </c>
+      <c r="C18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E18" s="77">
+        <f t="shared" ref="E18:E19" si="1">B18*10^-6/3</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="76">
+        <v>500</v>
+      </c>
+      <c r="C19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" t="s">
+        <v>217</v>
+      </c>
+      <c r="E19" s="77">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="76">
+        <v>500</v>
+      </c>
+      <c r="C20" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E20" s="77">
+        <f>B20*10^-6/3</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" s="76">
+        <v>500</v>
+      </c>
+      <c r="C21" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E21" s="77">
+        <f t="shared" ref="E21" si="2">B21*10^-6/3</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -53922,24 +54159,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK21"/>
+  <dimension ref="A1:AMK25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.59765625" style="21"/>
-    <col min="2" max="2" width="10.19921875" style="48"/>
-    <col min="3" max="3" width="10.796875" style="21"/>
-    <col min="4" max="4" width="37.46484375" style="21"/>
-    <col min="5" max="5" width="16.46484375" style="48"/>
-    <col min="6" max="6" width="29.33203125" style="21"/>
-    <col min="7" max="1025" width="9.06640625" style="21"/>
+    <col min="1" max="1" width="20" style="21" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="48"/>
+    <col min="3" max="3" width="10.85546875" style="21"/>
+    <col min="4" max="4" width="37.42578125" style="21"/>
+    <col min="5" max="5" width="16.42578125" style="48"/>
+    <col min="6" max="6" width="29.28515625" style="21"/>
+    <col min="7" max="1025" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
@@ -53957,7 +54194,7 @@
       </c>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="str">
         <f>truthStateParams!A2</f>
         <v>sig_b1_ss</v>
@@ -53980,7 +54217,7 @@
       </c>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="str">
         <f>truthStateParams!A3</f>
         <v>sig_b2_ss</v>
@@ -54003,7 +54240,7 @@
       </c>
       <c r="F3" s="55"/>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="str">
         <f>truthStateParams!A4</f>
         <v>sig_b3_ss</v>
@@ -54026,7 +54263,7 @@
       </c>
       <c r="F4" s="55"/>
     </row>
-    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="str">
         <f>truthStateParams!A5</f>
         <v>sig_b4_ss</v>
@@ -54049,7 +54286,7 @@
       </c>
       <c r="F5" s="55"/>
     </row>
-    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="str">
         <f>truthStateParams!A6</f>
         <v>sig_b5_ss</v>
@@ -54071,7 +54308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="str">
         <f>truthStateParams!A7</f>
         <v>sig_b6_ss</v>
@@ -54093,7 +54330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="str">
         <f>truthStateParams!A8</f>
         <v>sig_b7_ss</v>
@@ -54115,7 +54352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="str">
         <f>truthStateParams!A9</f>
         <v>Q_grav_x</v>
@@ -54137,7 +54374,7 @@
         <v>1.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="str">
         <f>truthStateParams!A10</f>
         <v>Q_grav_y</v>
@@ -54159,7 +54396,7 @@
         <v>1.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="str">
         <f>truthStateParams!A11</f>
         <v>Q_grav_z</v>
@@ -54181,7 +54418,7 @@
         <v>1.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="str">
         <f>truthStateParams!A12</f>
         <v>sig_ax_ss</v>
@@ -54203,7 +54440,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="str">
         <f>truthStateParams!A13</f>
         <v>sig_ay_ss</v>
@@ -54225,7 +54462,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="str">
         <f>truthStateParams!A14</f>
         <v>sig_az_ss</v>
@@ -54247,7 +54484,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="str">
         <f>truthStateParams!A15</f>
         <v>sig_nu1_ss</v>
@@ -54269,7 +54506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="str">
         <f>truthStateParams!A16</f>
         <v>sig_nu2_ss</v>
@@ -54291,7 +54528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="str">
         <f>truthStateParams!A17</f>
         <v>sig_nu3_ss</v>
@@ -54313,7 +54550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="str">
         <f>truthStateParams!A18</f>
         <v>sig_nu4_ss</v>
@@ -54335,7 +54572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="str">
         <f>truthStateParams!A19</f>
         <v>sig_nu5_ss</v>
@@ -54357,7 +54594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="str">
         <f>truthStateParams!A20</f>
         <v>sig_nu6_ss</v>
@@ -54379,12 +54616,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="str">
         <f>truthStateParams!A21</f>
         <v>sig_nu7_ss</v>
       </c>
-      <c r="B21" s="59">
+      <c r="B21" s="10">
         <f>truthStateParams!B21</f>
         <v>30</v>
       </c>
@@ -54399,6 +54636,94 @@
       <c r="E21" s="10">
         <f>truthStateParams!E21</f>
         <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="str">
+        <f>truthStateParams!A22</f>
+        <v>sig_bias_alpha</v>
+      </c>
+      <c r="B22" s="10">
+        <f>truthStateParams!B22</f>
+        <v>500</v>
+      </c>
+      <c r="C22" s="10" t="str">
+        <f>truthStateParams!C22</f>
+        <v>µrad</v>
+      </c>
+      <c r="D22" s="10" t="str">
+        <f>truthStateParams!D22</f>
+        <v>3-sigma right accension bias</v>
+      </c>
+      <c r="E22" s="10">
+        <f>truthStateParams!E22</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="str">
+        <f>truthStateParams!A23</f>
+        <v>sig_bias_delta</v>
+      </c>
+      <c r="B23" s="10">
+        <f>truthStateParams!B23</f>
+        <v>500</v>
+      </c>
+      <c r="C23" s="10" t="str">
+        <f>truthStateParams!C23</f>
+        <v>µrad</v>
+      </c>
+      <c r="D23" s="10" t="str">
+        <f>truthStateParams!D23</f>
+        <v>3-sigma declination bias</v>
+      </c>
+      <c r="E23" s="10">
+        <f>truthStateParams!E23</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="str">
+        <f>truthStateParams!A24</f>
+        <v>sig_meas_alpha</v>
+      </c>
+      <c r="B24" s="10">
+        <f>truthStateParams!B24</f>
+        <v>500</v>
+      </c>
+      <c r="C24" s="10" t="str">
+        <f>truthStateParams!C24</f>
+        <v>µrad</v>
+      </c>
+      <c r="D24" s="10" t="str">
+        <f>truthStateParams!D24</f>
+        <v>3-sigma right accension measurement uncertainty</v>
+      </c>
+      <c r="E24" s="10">
+        <f>truthStateParams!E24</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="str">
+        <f>truthStateParams!A25</f>
+        <v>sig_meas_delta</v>
+      </c>
+      <c r="B25" s="10">
+        <f>truthStateParams!B25</f>
+        <v>500</v>
+      </c>
+      <c r="C25" s="10" t="str">
+        <f>truthStateParams!C25</f>
+        <v>µrad</v>
+      </c>
+      <c r="D25" s="10" t="str">
+        <f>truthStateParams!D25</f>
+        <v>3-sigma declination measurement uncertainty</v>
+      </c>
+      <c r="E25" s="10">
+        <f>truthStateParams!E25</f>
+        <v>1.6666666666666666E-4</v>
       </c>
     </row>
   </sheetData>
@@ -54409,24 +54734,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMK21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="21"/>
-    <col min="2" max="2" width="10.19921875" style="21"/>
+    <col min="1" max="1" width="16.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="21" customWidth="1"/>
     <col min="3" max="3" width="8" style="21"/>
-    <col min="4" max="4" width="32.33203125" style="21"/>
-    <col min="5" max="5" width="13.9296875" style="48"/>
-    <col min="6" max="6" width="16.46484375" style="21"/>
-    <col min="7" max="1025" width="9.06640625" style="21"/>
+    <col min="4" max="4" width="32.28515625" style="21"/>
+    <col min="5" max="5" width="14" style="48"/>
+    <col min="6" max="6" width="16.42578125" style="21"/>
+    <col min="7" max="1025" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
@@ -54444,7 +54769,7 @@
       </c>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="str">
         <f>truthStateInitialUncertainty!A2</f>
         <v>sig_b1</v>
@@ -54467,7 +54792,7 @@
       </c>
       <c r="F2" s="55"/>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="str">
         <f>truthStateInitialUncertainty!A3</f>
         <v>sig_b2</v>
@@ -54490,7 +54815,7 @@
       </c>
       <c r="F3" s="55"/>
     </row>
-    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="str">
         <f>truthStateInitialUncertainty!A4</f>
         <v>sig_b3</v>
@@ -54513,7 +54838,7 @@
       </c>
       <c r="F4" s="55"/>
     </row>
-    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="str">
         <f>truthStateInitialUncertainty!A5</f>
         <v>sig_b4</v>
@@ -54536,7 +54861,7 @@
       </c>
       <c r="F5" s="55"/>
     </row>
-    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="str">
         <f>truthStateInitialUncertainty!A6</f>
         <v>sig_b5</v>
@@ -54558,7 +54883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="str">
         <f>truthStateInitialUncertainty!A7</f>
         <v>sig_b6</v>
@@ -54580,7 +54905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="str">
         <f>truthStateInitialUncertainty!A8</f>
         <v>sig_b7</v>
@@ -54602,7 +54927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="str">
         <f>truthStateInitialUncertainty!A9</f>
         <v>sig_px</v>
@@ -54624,7 +54949,7 @@
         <v>5.9958491600000006</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="str">
         <f>truthStateInitialUncertainty!A10</f>
         <v>sig_py</v>
@@ -54646,7 +54971,7 @@
         <v>5.9958491600000006</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="str">
         <f>truthStateInitialUncertainty!A11</f>
         <v>sig_pz</v>
@@ -54668,7 +54993,7 @@
         <v>5.9958491600000006</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="str">
         <f>truthStateInitialUncertainty!A12</f>
         <v>sig_vx</v>
@@ -54690,7 +55015,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="str">
         <f>truthStateInitialUncertainty!A13</f>
         <v>sig_vy</v>
@@ -54712,7 +55037,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="str">
         <f>truthStateInitialUncertainty!A14</f>
         <v>sig_vz</v>
@@ -54734,7 +55059,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="str">
         <f>truthStateInitialUncertainty!A15</f>
         <v>sig_ax</v>
@@ -54756,7 +55081,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="str">
         <f>truthStateInitialUncertainty!A16</f>
         <v>sig_ay</v>
@@ -54778,7 +55103,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="str">
         <f>truthStateInitialUncertainty!A17</f>
         <v>sig_az</v>
@@ -54800,19 +55125,93 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="10"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="13"/>
+    <row r="18" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="str">
+        <f>truthStateInitialUncertainty!A18</f>
+        <v>sig_bias_alpha</v>
+      </c>
+      <c r="B18" s="32">
+        <f>truthStateInitialUncertainty!B18</f>
+        <v>500</v>
+      </c>
+      <c r="C18" s="12" t="str">
+        <f>truthStateInitialUncertainty!C18</f>
+        <v>µrad</v>
+      </c>
+      <c r="D18" s="12" t="str">
+        <f>truthStateInitialUncertainty!D18</f>
+        <v>3-sigma right accension bias</v>
+      </c>
+      <c r="E18" s="61">
+        <f>truthStateInitialUncertainty!E18</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="15"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="13"/>
+    <row r="19" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="str">
+        <f>truthStateInitialUncertainty!A19</f>
+        <v>sig_bias_delta</v>
+      </c>
+      <c r="B19" s="32">
+        <f>truthStateInitialUncertainty!B19</f>
+        <v>500</v>
+      </c>
+      <c r="C19" s="12" t="str">
+        <f>truthStateInitialUncertainty!C19</f>
+        <v>µrad</v>
+      </c>
+      <c r="D19" s="12" t="str">
+        <f>truthStateInitialUncertainty!D19</f>
+        <v>3-sigma declination bias</v>
+      </c>
+      <c r="E19" s="61">
+        <f>truthStateInitialUncertainty!E19</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="str">
+        <f>truthStateInitialUncertainty!A20</f>
+        <v>sig_meas_alpha</v>
+      </c>
+      <c r="B20" s="32">
+        <f>truthStateInitialUncertainty!B20</f>
+        <v>500</v>
+      </c>
+      <c r="C20" s="12" t="str">
+        <f>truthStateInitialUncertainty!C20</f>
+        <v>µrad</v>
+      </c>
+      <c r="D20" s="12" t="str">
+        <f>truthStateInitialUncertainty!D20</f>
+        <v>3-sigma right accension measurement uncertainty</v>
+      </c>
+      <c r="E20" s="61">
+        <f>truthStateInitialUncertainty!E20</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="str">
+        <f>truthStateInitialUncertainty!A21</f>
+        <v>sig_meas_delta</v>
+      </c>
+      <c r="B21" s="32">
+        <f>truthStateInitialUncertainty!B21</f>
+        <v>500</v>
+      </c>
+      <c r="C21" s="12" t="str">
+        <f>truthStateInitialUncertainty!C21</f>
+        <v>µrad</v>
+      </c>
+      <c r="D21" s="12" t="str">
+        <f>truthStateInitialUncertainty!D21</f>
+        <v>3-sigma declination measurement uncertainty</v>
+      </c>
+      <c r="E21" s="61">
+        <f>truthStateInitialUncertainty!E21</f>
+        <v>1.6666666666666666E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -54828,17 +55227,17 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" style="1"/>
-    <col min="2" max="2" width="13.46484375" style="1"/>
-    <col min="3" max="3" width="9.06640625" style="1"/>
-    <col min="4" max="4" width="17.265625" style="1"/>
-    <col min="5" max="5" width="16.3984375" style="1"/>
-    <col min="6" max="1025" width="8.59765625" style="1"/>
+    <col min="1" max="1" width="11.140625" style="1"/>
+    <col min="2" max="2" width="13.42578125" style="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="17.28515625" style="1"/>
+    <col min="5" max="5" width="16.42578125" style="1"/>
+    <col min="6" max="1025" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -54856,7 +55255,7 @@
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
         <v>84</v>
       </c>
@@ -54873,7 +55272,7 @@
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>87</v>
       </c>
@@ -54890,7 +55289,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>89</v>
       </c>
@@ -54907,7 +55306,7 @@
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>91</v>
       </c>
@@ -54924,7 +55323,7 @@
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>93</v>
       </c>
@@ -54941,7 +55340,7 @@
       </c>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>95</v>
       </c>
@@ -54958,7 +55357,7 @@
       </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>97</v>
       </c>
@@ -54975,7 +55374,7 @@
       </c>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>99</v>
       </c>
@@ -54992,7 +55391,7 @@
       </c>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>101</v>
       </c>
@@ -55009,7 +55408,7 @@
       </c>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>103</v>
       </c>
@@ -55026,7 +55425,7 @@
       </c>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>105</v>
       </c>
@@ -55043,7 +55442,7 @@
       </c>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>107</v>
       </c>
@@ -55060,7 +55459,7 @@
       </c>
       <c r="F13" s="21"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>109</v>
       </c>
@@ -55077,7 +55476,7 @@
       </c>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>111</v>
       </c>
@@ -55094,7 +55493,7 @@
       </c>
       <c r="F15" s="21"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>114</v>
       </c>
@@ -55111,7 +55510,7 @@
       </c>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="71" t="s">
         <v>116</v>
       </c>

</xml_diff>